<commit_message>
This visualization highlights the strongest product associations using lift, helping identify which products should be bundled or recommended together.
</commit_message>
<xml_diff>
--- a/output/association_rules.xlsx
+++ b/output/association_rules.xlsx
@@ -508,25 +508,25 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>frozenset({"POPPY'S PLAYHOUSE KITCHEN"})</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>frozenset({"POPPY'S PLAYHOUSE BEDROOM "})</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>frozenset({"POPPY'S PLAYHOUSE KITCHEN"})</t>
-        </is>
-      </c>
       <c r="C2" t="n">
+        <v>0.04381443298969072</v>
+      </c>
+      <c r="D2" t="n">
         <v>0.04510309278350515</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.04381443298969072</v>
       </c>
       <c r="E2" t="n">
         <v>0.03608247422680412</v>
       </c>
       <c r="F2" t="n">
-        <v>0.7999999999999999</v>
+        <v>0.8235294117647058</v>
       </c>
       <c r="G2" t="n">
         <v>18.25882352941176</v>
@@ -538,16 +538,16 @@
         <v>0.03410630779041343</v>
       </c>
       <c r="J2" t="n">
-        <v>4.780927835051545</v>
+        <v>5.411082474226803</v>
       </c>
       <c r="K2" t="n">
-        <v>0.9898785425101214</v>
+        <v>0.9885444743935309</v>
       </c>
       <c r="L2" t="n">
         <v>0.6829268292682927</v>
       </c>
       <c r="M2" t="n">
-        <v>0.7908355795148247</v>
+        <v>0.8151940938318647</v>
       </c>
       <c r="N2" t="n">
         <v>0.8117647058823529</v>
@@ -556,25 +556,25 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>frozenset({"POPPY'S PLAYHOUSE BEDROOM "})</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>frozenset({"POPPY'S PLAYHOUSE KITCHEN"})</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>frozenset({"POPPY'S PLAYHOUSE BEDROOM "})</t>
-        </is>
-      </c>
       <c r="C3" t="n">
+        <v>0.04510309278350515</v>
+      </c>
+      <c r="D3" t="n">
         <v>0.04381443298969072</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.04510309278350515</v>
       </c>
       <c r="E3" t="n">
         <v>0.03608247422680412</v>
       </c>
       <c r="F3" t="n">
-        <v>0.8235294117647058</v>
+        <v>0.7999999999999999</v>
       </c>
       <c r="G3" t="n">
         <v>18.25882352941176</v>
@@ -586,16 +586,16 @@
         <v>0.03410630779041343</v>
       </c>
       <c r="J3" t="n">
-        <v>5.411082474226803</v>
+        <v>4.780927835051545</v>
       </c>
       <c r="K3" t="n">
-        <v>0.9885444743935309</v>
+        <v>0.9898785425101214</v>
       </c>
       <c r="L3" t="n">
         <v>0.6829268292682927</v>
       </c>
       <c r="M3" t="n">
-        <v>0.8151940938318647</v>
+        <v>0.7908355795148247</v>
       </c>
       <c r="N3" t="n">
         <v>0.8117647058823529</v>
@@ -604,25 +604,25 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>frozenset({'GREEN REGENCY TEACUP AND SAUCER'})</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>frozenset({'ROSES REGENCY TEACUP AND SAUCER '})</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>frozenset({'GREEN REGENCY TEACUP AND SAUCER'})</t>
-        </is>
-      </c>
       <c r="C4" t="n">
+        <v>0.04510309278350515</v>
+      </c>
+      <c r="D4" t="n">
         <v>0.04252577319587629</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.04510309278350515</v>
       </c>
       <c r="E4" t="n">
         <v>0.03221649484536082</v>
       </c>
       <c r="F4" t="n">
-        <v>0.7575757575757575</v>
+        <v>0.7142857142857142</v>
       </c>
       <c r="G4" t="n">
         <v>16.7965367965368</v>
@@ -634,16 +634,16 @@
         <v>0.03029845095121692</v>
       </c>
       <c r="J4" t="n">
-        <v>3.93894974226804</v>
+        <v>3.351159793814432</v>
       </c>
       <c r="K4" t="n">
-        <v>0.9822341857335126</v>
+        <v>0.9848852901484479</v>
       </c>
       <c r="L4" t="n">
         <v>0.5813953488372092</v>
       </c>
       <c r="M4" t="n">
-        <v>0.7461252198094303</v>
+        <v>0.7015958469525091</v>
       </c>
       <c r="N4" t="n">
         <v>0.7359307359307359</v>
@@ -652,25 +652,25 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>frozenset({'ROSES REGENCY TEACUP AND SAUCER '})</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>frozenset({'GREEN REGENCY TEACUP AND SAUCER'})</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>frozenset({'ROSES REGENCY TEACUP AND SAUCER '})</t>
-        </is>
-      </c>
       <c r="C5" t="n">
+        <v>0.04252577319587629</v>
+      </c>
+      <c r="D5" t="n">
         <v>0.04510309278350515</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.04252577319587629</v>
       </c>
       <c r="E5" t="n">
         <v>0.03221649484536082</v>
       </c>
       <c r="F5" t="n">
-        <v>0.7142857142857142</v>
+        <v>0.7575757575757575</v>
       </c>
       <c r="G5" t="n">
         <v>16.7965367965368</v>
@@ -682,16 +682,16 @@
         <v>0.03029845095121692</v>
       </c>
       <c r="J5" t="n">
-        <v>3.351159793814432</v>
+        <v>3.93894974226804</v>
       </c>
       <c r="K5" t="n">
-        <v>0.9848852901484479</v>
+        <v>0.9822341857335126</v>
       </c>
       <c r="L5" t="n">
         <v>0.5813953488372092</v>
       </c>
       <c r="M5" t="n">
-        <v>0.7015958469525091</v>
+        <v>0.7461252198094303</v>
       </c>
       <c r="N5" t="n">
         <v>0.7359307359307359</v>
@@ -700,25 +700,25 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
+          <t>frozenset({'WOOD 2 DRAWER CABINET WHITE FINISH'})</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
           <t>frozenset({'WOOD S/3 CABINET ANT WHITE FINISH'})</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>frozenset({'WOOD 2 DRAWER CABINET WHITE FINISH'})</t>
-        </is>
-      </c>
       <c r="C6" t="n">
+        <v>0.04510309278350515</v>
+      </c>
+      <c r="D6" t="n">
         <v>0.04639175257731959</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.04510309278350515</v>
       </c>
       <c r="E6" t="n">
         <v>0.03092783505154639</v>
       </c>
       <c r="F6" t="n">
-        <v>0.6666666666666666</v>
+        <v>0.6857142857142857</v>
       </c>
       <c r="G6" t="n">
         <v>14.78095238095238</v>
@@ -730,16 +730,16 @@
         <v>0.02883542353066213</v>
       </c>
       <c r="J6" t="n">
-        <v>2.864690721649485</v>
+        <v>3.034208059981256</v>
       </c>
       <c r="K6" t="n">
-        <v>0.9777027027027028</v>
+        <v>0.97638326585695</v>
       </c>
       <c r="L6" t="n">
         <v>0.5106382978723404</v>
       </c>
       <c r="M6" t="n">
-        <v>0.6509221772379666</v>
+        <v>0.6704247104247104</v>
       </c>
       <c r="N6" t="n">
         <v>0.6761904761904762</v>
@@ -748,25 +748,25 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
+          <t>frozenset({'WOOD S/3 CABINET ANT WHITE FINISH'})</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>frozenset({'WOOD 2 DRAWER CABINET WHITE FINISH'})</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>frozenset({'WOOD S/3 CABINET ANT WHITE FINISH'})</t>
-        </is>
-      </c>
       <c r="C7" t="n">
+        <v>0.04639175257731959</v>
+      </c>
+      <c r="D7" t="n">
         <v>0.04510309278350515</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0.04639175257731959</v>
       </c>
       <c r="E7" t="n">
         <v>0.03092783505154639</v>
       </c>
       <c r="F7" t="n">
-        <v>0.6857142857142857</v>
+        <v>0.6666666666666666</v>
       </c>
       <c r="G7" t="n">
         <v>14.78095238095238</v>
@@ -778,16 +778,16 @@
         <v>0.02883542353066213</v>
       </c>
       <c r="J7" t="n">
-        <v>3.034208059981256</v>
+        <v>2.864690721649485</v>
       </c>
       <c r="K7" t="n">
-        <v>0.97638326585695</v>
+        <v>0.9777027027027028</v>
       </c>
       <c r="L7" t="n">
         <v>0.5106382978723404</v>
       </c>
       <c r="M7" t="n">
-        <v>0.6704247104247104</v>
+        <v>0.6509221772379666</v>
       </c>
       <c r="N7" t="n">
         <v>0.6761904761904762</v>
@@ -988,25 +988,25 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>frozenset({'LARGE POPCORN HOLDER '})</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
           <t>frozenset({'SMALL POPCORN HOLDER'})</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>frozenset({'LARGE POPCORN HOLDER '})</t>
-        </is>
-      </c>
       <c r="C12" t="n">
+        <v>0.04123711340206185</v>
+      </c>
+      <c r="D12" t="n">
         <v>0.06829896907216494</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0.04123711340206185</v>
       </c>
       <c r="E12" t="n">
         <v>0.03608247422680412</v>
       </c>
       <c r="F12" t="n">
-        <v>0.5283018867924528</v>
+        <v>0.8749999999999999</v>
       </c>
       <c r="G12" t="n">
         <v>12.81132075471698</v>
@@ -1018,16 +1018,16 @@
         <v>0.03326602189393134</v>
       </c>
       <c r="J12" t="n">
-        <v>2.032577319587629</v>
+        <v>7.453608247422674</v>
       </c>
       <c r="K12" t="n">
-        <v>0.9895277613119936</v>
+        <v>0.9615975422427036</v>
       </c>
       <c r="L12" t="n">
         <v>0.4912280701754385</v>
       </c>
       <c r="M12" t="n">
-        <v>0.5080137959018056</v>
+        <v>0.8658367911479944</v>
       </c>
       <c r="N12" t="n">
         <v>0.7016509433962264</v>
@@ -1036,25 +1036,25 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>frozenset({'SMALL POPCORN HOLDER'})</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>frozenset({'LARGE POPCORN HOLDER '})</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>frozenset({'SMALL POPCORN HOLDER'})</t>
-        </is>
-      </c>
       <c r="C13" t="n">
+        <v>0.06829896907216494</v>
+      </c>
+      <c r="D13" t="n">
         <v>0.04123711340206185</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.06829896907216494</v>
       </c>
       <c r="E13" t="n">
         <v>0.03608247422680412</v>
       </c>
       <c r="F13" t="n">
-        <v>0.8749999999999999</v>
+        <v>0.5283018867924528</v>
       </c>
       <c r="G13" t="n">
         <v>12.81132075471698</v>
@@ -1066,16 +1066,16 @@
         <v>0.03326602189393134</v>
       </c>
       <c r="J13" t="n">
-        <v>7.453608247422674</v>
+        <v>2.032577319587629</v>
       </c>
       <c r="K13" t="n">
-        <v>0.9615975422427036</v>
+        <v>0.9895277613119936</v>
       </c>
       <c r="L13" t="n">
         <v>0.4912280701754385</v>
       </c>
       <c r="M13" t="n">
-        <v>0.8658367911479944</v>
+        <v>0.5080137959018056</v>
       </c>
       <c r="N13" t="n">
         <v>0.7016509433962264</v>
@@ -1665,7 +1665,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>frozenset({'WHITE HANGING HEART T-LIGHT HOLDER', 'RED WOOLLY HOTTIE WHITE HEART.'})</t>
+          <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.', 'WHITE HANGING HEART T-LIGHT HOLDER'})</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -1708,7 +1708,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>frozenset({'WHITE HANGING HEART T-LIGHT HOLDER', 'RED WOOLLY HOTTIE WHITE HEART.'})</t>
+          <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.', 'WHITE HANGING HEART T-LIGHT HOLDER'})</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1948,25 +1948,25 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
+          <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.'})</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
           <t>frozenset({'WHITE HANGING HEART T-LIGHT HOLDER', 'KNITTED UNION FLAG HOT WATER BOTTLE'})</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.'})</t>
-        </is>
-      </c>
       <c r="C32" t="n">
+        <v>0.1005154639175258</v>
+      </c>
+      <c r="D32" t="n">
         <v>0.04639175257731959</v>
-      </c>
-      <c r="D32" t="n">
-        <v>0.1005154639175258</v>
       </c>
       <c r="E32" t="n">
         <v>0.03865979381443299</v>
       </c>
       <c r="F32" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.3846153846153846</v>
       </c>
       <c r="G32" t="n">
         <v>8.290598290598291</v>
@@ -1978,16 +1978,16 @@
         <v>0.03399670528217664</v>
       </c>
       <c r="J32" t="n">
-        <v>5.396907216494847</v>
+        <v>1.549613402061855</v>
       </c>
       <c r="K32" t="n">
-        <v>0.9221621621621622</v>
+        <v>0.9776504297994268</v>
       </c>
       <c r="L32" t="n">
         <v>0.3571428571428572</v>
       </c>
       <c r="M32" t="n">
-        <v>0.8147086914995225</v>
+        <v>0.3546777546777547</v>
       </c>
       <c r="N32" t="n">
         <v>0.608974358974359</v>
@@ -1996,25 +1996,25 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
+          <t>frozenset({'WHITE HANGING HEART T-LIGHT HOLDER', 'KNITTED UNION FLAG HOT WATER BOTTLE'})</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
           <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.'})</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>frozenset({'WHITE HANGING HEART T-LIGHT HOLDER', 'KNITTED UNION FLAG HOT WATER BOTTLE'})</t>
-        </is>
-      </c>
       <c r="C33" t="n">
+        <v>0.04639175257731959</v>
+      </c>
+      <c r="D33" t="n">
         <v>0.1005154639175258</v>
-      </c>
-      <c r="D33" t="n">
-        <v>0.04639175257731959</v>
       </c>
       <c r="E33" t="n">
         <v>0.03865979381443299</v>
       </c>
       <c r="F33" t="n">
-        <v>0.3846153846153846</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="G33" t="n">
         <v>8.290598290598291</v>
@@ -2026,16 +2026,16 @@
         <v>0.03399670528217664</v>
       </c>
       <c r="J33" t="n">
-        <v>1.549613402061855</v>
+        <v>5.396907216494847</v>
       </c>
       <c r="K33" t="n">
-        <v>0.9776504297994268</v>
+        <v>0.9221621621621622</v>
       </c>
       <c r="L33" t="n">
         <v>0.3571428571428572</v>
       </c>
       <c r="M33" t="n">
-        <v>0.3546777546777547</v>
+        <v>0.8147086914995225</v>
       </c>
       <c r="N33" t="n">
         <v>0.608974358974359</v>
@@ -2044,25 +2044,25 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER RED RETROSPOT', 'HAND WARMER OWL DESIGN'})</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN'})</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER OWL DESIGN', 'HAND WARMER RED RETROSPOT'})</t>
-        </is>
-      </c>
       <c r="C34" t="n">
+        <v>0.04896907216494845</v>
+      </c>
+      <c r="D34" t="n">
         <v>0.09922680412371133</v>
-      </c>
-      <c r="D34" t="n">
-        <v>0.04896907216494845</v>
       </c>
       <c r="E34" t="n">
         <v>0.03865979381443299</v>
       </c>
       <c r="F34" t="n">
-        <v>0.3896103896103896</v>
+        <v>0.7894736842105263</v>
       </c>
       <c r="G34" t="n">
         <v>7.956254272043746</v>
@@ -2074,16 +2074,16 @@
         <v>0.03380074928260177</v>
       </c>
       <c r="J34" t="n">
-        <v>1.558071945602106</v>
+        <v>4.278672680412371</v>
       </c>
       <c r="K34" t="n">
-        <v>0.9706247019551741</v>
+        <v>0.9193315266486</v>
       </c>
       <c r="L34" t="n">
         <v>0.3529411764705883</v>
       </c>
       <c r="M34" t="n">
-        <v>0.3581811142786753</v>
+        <v>0.7662826594382953</v>
       </c>
       <c r="N34" t="n">
         <v>0.589542036910458</v>
@@ -2092,25 +2092,25 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER OWL DESIGN', 'HAND WARMER RED RETROSPOT'})</t>
+          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN'})</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN'})</t>
+          <t>frozenset({'HAND WARMER RED RETROSPOT', 'HAND WARMER OWL DESIGN'})</t>
         </is>
       </c>
       <c r="C35" t="n">
+        <v>0.09922680412371133</v>
+      </c>
+      <c r="D35" t="n">
         <v>0.04896907216494845</v>
-      </c>
-      <c r="D35" t="n">
-        <v>0.09922680412371133</v>
       </c>
       <c r="E35" t="n">
         <v>0.03865979381443299</v>
       </c>
       <c r="F35" t="n">
-        <v>0.7894736842105263</v>
+        <v>0.3896103896103896</v>
       </c>
       <c r="G35" t="n">
         <v>7.956254272043746</v>
@@ -2122,16 +2122,16 @@
         <v>0.03380074928260177</v>
       </c>
       <c r="J35" t="n">
-        <v>4.278672680412371</v>
+        <v>1.558071945602106</v>
       </c>
       <c r="K35" t="n">
-        <v>0.9193315266486</v>
+        <v>0.9706247019551741</v>
       </c>
       <c r="L35" t="n">
         <v>0.3529411764705883</v>
       </c>
       <c r="M35" t="n">
-        <v>0.7662826594382953</v>
+        <v>0.3581811142786753</v>
       </c>
       <c r="N35" t="n">
         <v>0.589542036910458</v>
@@ -2241,7 +2241,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER RED RETROSPOT', 'HAND WARMER SCOTTY DOG DESIGN'})</t>
+          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN', 'HAND WARMER RED RETROSPOT'})</t>
         </is>
       </c>
       <c r="C38" t="n">
@@ -2284,7 +2284,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER RED RETROSPOT', 'HAND WARMER SCOTTY DOG DESIGN'})</t>
+          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN', 'HAND WARMER RED RETROSPOT'})</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -2332,25 +2332,25 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
+          <t>frozenset({'HOT WATER BOTTLE I AM SO POORLY'})</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
           <t>frozenset({'CHOCOLATE HOT WATER BOTTLE'})</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>frozenset({'HOT WATER BOTTLE I AM SO POORLY'})</t>
-        </is>
-      </c>
       <c r="C40" t="n">
+        <v>0.05798969072164949</v>
+      </c>
+      <c r="D40" t="n">
         <v>0.07860824742268041</v>
-      </c>
-      <c r="D40" t="n">
-        <v>0.05798969072164949</v>
       </c>
       <c r="E40" t="n">
         <v>0.03479381443298969</v>
       </c>
       <c r="F40" t="n">
-        <v>0.4426229508196722</v>
+        <v>0.6</v>
       </c>
       <c r="G40" t="n">
         <v>7.632786885245902</v>
@@ -2362,16 +2362,16 @@
         <v>0.03023534647677755</v>
       </c>
       <c r="J40" t="n">
-        <v>1.690077319587629</v>
+        <v>2.303479381443299</v>
       </c>
       <c r="K40" t="n">
-        <v>0.943123543123543</v>
+        <v>0.9224806201550387</v>
       </c>
       <c r="L40" t="n">
         <v>0.3417721518987342</v>
       </c>
       <c r="M40" t="n">
-        <v>0.4083110941669844</v>
+        <v>0.5658741258741258</v>
       </c>
       <c r="N40" t="n">
         <v>0.521311475409836</v>
@@ -2380,25 +2380,25 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
+          <t>frozenset({'CHOCOLATE HOT WATER BOTTLE'})</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
           <t>frozenset({'HOT WATER BOTTLE I AM SO POORLY'})</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>frozenset({'CHOCOLATE HOT WATER BOTTLE'})</t>
-        </is>
-      </c>
       <c r="C41" t="n">
+        <v>0.07860824742268041</v>
+      </c>
+      <c r="D41" t="n">
         <v>0.05798969072164949</v>
-      </c>
-      <c r="D41" t="n">
-        <v>0.07860824742268041</v>
       </c>
       <c r="E41" t="n">
         <v>0.03479381443298969</v>
       </c>
       <c r="F41" t="n">
-        <v>0.6</v>
+        <v>0.4426229508196722</v>
       </c>
       <c r="G41" t="n">
         <v>7.632786885245902</v>
@@ -2410,16 +2410,16 @@
         <v>0.03023534647677755</v>
       </c>
       <c r="J41" t="n">
-        <v>2.303479381443299</v>
+        <v>1.690077319587629</v>
       </c>
       <c r="K41" t="n">
-        <v>0.9224806201550387</v>
+        <v>0.943123543123543</v>
       </c>
       <c r="L41" t="n">
         <v>0.3417721518987342</v>
       </c>
       <c r="M41" t="n">
-        <v>0.5658741258741258</v>
+        <v>0.4083110941669844</v>
       </c>
       <c r="N41" t="n">
         <v>0.521311475409836</v>
@@ -2625,7 +2625,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER OWL DESIGN', 'HAND WARMER UNION JACK'})</t>
+          <t>frozenset({'HAND WARMER UNION JACK', 'HAND WARMER OWL DESIGN'})</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -2668,7 +2668,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER OWL DESIGN', 'HAND WARMER UNION JACK'})</t>
+          <t>frozenset({'HAND WARMER UNION JACK', 'HAND WARMER OWL DESIGN'})</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -2812,7 +2812,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER OWL DESIGN', 'HAND WARMER SCOTTY DOG DESIGN'})</t>
+          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN', 'HAND WARMER OWL DESIGN'})</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -2865,7 +2865,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER OWL DESIGN', 'HAND WARMER SCOTTY DOG DESIGN'})</t>
+          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN', 'HAND WARMER OWL DESIGN'})</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -2913,7 +2913,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER SCOTTY DOG DESIGN'})</t>
+          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN', 'HAND WARMER BIRD DESIGN'})</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -2956,7 +2956,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER SCOTTY DOG DESIGN'})</t>
+          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN', 'HAND WARMER BIRD DESIGN'})</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -3004,25 +3004,25 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN'})</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER OWL DESIGN'})</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN'})</t>
-        </is>
-      </c>
       <c r="C54" t="n">
+        <v>0.09922680412371133</v>
+      </c>
+      <c r="D54" t="n">
         <v>0.05798969072164949</v>
-      </c>
-      <c r="D54" t="n">
-        <v>0.09922680412371133</v>
       </c>
       <c r="E54" t="n">
         <v>0.03994845360824742</v>
       </c>
       <c r="F54" t="n">
-        <v>0.6888888888888888</v>
+        <v>0.4025974025974026</v>
       </c>
       <c r="G54" t="n">
         <v>6.942568542568542</v>
@@ -3034,16 +3034,16 @@
         <v>0.0341943219258157</v>
       </c>
       <c r="J54" t="n">
-        <v>2.895342415316641</v>
+        <v>1.576843343792022</v>
       </c>
       <c r="K54" t="n">
-        <v>0.9086536339967344</v>
+        <v>0.950251511375698</v>
       </c>
       <c r="L54" t="n">
         <v>0.3406593406593406</v>
       </c>
       <c r="M54" t="n">
-        <v>0.6546177078365918</v>
+        <v>0.3658215929077762</v>
       </c>
       <c r="N54" t="n">
         <v>0.5457431457431456</v>
@@ -3052,25 +3052,25 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER OWL DESIGN'})</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN'})</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER OWL DESIGN'})</t>
-        </is>
-      </c>
       <c r="C55" t="n">
+        <v>0.05798969072164949</v>
+      </c>
+      <c r="D55" t="n">
         <v>0.09922680412371133</v>
-      </c>
-      <c r="D55" t="n">
-        <v>0.05798969072164949</v>
       </c>
       <c r="E55" t="n">
         <v>0.03994845360824742</v>
       </c>
       <c r="F55" t="n">
-        <v>0.4025974025974026</v>
+        <v>0.6888888888888888</v>
       </c>
       <c r="G55" t="n">
         <v>6.942568542568542</v>
@@ -3082,16 +3082,16 @@
         <v>0.0341943219258157</v>
       </c>
       <c r="J55" t="n">
-        <v>1.576843343792022</v>
+        <v>2.895342415316641</v>
       </c>
       <c r="K55" t="n">
-        <v>0.950251511375698</v>
+        <v>0.9086536339967344</v>
       </c>
       <c r="L55" t="n">
         <v>0.3406593406593406</v>
       </c>
       <c r="M55" t="n">
-        <v>0.3658215929077762</v>
+        <v>0.6546177078365918</v>
       </c>
       <c r="N55" t="n">
         <v>0.5457431457431456</v>
@@ -3100,25 +3100,25 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
+          <t>frozenset({'HEART OF WICKER LARGE'})</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
           <t>frozenset({'HEART OF WICKER SMALL'})</t>
         </is>
       </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>frozenset({'HEART OF WICKER LARGE'})</t>
-        </is>
-      </c>
       <c r="C56" t="n">
+        <v>0.07860824742268041</v>
+      </c>
+      <c r="D56" t="n">
         <v>0.08505154639175258</v>
-      </c>
-      <c r="D56" t="n">
-        <v>0.07860824742268041</v>
       </c>
       <c r="E56" t="n">
         <v>0.04639175257731959</v>
       </c>
       <c r="F56" t="n">
-        <v>0.5454545454545454</v>
+        <v>0.5901639344262295</v>
       </c>
       <c r="G56" t="n">
         <v>6.938897168405365</v>
@@ -3130,16 +3130,16 @@
         <v>0.03970599957487512</v>
       </c>
       <c r="J56" t="n">
-        <v>2.027061855670103</v>
+        <v>2.232474226804124</v>
       </c>
       <c r="K56" t="n">
-        <v>0.9354460093896714</v>
+        <v>0.9289044289044287</v>
       </c>
       <c r="L56" t="n">
         <v>0.3956043956043956</v>
       </c>
       <c r="M56" t="n">
-        <v>0.5066751430387794</v>
+        <v>0.552066497344724</v>
       </c>
       <c r="N56" t="n">
         <v>0.5678092399403875</v>
@@ -3148,25 +3148,25 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
+          <t>frozenset({'HEART OF WICKER SMALL'})</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
           <t>frozenset({'HEART OF WICKER LARGE'})</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>frozenset({'HEART OF WICKER SMALL'})</t>
-        </is>
-      </c>
       <c r="C57" t="n">
+        <v>0.08505154639175258</v>
+      </c>
+      <c r="D57" t="n">
         <v>0.07860824742268041</v>
-      </c>
-      <c r="D57" t="n">
-        <v>0.08505154639175258</v>
       </c>
       <c r="E57" t="n">
         <v>0.04639175257731959</v>
       </c>
       <c r="F57" t="n">
-        <v>0.5901639344262295</v>
+        <v>0.5454545454545454</v>
       </c>
       <c r="G57" t="n">
         <v>6.938897168405365</v>
@@ -3178,16 +3178,16 @@
         <v>0.03970599957487512</v>
       </c>
       <c r="J57" t="n">
-        <v>2.232474226804124</v>
+        <v>2.027061855670103</v>
       </c>
       <c r="K57" t="n">
-        <v>0.9289044289044287</v>
+        <v>0.9354460093896714</v>
       </c>
       <c r="L57" t="n">
         <v>0.3956043956043956</v>
       </c>
       <c r="M57" t="n">
-        <v>0.552066497344724</v>
+        <v>0.5066751430387794</v>
       </c>
       <c r="N57" t="n">
         <v>0.5678092399403875</v>
@@ -3297,7 +3297,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER SCOTTY DOG DESIGN'})</t>
+          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN', 'HAND WARMER BIRD DESIGN'})</t>
         </is>
       </c>
       <c r="C60" t="n">
@@ -3340,7 +3340,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER SCOTTY DOG DESIGN'})</t>
+          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN', 'HAND WARMER BIRD DESIGN'})</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -3676,25 +3676,25 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
+          <t>frozenset({'PAPER CHAIN KIT VINTAGE CHRISTMAS'})</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
           <t>frozenset({'60 CAKE CASES VINTAGE CHRISTMAS'})</t>
         </is>
       </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>frozenset({'PAPER CHAIN KIT VINTAGE CHRISTMAS'})</t>
-        </is>
-      </c>
       <c r="C68" t="n">
+        <v>0.09020618556701031</v>
+      </c>
+      <c r="D68" t="n">
         <v>0.05798969072164949</v>
-      </c>
-      <c r="D68" t="n">
-        <v>0.09020618556701031</v>
       </c>
       <c r="E68" t="n">
         <v>0.03479381443298969</v>
       </c>
       <c r="F68" t="n">
-        <v>0.6</v>
+        <v>0.3857142857142857</v>
       </c>
       <c r="G68" t="n">
         <v>6.651428571428571</v>
@@ -3706,16 +3706,16 @@
         <v>0.02956278563077904</v>
       </c>
       <c r="J68" t="n">
-        <v>2.274484536082474</v>
+        <v>1.533505154639175</v>
       </c>
       <c r="K68" t="n">
-        <v>0.9019607843137255</v>
+        <v>0.9338999055712937</v>
       </c>
       <c r="L68" t="n">
         <v>0.3068181818181818</v>
       </c>
       <c r="M68" t="n">
-        <v>0.5603399433427761</v>
+        <v>0.3478991596638655</v>
       </c>
       <c r="N68" t="n">
         <v>0.4928571428571429</v>
@@ -3724,25 +3724,25 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
+          <t>frozenset({'60 CAKE CASES VINTAGE CHRISTMAS'})</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
           <t>frozenset({'PAPER CHAIN KIT VINTAGE CHRISTMAS'})</t>
         </is>
       </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>frozenset({'60 CAKE CASES VINTAGE CHRISTMAS'})</t>
-        </is>
-      </c>
       <c r="C69" t="n">
+        <v>0.05798969072164949</v>
+      </c>
+      <c r="D69" t="n">
         <v>0.09020618556701031</v>
-      </c>
-      <c r="D69" t="n">
-        <v>0.05798969072164949</v>
       </c>
       <c r="E69" t="n">
         <v>0.03479381443298969</v>
       </c>
       <c r="F69" t="n">
-        <v>0.3857142857142857</v>
+        <v>0.6</v>
       </c>
       <c r="G69" t="n">
         <v>6.651428571428571</v>
@@ -3754,16 +3754,16 @@
         <v>0.02956278563077904</v>
       </c>
       <c r="J69" t="n">
-        <v>1.533505154639175</v>
+        <v>2.274484536082474</v>
       </c>
       <c r="K69" t="n">
-        <v>0.9338999055712937</v>
+        <v>0.9019607843137255</v>
       </c>
       <c r="L69" t="n">
         <v>0.3068181818181818</v>
       </c>
       <c r="M69" t="n">
-        <v>0.3478991596638655</v>
+        <v>0.5603399433427761</v>
       </c>
       <c r="N69" t="n">
         <v>0.4928571428571429</v>
@@ -3772,25 +3772,25 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER OWL DESIGN'})</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN'})</t>
         </is>
       </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER OWL DESIGN'})</t>
-        </is>
-      </c>
       <c r="C70" t="n">
+        <v>0.09793814432989691</v>
+      </c>
+      <c r="D70" t="n">
         <v>0.09922680412371133</v>
-      </c>
-      <c r="D70" t="n">
-        <v>0.09793814432989691</v>
       </c>
       <c r="E70" t="n">
         <v>0.06443298969072164</v>
       </c>
       <c r="F70" t="n">
-        <v>0.6493506493506493</v>
+        <v>0.6578947368421052</v>
       </c>
       <c r="G70" t="n">
         <v>6.630211893369788</v>
@@ -3802,16 +3802,16 @@
         <v>0.05471490062705919</v>
       </c>
       <c r="J70" t="n">
-        <v>2.572546773577701</v>
+        <v>2.633029341792228</v>
       </c>
       <c r="K70" t="n">
-        <v>0.9427181688125893</v>
+        <v>0.9413714285714285</v>
       </c>
       <c r="L70" t="n">
         <v>0.4854368932038834</v>
       </c>
       <c r="M70" t="n">
-        <v>0.6112801484230056</v>
+        <v>0.6202093215872299</v>
       </c>
       <c r="N70" t="n">
         <v>0.6536226930963773</v>
@@ -3820,25 +3820,25 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN'})</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER OWL DESIGN'})</t>
         </is>
       </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN'})</t>
-        </is>
-      </c>
       <c r="C71" t="n">
+        <v>0.09922680412371133</v>
+      </c>
+      <c r="D71" t="n">
         <v>0.09793814432989691</v>
-      </c>
-      <c r="D71" t="n">
-        <v>0.09922680412371133</v>
       </c>
       <c r="E71" t="n">
         <v>0.06443298969072164</v>
       </c>
       <c r="F71" t="n">
-        <v>0.6578947368421052</v>
+        <v>0.6493506493506493</v>
       </c>
       <c r="G71" t="n">
         <v>6.630211893369788</v>
@@ -3850,16 +3850,16 @@
         <v>0.05471490062705919</v>
       </c>
       <c r="J71" t="n">
-        <v>2.633029341792228</v>
+        <v>2.572546773577701</v>
       </c>
       <c r="K71" t="n">
-        <v>0.9413714285714285</v>
+        <v>0.9427181688125893</v>
       </c>
       <c r="L71" t="n">
         <v>0.4854368932038834</v>
       </c>
       <c r="M71" t="n">
-        <v>0.6202093215872299</v>
+        <v>0.6112801484230056</v>
       </c>
       <c r="N71" t="n">
         <v>0.6536226930963773</v>
@@ -3873,7 +3873,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER UNION JACK'})</t>
+          <t>frozenset({'HAND WARMER UNION JACK', 'HAND WARMER BIRD DESIGN'})</t>
         </is>
       </c>
       <c r="C72" t="n">
@@ -3916,7 +3916,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER UNION JACK'})</t>
+          <t>frozenset({'HAND WARMER UNION JACK', 'HAND WARMER BIRD DESIGN'})</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -3964,25 +3964,25 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER RED RETROSPOT'})</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER OWL DESIGN'})</t>
         </is>
       </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER RED RETROSPOT'})</t>
-        </is>
-      </c>
       <c r="C74" t="n">
+        <v>0.08505154639175258</v>
+      </c>
+      <c r="D74" t="n">
         <v>0.05798969072164949</v>
-      </c>
-      <c r="D74" t="n">
-        <v>0.08505154639175258</v>
       </c>
       <c r="E74" t="n">
         <v>0.03221649484536082</v>
       </c>
       <c r="F74" t="n">
-        <v>0.5555555555555555</v>
+        <v>0.3787878787878787</v>
       </c>
       <c r="G74" t="n">
         <v>6.531986531986531</v>
@@ -3994,16 +3994,16 @@
         <v>0.02728438197470507</v>
       </c>
       <c r="J74" t="n">
-        <v>2.058634020618556</v>
+        <v>1.516406839326125</v>
       </c>
       <c r="K74" t="n">
-        <v>0.8990424076607387</v>
+        <v>0.9256338028169014</v>
       </c>
       <c r="L74" t="n">
         <v>0.2906976744186046</v>
       </c>
       <c r="M74" t="n">
-        <v>0.5142410015649451</v>
+        <v>0.3405463665381585</v>
       </c>
       <c r="N74" t="n">
         <v>0.4671717171717171</v>
@@ -4012,25 +4012,25 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER OWL DESIGN'})</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER RED RETROSPOT'})</t>
         </is>
       </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER OWL DESIGN'})</t>
-        </is>
-      </c>
       <c r="C75" t="n">
+        <v>0.05798969072164949</v>
+      </c>
+      <c r="D75" t="n">
         <v>0.08505154639175258</v>
-      </c>
-      <c r="D75" t="n">
-        <v>0.05798969072164949</v>
       </c>
       <c r="E75" t="n">
         <v>0.03221649484536082</v>
       </c>
       <c r="F75" t="n">
-        <v>0.3787878787878787</v>
+        <v>0.5555555555555555</v>
       </c>
       <c r="G75" t="n">
         <v>6.531986531986531</v>
@@ -4042,16 +4042,16 @@
         <v>0.02728438197470507</v>
       </c>
       <c r="J75" t="n">
-        <v>1.516406839326125</v>
+        <v>2.058634020618556</v>
       </c>
       <c r="K75" t="n">
-        <v>0.9256338028169014</v>
+        <v>0.8990424076607387</v>
       </c>
       <c r="L75" t="n">
         <v>0.2906976744186046</v>
       </c>
       <c r="M75" t="n">
-        <v>0.3405463665381585</v>
+        <v>0.5142410015649451</v>
       </c>
       <c r="N75" t="n">
         <v>0.4671717171717171</v>
@@ -4065,7 +4065,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER UNION JACK'})</t>
+          <t>frozenset({'HAND WARMER UNION JACK', 'HAND WARMER BIRD DESIGN'})</t>
         </is>
       </c>
       <c r="C76" t="n">
@@ -4108,7 +4108,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER UNION JACK'})</t>
+          <t>frozenset({'HAND WARMER UNION JACK', 'HAND WARMER BIRD DESIGN'})</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -4348,25 +4348,25 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
+          <t>frozenset({'HOT WATER BOTTLE TEA AND SYMPATHY'})</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
           <t>frozenset({'CHOCOLATE HOT WATER BOTTLE'})</t>
         </is>
       </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>frozenset({'HOT WATER BOTTLE TEA AND SYMPATHY'})</t>
-        </is>
-      </c>
       <c r="C82" t="n">
+        <v>0.09278350515463918</v>
+      </c>
+      <c r="D82" t="n">
         <v>0.07860824742268041</v>
-      </c>
-      <c r="D82" t="n">
-        <v>0.09278350515463918</v>
       </c>
       <c r="E82" t="n">
         <v>0.04639175257731959</v>
       </c>
       <c r="F82" t="n">
-        <v>0.5901639344262295</v>
+        <v>0.5</v>
       </c>
       <c r="G82" t="n">
         <v>6.360655737704918</v>
@@ -4378,16 +4378,16 @@
         <v>0.03909820384738017</v>
       </c>
       <c r="J82" t="n">
-        <v>2.21360824742268</v>
+        <v>1.842783505154639</v>
       </c>
       <c r="K82" t="n">
-        <v>0.9146853146853147</v>
+        <v>0.9289772727272728</v>
       </c>
       <c r="L82" t="n">
         <v>0.3711340206185567</v>
       </c>
       <c r="M82" t="n">
-        <v>0.5482488822652757</v>
+        <v>0.4573426573426573</v>
       </c>
       <c r="N82" t="n">
         <v>0.5450819672131147</v>
@@ -4396,25 +4396,25 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
+          <t>frozenset({'CHOCOLATE HOT WATER BOTTLE'})</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
           <t>frozenset({'HOT WATER BOTTLE TEA AND SYMPATHY'})</t>
         </is>
       </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>frozenset({'CHOCOLATE HOT WATER BOTTLE'})</t>
-        </is>
-      </c>
       <c r="C83" t="n">
+        <v>0.07860824742268041</v>
+      </c>
+      <c r="D83" t="n">
         <v>0.09278350515463918</v>
-      </c>
-      <c r="D83" t="n">
-        <v>0.07860824742268041</v>
       </c>
       <c r="E83" t="n">
         <v>0.04639175257731959</v>
       </c>
       <c r="F83" t="n">
-        <v>0.5</v>
+        <v>0.5901639344262295</v>
       </c>
       <c r="G83" t="n">
         <v>6.360655737704918</v>
@@ -4426,16 +4426,16 @@
         <v>0.03909820384738017</v>
       </c>
       <c r="J83" t="n">
-        <v>1.842783505154639</v>
+        <v>2.21360824742268</v>
       </c>
       <c r="K83" t="n">
-        <v>0.9289772727272728</v>
+        <v>0.9146853146853147</v>
       </c>
       <c r="L83" t="n">
         <v>0.3711340206185567</v>
       </c>
       <c r="M83" t="n">
-        <v>0.4573426573426573</v>
+        <v>0.5482488822652757</v>
       </c>
       <c r="N83" t="n">
         <v>0.5450819672131147</v>
@@ -4444,25 +4444,25 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
+          <t>frozenset({'HOT WATER BOTTLE I AM SO POORLY'})</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
           <t>frozenset({'WHITE SKULL HOT WATER BOTTLE '})</t>
         </is>
       </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>frozenset({'HOT WATER BOTTLE I AM SO POORLY'})</t>
-        </is>
-      </c>
       <c r="C84" t="n">
+        <v>0.05798969072164949</v>
+      </c>
+      <c r="D84" t="n">
         <v>0.08505154639175258</v>
-      </c>
-      <c r="D84" t="n">
-        <v>0.05798969072164949</v>
       </c>
       <c r="E84" t="n">
         <v>0.03092783505154639</v>
       </c>
       <c r="F84" t="n">
-        <v>0.3636363636363636</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="G84" t="n">
         <v>6.27070707070707</v>
@@ -4474,16 +4474,16 @@
         <v>0.02599572218089064</v>
       </c>
       <c r="J84" t="n">
-        <v>1.480301914580265</v>
+        <v>1.96060382916053</v>
       </c>
       <c r="K84" t="n">
-        <v>0.918661971830986</v>
+        <v>0.8922708618331053</v>
       </c>
       <c r="L84" t="n">
         <v>0.2758620689655173</v>
       </c>
       <c r="M84" t="n">
-        <v>0.3244621315756747</v>
+        <v>0.4899530516431925</v>
       </c>
       <c r="N84" t="n">
         <v>0.4484848484848485</v>
@@ -4492,25 +4492,25 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
+          <t>frozenset({'WHITE SKULL HOT WATER BOTTLE '})</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
           <t>frozenset({'HOT WATER BOTTLE I AM SO POORLY'})</t>
         </is>
       </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>frozenset({'WHITE SKULL HOT WATER BOTTLE '})</t>
-        </is>
-      </c>
       <c r="C85" t="n">
+        <v>0.08505154639175258</v>
+      </c>
+      <c r="D85" t="n">
         <v>0.05798969072164949</v>
-      </c>
-      <c r="D85" t="n">
-        <v>0.08505154639175258</v>
       </c>
       <c r="E85" t="n">
         <v>0.03092783505154639</v>
       </c>
       <c r="F85" t="n">
-        <v>0.5333333333333333</v>
+        <v>0.3636363636363636</v>
       </c>
       <c r="G85" t="n">
         <v>6.27070707070707</v>
@@ -4522,16 +4522,16 @@
         <v>0.02599572218089064</v>
       </c>
       <c r="J85" t="n">
-        <v>1.96060382916053</v>
+        <v>1.480301914580265</v>
       </c>
       <c r="K85" t="n">
-        <v>0.8922708618331053</v>
+        <v>0.918661971830986</v>
       </c>
       <c r="L85" t="n">
         <v>0.2758620689655173</v>
       </c>
       <c r="M85" t="n">
-        <v>0.4899530516431925</v>
+        <v>0.3244621315756747</v>
       </c>
       <c r="N85" t="n">
         <v>0.4484848484848485</v>
@@ -4636,25 +4636,25 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN'})</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER RED RETROSPOT'})</t>
         </is>
       </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN'})</t>
-        </is>
-      </c>
       <c r="C88" t="n">
+        <v>0.09922680412371133</v>
+      </c>
+      <c r="D88" t="n">
         <v>0.08505154639175258</v>
-      </c>
-      <c r="D88" t="n">
-        <v>0.09922680412371133</v>
       </c>
       <c r="E88" t="n">
         <v>0.05154639175257732</v>
       </c>
       <c r="F88" t="n">
-        <v>0.606060606060606</v>
+        <v>0.5194805194805194</v>
       </c>
       <c r="G88" t="n">
         <v>6.107831562377016</v>
@@ -4666,16 +4666,16 @@
         <v>0.04310699861834413</v>
       </c>
       <c r="J88" t="n">
-        <v>2.28657811260904</v>
+        <v>1.904081916968515</v>
       </c>
       <c r="K88" t="n">
-        <v>0.9140140845070422</v>
+        <v>0.9283977110157366</v>
       </c>
       <c r="L88" t="n">
         <v>0.3883495145631067</v>
       </c>
       <c r="M88" t="n">
-        <v>0.5626652794034768</v>
+        <v>0.4748125114322297</v>
       </c>
       <c r="N88" t="n">
         <v>0.5627705627705627</v>
@@ -4684,25 +4684,25 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER RED RETROSPOT'})</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN'})</t>
         </is>
       </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER RED RETROSPOT'})</t>
-        </is>
-      </c>
       <c r="C89" t="n">
+        <v>0.08505154639175258</v>
+      </c>
+      <c r="D89" t="n">
         <v>0.09922680412371133</v>
-      </c>
-      <c r="D89" t="n">
-        <v>0.08505154639175258</v>
       </c>
       <c r="E89" t="n">
         <v>0.05154639175257732</v>
       </c>
       <c r="F89" t="n">
-        <v>0.5194805194805194</v>
+        <v>0.606060606060606</v>
       </c>
       <c r="G89" t="n">
         <v>6.107831562377016</v>
@@ -4714,16 +4714,16 @@
         <v>0.04310699861834413</v>
       </c>
       <c r="J89" t="n">
-        <v>1.904081916968515</v>
+        <v>2.28657811260904</v>
       </c>
       <c r="K89" t="n">
-        <v>0.9283977110157366</v>
+        <v>0.9140140845070422</v>
       </c>
       <c r="L89" t="n">
         <v>0.3883495145631067</v>
       </c>
       <c r="M89" t="n">
-        <v>0.4748125114322297</v>
+        <v>0.5626652794034768</v>
       </c>
       <c r="N89" t="n">
         <v>0.5627705627705627</v>
@@ -5500,7 +5500,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER OWL DESIGN', 'HAND WARMER UNION JACK'})</t>
+          <t>frozenset({'HAND WARMER UNION JACK', 'HAND WARMER OWL DESIGN'})</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -5553,7 +5553,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER OWL DESIGN', 'HAND WARMER UNION JACK'})</t>
+          <t>frozenset({'HAND WARMER UNION JACK', 'HAND WARMER OWL DESIGN'})</t>
         </is>
       </c>
       <c r="C107" t="n">
@@ -5596,25 +5596,25 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
+          <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.', 'KNITTED UNION FLAG HOT WATER BOTTLE'})</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
           <t>frozenset({'WHITE HANGING HEART T-LIGHT HOLDER'})</t>
         </is>
       </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>frozenset({'KNITTED UNION FLAG HOT WATER BOTTLE', 'RED WOOLLY HOTTIE WHITE HEART.'})</t>
-        </is>
-      </c>
       <c r="C108" t="n">
+        <v>0.05283505154639175</v>
+      </c>
+      <c r="D108" t="n">
         <v>0.1378865979381443</v>
-      </c>
-      <c r="D108" t="n">
-        <v>0.05283505154639175</v>
       </c>
       <c r="E108" t="n">
         <v>0.03865979381443299</v>
       </c>
       <c r="F108" t="n">
-        <v>0.2803738317757009</v>
+        <v>0.7317073170731707</v>
       </c>
       <c r="G108" t="n">
         <v>5.306587645315705</v>
@@ -5626,16 +5626,16 @@
         <v>0.03137454830481454</v>
       </c>
       <c r="J108" t="n">
-        <v>1.316190253045923</v>
+        <v>3.213331771321462</v>
       </c>
       <c r="K108" t="n">
-        <v>0.9413552566018932</v>
+        <v>0.8568253968253967</v>
       </c>
       <c r="L108" t="n">
         <v>0.2542372881355932</v>
       </c>
       <c r="M108" t="n">
-        <v>0.240231419670672</v>
+        <v>0.6887965292208976</v>
       </c>
       <c r="N108" t="n">
         <v>0.5060405744244358</v>
@@ -5644,25 +5644,25 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>frozenset({'KNITTED UNION FLAG HOT WATER BOTTLE', 'RED WOOLLY HOTTIE WHITE HEART.'})</t>
+          <t>frozenset({'WHITE HANGING HEART T-LIGHT HOLDER'})</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>frozenset({'WHITE HANGING HEART T-LIGHT HOLDER'})</t>
+          <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.', 'KNITTED UNION FLAG HOT WATER BOTTLE'})</t>
         </is>
       </c>
       <c r="C109" t="n">
+        <v>0.1378865979381443</v>
+      </c>
+      <c r="D109" t="n">
         <v>0.05283505154639175</v>
-      </c>
-      <c r="D109" t="n">
-        <v>0.1378865979381443</v>
       </c>
       <c r="E109" t="n">
         <v>0.03865979381443299</v>
       </c>
       <c r="F109" t="n">
-        <v>0.7317073170731707</v>
+        <v>0.2803738317757009</v>
       </c>
       <c r="G109" t="n">
         <v>5.306587645315705</v>
@@ -5674,16 +5674,16 @@
         <v>0.03137454830481454</v>
       </c>
       <c r="J109" t="n">
-        <v>3.213331771321462</v>
+        <v>1.316190253045923</v>
       </c>
       <c r="K109" t="n">
-        <v>0.8568253968253967</v>
+        <v>0.9413552566018932</v>
       </c>
       <c r="L109" t="n">
         <v>0.2542372881355932</v>
       </c>
       <c r="M109" t="n">
-        <v>0.6887965292208976</v>
+        <v>0.240231419670672</v>
       </c>
       <c r="N109" t="n">
         <v>0.5060405744244358</v>
@@ -5884,25 +5884,25 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
+          <t>frozenset({'SCOTTIE DOG HOT WATER BOTTLE'})</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
           <t>frozenset({'FAWN BLUE HOT WATER BOTTLE'})</t>
         </is>
       </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>frozenset({'SCOTTIE DOG HOT WATER BOTTLE'})</t>
-        </is>
-      </c>
       <c r="C114" t="n">
+        <v>0.08762886597938144</v>
+      </c>
+      <c r="D114" t="n">
         <v>0.06829896907216494</v>
-      </c>
-      <c r="D114" t="n">
-        <v>0.08762886597938144</v>
       </c>
       <c r="E114" t="n">
         <v>0.03092783505154639</v>
       </c>
       <c r="F114" t="n">
-        <v>0.4528301886792453</v>
+        <v>0.3529411764705883</v>
       </c>
       <c r="G114" t="n">
         <v>5.167591564927859</v>
@@ -5914,16 +5914,16 @@
         <v>0.02494287384419173</v>
       </c>
       <c r="J114" t="n">
-        <v>1.667436900106648</v>
+        <v>1.439901593252109</v>
       </c>
       <c r="K114" t="n">
-        <v>0.8656062701705857</v>
+        <v>0.8839453860640303</v>
       </c>
       <c r="L114" t="n">
         <v>0.2474226804123711</v>
       </c>
       <c r="M114" t="n">
-        <v>0.4002771559535232</v>
+        <v>0.3055080953543243</v>
       </c>
       <c r="N114" t="n">
         <v>0.4028856825749168</v>
@@ -5932,25 +5932,25 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
+          <t>frozenset({'FAWN BLUE HOT WATER BOTTLE'})</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
           <t>frozenset({'SCOTTIE DOG HOT WATER BOTTLE'})</t>
         </is>
       </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>frozenset({'FAWN BLUE HOT WATER BOTTLE'})</t>
-        </is>
-      </c>
       <c r="C115" t="n">
+        <v>0.06829896907216494</v>
+      </c>
+      <c r="D115" t="n">
         <v>0.08762886597938144</v>
-      </c>
-      <c r="D115" t="n">
-        <v>0.06829896907216494</v>
       </c>
       <c r="E115" t="n">
         <v>0.03092783505154639</v>
       </c>
       <c r="F115" t="n">
-        <v>0.3529411764705883</v>
+        <v>0.4528301886792453</v>
       </c>
       <c r="G115" t="n">
         <v>5.167591564927859</v>
@@ -5962,16 +5962,16 @@
         <v>0.02494287384419173</v>
       </c>
       <c r="J115" t="n">
-        <v>1.439901593252109</v>
+        <v>1.667436900106648</v>
       </c>
       <c r="K115" t="n">
-        <v>0.8839453860640303</v>
+        <v>0.8656062701705857</v>
       </c>
       <c r="L115" t="n">
         <v>0.2474226804123711</v>
       </c>
       <c r="M115" t="n">
-        <v>0.3055080953543243</v>
+        <v>0.4002771559535232</v>
       </c>
       <c r="N115" t="n">
         <v>0.4028856825749168</v>
@@ -5985,7 +5985,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER OWL DESIGN', 'HAND WARMER RED RETROSPOT'})</t>
+          <t>frozenset({'HAND WARMER RED RETROSPOT', 'HAND WARMER OWL DESIGN'})</t>
         </is>
       </c>
       <c r="C116" t="n">
@@ -6028,7 +6028,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER UNION JACK', 'HAND WARMER SCOTTY DOG DESIGN'})</t>
+          <t>frozenset({'HAND WARMER RED RETROSPOT', 'HAND WARMER OWL DESIGN'})</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -6124,7 +6124,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER OWL DESIGN', 'HAND WARMER RED RETROSPOT'})</t>
+          <t>frozenset({'HAND WARMER UNION JACK', 'HAND WARMER SCOTTY DOG DESIGN'})</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -6172,25 +6172,25 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
+          <t>frozenset({'WHITE METAL LANTERN'})</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
           <t>frozenset({'WHITE HANGING HEART T-LIGHT HOLDER'})</t>
         </is>
       </c>
-      <c r="B120" t="inlineStr">
-        <is>
-          <t>frozenset({'WHITE METAL LANTERN'})</t>
-        </is>
-      </c>
       <c r="C120" t="n">
+        <v>0.04381443298969072</v>
+      </c>
+      <c r="D120" t="n">
         <v>0.1378865979381443</v>
-      </c>
-      <c r="D120" t="n">
-        <v>0.04381443298969072</v>
       </c>
       <c r="E120" t="n">
         <v>0.03092783505154639</v>
       </c>
       <c r="F120" t="n">
-        <v>0.2242990654205607</v>
+        <v>0.7058823529411765</v>
       </c>
       <c r="G120" t="n">
         <v>5.119296316657504</v>
@@ -6202,16 +6202,16 @@
         <v>0.02488641194600914</v>
       </c>
       <c r="J120" t="n">
-        <v>1.23267295988076</v>
+        <v>2.93118556701031</v>
       </c>
       <c r="K120" t="n">
-        <v>0.9333582461385151</v>
+        <v>0.8415318957771788</v>
       </c>
       <c r="L120" t="n">
         <v>0.2051282051282051</v>
       </c>
       <c r="M120" t="n">
-        <v>0.1887548177444139</v>
+        <v>0.6588411149213048</v>
       </c>
       <c r="N120" t="n">
         <v>0.4650907091808686</v>
@@ -6220,25 +6220,25 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
+          <t>frozenset({'WHITE HANGING HEART T-LIGHT HOLDER'})</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
           <t>frozenset({'WHITE METAL LANTERN'})</t>
         </is>
       </c>
-      <c r="B121" t="inlineStr">
-        <is>
-          <t>frozenset({'WHITE HANGING HEART T-LIGHT HOLDER'})</t>
-        </is>
-      </c>
       <c r="C121" t="n">
+        <v>0.1378865979381443</v>
+      </c>
+      <c r="D121" t="n">
         <v>0.04381443298969072</v>
-      </c>
-      <c r="D121" t="n">
-        <v>0.1378865979381443</v>
       </c>
       <c r="E121" t="n">
         <v>0.03092783505154639</v>
       </c>
       <c r="F121" t="n">
-        <v>0.7058823529411765</v>
+        <v>0.2242990654205607</v>
       </c>
       <c r="G121" t="n">
         <v>5.119296316657504</v>
@@ -6250,16 +6250,16 @@
         <v>0.02488641194600914</v>
       </c>
       <c r="J121" t="n">
-        <v>2.93118556701031</v>
+        <v>1.23267295988076</v>
       </c>
       <c r="K121" t="n">
-        <v>0.8415318957771788</v>
+        <v>0.9333582461385151</v>
       </c>
       <c r="L121" t="n">
         <v>0.2051282051282051</v>
       </c>
       <c r="M121" t="n">
-        <v>0.6588411149213048</v>
+        <v>0.1887548177444139</v>
       </c>
       <c r="N121" t="n">
         <v>0.4650907091808686</v>
@@ -6268,7 +6268,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER RED RETROSPOT', 'HAND WARMER SCOTTY DOG DESIGN'})</t>
+          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN', 'HAND WARMER RED RETROSPOT'})</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -6369,7 +6369,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER RED RETROSPOT', 'HAND WARMER SCOTTY DOG DESIGN'})</t>
+          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN', 'HAND WARMER RED RETROSPOT'})</t>
         </is>
       </c>
       <c r="C124" t="n">
@@ -6556,25 +6556,25 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN', 'HAND WARMER BIRD DESIGN'})</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER UNION JACK'})</t>
         </is>
       </c>
-      <c r="B128" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER SCOTTY DOG DESIGN'})</t>
-        </is>
-      </c>
       <c r="C128" t="n">
+        <v>0.05798969072164949</v>
+      </c>
+      <c r="D128" t="n">
         <v>0.1134020618556701</v>
-      </c>
-      <c r="D128" t="n">
-        <v>0.05798969072164949</v>
       </c>
       <c r="E128" t="n">
         <v>0.03221649484536082</v>
       </c>
       <c r="F128" t="n">
-        <v>0.2840909090909091</v>
+        <v>0.5555555555555555</v>
       </c>
       <c r="G128" t="n">
         <v>4.898989898989898</v>
@@ -6586,16 +6586,16 @@
         <v>0.02564034435115315</v>
       </c>
       <c r="J128" t="n">
-        <v>1.315823924071347</v>
+        <v>1.994845360824742</v>
       </c>
       <c r="K128" t="n">
-        <v>0.8976744186046511</v>
+        <v>0.8448700410396717</v>
       </c>
       <c r="L128" t="n">
         <v>0.2314814814814815</v>
       </c>
       <c r="M128" t="n">
-        <v>0.240019898022634</v>
+        <v>0.4987080103359173</v>
       </c>
       <c r="N128" t="n">
         <v>0.4198232323232323</v>
@@ -6604,25 +6604,25 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER SCOTTY DOG DESIGN'})</t>
+          <t>frozenset({'HAND WARMER UNION JACK'})</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER UNION JACK'})</t>
+          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN', 'HAND WARMER BIRD DESIGN'})</t>
         </is>
       </c>
       <c r="C129" t="n">
+        <v>0.1134020618556701</v>
+      </c>
+      <c r="D129" t="n">
         <v>0.05798969072164949</v>
-      </c>
-      <c r="D129" t="n">
-        <v>0.1134020618556701</v>
       </c>
       <c r="E129" t="n">
         <v>0.03221649484536082</v>
       </c>
       <c r="F129" t="n">
-        <v>0.5555555555555555</v>
+        <v>0.2840909090909091</v>
       </c>
       <c r="G129" t="n">
         <v>4.898989898989898</v>
@@ -6634,16 +6634,16 @@
         <v>0.02564034435115315</v>
       </c>
       <c r="J129" t="n">
-        <v>1.994845360824742</v>
+        <v>1.315823924071347</v>
       </c>
       <c r="K129" t="n">
-        <v>0.8448700410396717</v>
+        <v>0.8976744186046511</v>
       </c>
       <c r="L129" t="n">
         <v>0.2314814814814815</v>
       </c>
       <c r="M129" t="n">
-        <v>0.4987080103359173</v>
+        <v>0.240019898022634</v>
       </c>
       <c r="N129" t="n">
         <v>0.4198232323232323</v>
@@ -6945,7 +6945,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER OWL DESIGN', 'HAND WARMER SCOTTY DOG DESIGN'})</t>
+          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN', 'HAND WARMER OWL DESIGN'})</t>
         </is>
       </c>
       <c r="C136" t="n">
@@ -6988,7 +6988,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER OWL DESIGN', 'HAND WARMER SCOTTY DOG DESIGN'})</t>
+          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN', 'HAND WARMER OWL DESIGN'})</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -7036,25 +7036,25 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER UNION JACK'})</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER OWL DESIGN'})</t>
         </is>
       </c>
-      <c r="B138" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER UNION JACK'})</t>
-        </is>
-      </c>
       <c r="C138" t="n">
+        <v>0.1134020618556701</v>
+      </c>
+      <c r="D138" t="n">
         <v>0.05798969072164949</v>
-      </c>
-      <c r="D138" t="n">
-        <v>0.1134020618556701</v>
       </c>
       <c r="E138" t="n">
         <v>0.03092783505154639</v>
       </c>
       <c r="F138" t="n">
-        <v>0.5333333333333333</v>
+        <v>0.2727272727272728</v>
       </c>
       <c r="G138" t="n">
         <v>4.703030303030303</v>
@@ -7066,16 +7066,16 @@
         <v>0.02435168455733872</v>
       </c>
       <c r="J138" t="n">
-        <v>1.899852724594993</v>
+        <v>1.295264175257732</v>
       </c>
       <c r="K138" t="n">
-        <v>0.8358413132694938</v>
+        <v>0.8880813953488372</v>
       </c>
       <c r="L138" t="n">
         <v>0.2201834862385321</v>
       </c>
       <c r="M138" t="n">
-        <v>0.4736434108527132</v>
+        <v>0.2279567218007711</v>
       </c>
       <c r="N138" t="n">
         <v>0.4030303030303031</v>
@@ -7084,25 +7084,25 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER OWL DESIGN'})</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER UNION JACK'})</t>
         </is>
       </c>
-      <c r="B139" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER OWL DESIGN'})</t>
-        </is>
-      </c>
       <c r="C139" t="n">
+        <v>0.05798969072164949</v>
+      </c>
+      <c r="D139" t="n">
         <v>0.1134020618556701</v>
-      </c>
-      <c r="D139" t="n">
-        <v>0.05798969072164949</v>
       </c>
       <c r="E139" t="n">
         <v>0.03092783505154639</v>
       </c>
       <c r="F139" t="n">
-        <v>0.2727272727272728</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="G139" t="n">
         <v>4.703030303030303</v>
@@ -7114,16 +7114,16 @@
         <v>0.02435168455733872</v>
       </c>
       <c r="J139" t="n">
-        <v>1.295264175257732</v>
+        <v>1.899852724594993</v>
       </c>
       <c r="K139" t="n">
-        <v>0.8880813953488372</v>
+        <v>0.8358413132694938</v>
       </c>
       <c r="L139" t="n">
         <v>0.2201834862385321</v>
       </c>
       <c r="M139" t="n">
-        <v>0.2279567218007711</v>
+        <v>0.4736434108527132</v>
       </c>
       <c r="N139" t="n">
         <v>0.4030303030303031</v>
@@ -7132,25 +7132,25 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
+          <t>frozenset({'WHITE SKULL HOT WATER BOTTLE '})</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
           <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.'})</t>
         </is>
       </c>
-      <c r="B140" t="inlineStr">
-        <is>
-          <t>frozenset({'WHITE SKULL HOT WATER BOTTLE '})</t>
-        </is>
-      </c>
       <c r="C140" t="n">
+        <v>0.08505154639175258</v>
+      </c>
+      <c r="D140" t="n">
         <v>0.1005154639175258</v>
-      </c>
-      <c r="D140" t="n">
-        <v>0.08505154639175258</v>
       </c>
       <c r="E140" t="n">
         <v>0.03994845360824742</v>
       </c>
       <c r="F140" t="n">
-        <v>0.3974358974358974</v>
+        <v>0.4696969696969697</v>
       </c>
       <c r="G140" t="n">
         <v>4.672882672882673</v>
@@ -7162,16 +7162,16 @@
         <v>0.03139945796577744</v>
       </c>
       <c r="J140" t="n">
-        <v>1.518425093222198</v>
+        <v>1.696170839469809</v>
       </c>
       <c r="K140" t="n">
-        <v>0.8738330714483777</v>
+        <v>0.8590640617900954</v>
       </c>
       <c r="L140" t="n">
         <v>0.2743362831858407</v>
       </c>
       <c r="M140" t="n">
-        <v>0.3414228963524738</v>
+        <v>0.4104367456802986</v>
       </c>
       <c r="N140" t="n">
         <v>0.4335664335664335</v>
@@ -7180,25 +7180,25 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
+          <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.'})</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
           <t>frozenset({'WHITE SKULL HOT WATER BOTTLE '})</t>
         </is>
       </c>
-      <c r="B141" t="inlineStr">
-        <is>
-          <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.'})</t>
-        </is>
-      </c>
       <c r="C141" t="n">
+        <v>0.1005154639175258</v>
+      </c>
+      <c r="D141" t="n">
         <v>0.08505154639175258</v>
-      </c>
-      <c r="D141" t="n">
-        <v>0.1005154639175258</v>
       </c>
       <c r="E141" t="n">
         <v>0.03994845360824742</v>
       </c>
       <c r="F141" t="n">
-        <v>0.4696969696969697</v>
+        <v>0.3974358974358974</v>
       </c>
       <c r="G141" t="n">
         <v>4.672882672882673</v>
@@ -7210,16 +7210,16 @@
         <v>0.03139945796577744</v>
       </c>
       <c r="J141" t="n">
-        <v>1.696170839469809</v>
+        <v>1.518425093222198</v>
       </c>
       <c r="K141" t="n">
-        <v>0.8590640617900954</v>
+        <v>0.8738330714483777</v>
       </c>
       <c r="L141" t="n">
         <v>0.2743362831858407</v>
       </c>
       <c r="M141" t="n">
-        <v>0.4104367456802986</v>
+        <v>0.3414228963524738</v>
       </c>
       <c r="N141" t="n">
         <v>0.4335664335664335</v>
@@ -7516,25 +7516,25 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
+          <t>frozenset({'WHITE SKULL HOT WATER BOTTLE '})</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
           <t>frozenset({'HOT WATER BOTTLE TEA AND SYMPATHY'})</t>
         </is>
       </c>
-      <c r="B148" t="inlineStr">
-        <is>
-          <t>frozenset({'WHITE SKULL HOT WATER BOTTLE '})</t>
-        </is>
-      </c>
       <c r="C148" t="n">
+        <v>0.08505154639175258</v>
+      </c>
+      <c r="D148" t="n">
         <v>0.09278350515463918</v>
-      </c>
-      <c r="D148" t="n">
-        <v>0.08505154639175258</v>
       </c>
       <c r="E148" t="n">
         <v>0.03608247422680412</v>
       </c>
       <c r="F148" t="n">
-        <v>0.3888888888888888</v>
+        <v>0.4242424242424242</v>
       </c>
       <c r="G148" t="n">
         <v>4.572390572390572</v>
@@ -7546,16 +7546,16 @@
         <v>0.02819109363375491</v>
       </c>
       <c r="J148" t="n">
-        <v>1.497188378631678</v>
+        <v>1.575691806836679</v>
       </c>
       <c r="K148" t="n">
-        <v>0.8612012987012986</v>
+        <v>0.8539235412474848</v>
       </c>
       <c r="L148" t="n">
         <v>0.2545454545454545</v>
       </c>
       <c r="M148" t="n">
-        <v>0.3320813771517996</v>
+        <v>0.365358126721763</v>
       </c>
       <c r="N148" t="n">
         <v>0.4065656565656565</v>
@@ -7564,25 +7564,25 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
+          <t>frozenset({'HOT WATER BOTTLE TEA AND SYMPATHY'})</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
           <t>frozenset({'WHITE SKULL HOT WATER BOTTLE '})</t>
         </is>
       </c>
-      <c r="B149" t="inlineStr">
-        <is>
-          <t>frozenset({'HOT WATER BOTTLE TEA AND SYMPATHY'})</t>
-        </is>
-      </c>
       <c r="C149" t="n">
+        <v>0.09278350515463918</v>
+      </c>
+      <c r="D149" t="n">
         <v>0.08505154639175258</v>
-      </c>
-      <c r="D149" t="n">
-        <v>0.09278350515463918</v>
       </c>
       <c r="E149" t="n">
         <v>0.03608247422680412</v>
       </c>
       <c r="F149" t="n">
-        <v>0.4242424242424242</v>
+        <v>0.3888888888888888</v>
       </c>
       <c r="G149" t="n">
         <v>4.572390572390572</v>
@@ -7594,16 +7594,16 @@
         <v>0.02819109363375491</v>
       </c>
       <c r="J149" t="n">
-        <v>1.575691806836679</v>
+        <v>1.497188378631678</v>
       </c>
       <c r="K149" t="n">
-        <v>0.8539235412474848</v>
+        <v>0.8612012987012986</v>
       </c>
       <c r="L149" t="n">
         <v>0.2545454545454545</v>
       </c>
       <c r="M149" t="n">
-        <v>0.365358126721763</v>
+        <v>0.3320813771517996</v>
       </c>
       <c r="N149" t="n">
         <v>0.4065656565656565</v>
@@ -7612,25 +7612,25 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER OWL DESIGN', 'HAND WARMER SCOTTY DOG DESIGN'})</t>
+          <t>frozenset({'HAND WARMER UNION JACK'})</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER UNION JACK'})</t>
+          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN', 'HAND WARMER OWL DESIGN'})</t>
         </is>
       </c>
       <c r="C150" t="n">
+        <v>0.1134020618556701</v>
+      </c>
+      <c r="D150" t="n">
         <v>0.06443298969072164</v>
-      </c>
-      <c r="D150" t="n">
-        <v>0.1134020618556701</v>
       </c>
       <c r="E150" t="n">
         <v>0.03221649484536082</v>
       </c>
       <c r="F150" t="n">
-        <v>0.5</v>
+        <v>0.2840909090909091</v>
       </c>
       <c r="G150" t="n">
         <v>4.409090909090909</v>
@@ -7642,16 +7642,16 @@
         <v>0.02490966096290785</v>
       </c>
       <c r="J150" t="n">
-        <v>1.77319587628866</v>
+        <v>1.306823760432008</v>
       </c>
       <c r="K150" t="n">
-        <v>0.8264462809917354</v>
+        <v>0.8720930232558139</v>
       </c>
       <c r="L150" t="n">
         <v>0.2212389380530974</v>
       </c>
       <c r="M150" t="n">
-        <v>0.436046511627907</v>
+        <v>0.234785875281743</v>
       </c>
       <c r="N150" t="n">
         <v>0.3920454545454545</v>
@@ -7660,25 +7660,25 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN', 'HAND WARMER OWL DESIGN'})</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER UNION JACK'})</t>
         </is>
       </c>
-      <c r="B151" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER OWL DESIGN', 'HAND WARMER SCOTTY DOG DESIGN'})</t>
-        </is>
-      </c>
       <c r="C151" t="n">
+        <v>0.06443298969072164</v>
+      </c>
+      <c r="D151" t="n">
         <v>0.1134020618556701</v>
-      </c>
-      <c r="D151" t="n">
-        <v>0.06443298969072164</v>
       </c>
       <c r="E151" t="n">
         <v>0.03221649484536082</v>
       </c>
       <c r="F151" t="n">
-        <v>0.2840909090909091</v>
+        <v>0.5</v>
       </c>
       <c r="G151" t="n">
         <v>4.409090909090909</v>
@@ -7690,16 +7690,16 @@
         <v>0.02490966096290785</v>
       </c>
       <c r="J151" t="n">
-        <v>1.306823760432008</v>
+        <v>1.77319587628866</v>
       </c>
       <c r="K151" t="n">
-        <v>0.8720930232558139</v>
+        <v>0.8264462809917354</v>
       </c>
       <c r="L151" t="n">
         <v>0.2212389380530974</v>
       </c>
       <c r="M151" t="n">
-        <v>0.234785875281743</v>
+        <v>0.436046511627907</v>
       </c>
       <c r="N151" t="n">
         <v>0.3920454545454545</v>
@@ -7708,25 +7708,25 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER RED RETROSPOT'})</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER UNION JACK'})</t>
         </is>
       </c>
-      <c r="B152" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER RED RETROSPOT'})</t>
-        </is>
-      </c>
       <c r="C152" t="n">
+        <v>0.08505154639175258</v>
+      </c>
+      <c r="D152" t="n">
         <v>0.1134020618556701</v>
-      </c>
-      <c r="D152" t="n">
-        <v>0.08505154639175258</v>
       </c>
       <c r="E152" t="n">
         <v>0.04252577319587629</v>
       </c>
       <c r="F152" t="n">
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
       <c r="G152" t="n">
         <v>4.409090909090909</v>
@@ -7738,16 +7738,16 @@
         <v>0.03288075247103837</v>
       </c>
       <c r="J152" t="n">
-        <v>1.463917525773196</v>
+        <v>1.77319587628866</v>
       </c>
       <c r="K152" t="n">
-        <v>0.8720930232558141</v>
+        <v>0.8450704225352111</v>
       </c>
       <c r="L152" t="n">
         <v>0.2727272727272728</v>
       </c>
       <c r="M152" t="n">
-        <v>0.3169014084507042</v>
+        <v>0.436046511627907</v>
       </c>
       <c r="N152" t="n">
         <v>0.4375</v>
@@ -7756,25 +7756,25 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER UNION JACK'})</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER RED RETROSPOT'})</t>
         </is>
       </c>
-      <c r="B153" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER UNION JACK'})</t>
-        </is>
-      </c>
       <c r="C153" t="n">
+        <v>0.1134020618556701</v>
+      </c>
+      <c r="D153" t="n">
         <v>0.08505154639175258</v>
-      </c>
-      <c r="D153" t="n">
-        <v>0.1134020618556701</v>
       </c>
       <c r="E153" t="n">
         <v>0.04252577319587629</v>
       </c>
       <c r="F153" t="n">
-        <v>0.5</v>
+        <v>0.375</v>
       </c>
       <c r="G153" t="n">
         <v>4.409090909090909</v>
@@ -7786,16 +7786,16 @@
         <v>0.03288075247103837</v>
       </c>
       <c r="J153" t="n">
-        <v>1.77319587628866</v>
+        <v>1.463917525773196</v>
       </c>
       <c r="K153" t="n">
-        <v>0.8450704225352111</v>
+        <v>0.8720930232558141</v>
       </c>
       <c r="L153" t="n">
         <v>0.2727272727272728</v>
       </c>
       <c r="M153" t="n">
-        <v>0.436046511627907</v>
+        <v>0.3169014084507042</v>
       </c>
       <c r="N153" t="n">
         <v>0.4375</v>
@@ -7804,25 +7804,25 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
+          <t>frozenset({'SCOTTIE DOG HOT WATER BOTTLE'})</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
           <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.'})</t>
         </is>
       </c>
-      <c r="B154" t="inlineStr">
-        <is>
-          <t>frozenset({'SCOTTIE DOG HOT WATER BOTTLE'})</t>
-        </is>
-      </c>
       <c r="C154" t="n">
+        <v>0.08762886597938144</v>
+      </c>
+      <c r="D154" t="n">
         <v>0.1005154639175258</v>
-      </c>
-      <c r="D154" t="n">
-        <v>0.08762886597938144</v>
       </c>
       <c r="E154" t="n">
         <v>0.03865979381443299</v>
       </c>
       <c r="F154" t="n">
-        <v>0.3846153846153846</v>
+        <v>0.4411764705882353</v>
       </c>
       <c r="G154" t="n">
         <v>4.389140271493213</v>
@@ -7834,16 +7834,16 @@
         <v>0.02985173769794877</v>
       </c>
       <c r="J154" t="n">
-        <v>1.482603092783505</v>
+        <v>1.609603906673901</v>
       </c>
       <c r="K154" t="n">
-        <v>0.8584527220630372</v>
+        <v>0.8463276836158192</v>
       </c>
       <c r="L154" t="n">
         <v>0.2586206896551724</v>
       </c>
       <c r="M154" t="n">
-        <v>0.3255106475445459</v>
+        <v>0.3787291420866341</v>
       </c>
       <c r="N154" t="n">
         <v>0.41289592760181</v>
@@ -7852,25 +7852,25 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
+          <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.'})</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
           <t>frozenset({'SCOTTIE DOG HOT WATER BOTTLE'})</t>
         </is>
       </c>
-      <c r="B155" t="inlineStr">
-        <is>
-          <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.'})</t>
-        </is>
-      </c>
       <c r="C155" t="n">
+        <v>0.1005154639175258</v>
+      </c>
+      <c r="D155" t="n">
         <v>0.08762886597938144</v>
-      </c>
-      <c r="D155" t="n">
-        <v>0.1005154639175258</v>
       </c>
       <c r="E155" t="n">
         <v>0.03865979381443299</v>
       </c>
       <c r="F155" t="n">
-        <v>0.4411764705882353</v>
+        <v>0.3846153846153846</v>
       </c>
       <c r="G155" t="n">
         <v>4.389140271493213</v>
@@ -7882,16 +7882,16 @@
         <v>0.02985173769794877</v>
       </c>
       <c r="J155" t="n">
-        <v>1.609603906673901</v>
+        <v>1.482603092783505</v>
       </c>
       <c r="K155" t="n">
-        <v>0.8463276836158192</v>
+        <v>0.8584527220630372</v>
       </c>
       <c r="L155" t="n">
         <v>0.2586206896551724</v>
       </c>
       <c r="M155" t="n">
-        <v>0.3787291420866341</v>
+        <v>0.3255106475445459</v>
       </c>
       <c r="N155" t="n">
         <v>0.41289592760181</v>
@@ -8284,25 +8284,25 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER UNION JACK'})</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER OWL DESIGN'})</t>
         </is>
       </c>
-      <c r="B164" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER UNION JACK'})</t>
-        </is>
-      </c>
       <c r="C164" t="n">
+        <v>0.1134020618556701</v>
+      </c>
+      <c r="D164" t="n">
         <v>0.09793814432989691</v>
-      </c>
-      <c r="D164" t="n">
-        <v>0.1134020618556701</v>
       </c>
       <c r="E164" t="n">
         <v>0.04510309278350515</v>
       </c>
       <c r="F164" t="n">
-        <v>0.4605263157894737</v>
+        <v>0.3977272727272727</v>
       </c>
       <c r="G164" t="n">
         <v>4.061004784688995</v>
@@ -8314,16 +8314,16 @@
         <v>0.03399670528217664</v>
       </c>
       <c r="J164" t="n">
-        <v>1.643449836560221</v>
+        <v>1.497763081112624</v>
       </c>
       <c r="K164" t="n">
-        <v>0.8355918367346939</v>
+        <v>0.8501661129568105</v>
       </c>
       <c r="L164" t="n">
         <v>0.2713178294573643</v>
       </c>
       <c r="M164" t="n">
-        <v>0.3915238678090576</v>
+        <v>0.3323376623376623</v>
       </c>
       <c r="N164" t="n">
         <v>0.4291267942583732</v>
@@ -8332,25 +8332,25 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER OWL DESIGN'})</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER UNION JACK'})</t>
         </is>
       </c>
-      <c r="B165" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER OWL DESIGN'})</t>
-        </is>
-      </c>
       <c r="C165" t="n">
+        <v>0.09793814432989691</v>
+      </c>
+      <c r="D165" t="n">
         <v>0.1134020618556701</v>
-      </c>
-      <c r="D165" t="n">
-        <v>0.09793814432989691</v>
       </c>
       <c r="E165" t="n">
         <v>0.04510309278350515</v>
       </c>
       <c r="F165" t="n">
-        <v>0.3977272727272727</v>
+        <v>0.4605263157894737</v>
       </c>
       <c r="G165" t="n">
         <v>4.061004784688995</v>
@@ -8362,16 +8362,16 @@
         <v>0.03399670528217664</v>
       </c>
       <c r="J165" t="n">
-        <v>1.497763081112624</v>
+        <v>1.643449836560221</v>
       </c>
       <c r="K165" t="n">
-        <v>0.8501661129568105</v>
+        <v>0.8355918367346939</v>
       </c>
       <c r="L165" t="n">
         <v>0.2713178294573643</v>
       </c>
       <c r="M165" t="n">
-        <v>0.3323376623376623</v>
+        <v>0.3915238678090576</v>
       </c>
       <c r="N165" t="n">
         <v>0.4291267942583732</v>
@@ -8380,25 +8380,25 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
+          <t>frozenset({'SCOTTIE DOG HOT WATER BOTTLE'})</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN'})</t>
         </is>
       </c>
-      <c r="B166" t="inlineStr">
-        <is>
-          <t>frozenset({'SCOTTIE DOG HOT WATER BOTTLE'})</t>
-        </is>
-      </c>
       <c r="C166" t="n">
+        <v>0.08762886597938144</v>
+      </c>
+      <c r="D166" t="n">
         <v>0.09922680412371133</v>
-      </c>
-      <c r="D166" t="n">
-        <v>0.08762886597938144</v>
       </c>
       <c r="E166" t="n">
         <v>0.03479381443298969</v>
       </c>
       <c r="F166" t="n">
-        <v>0.3506493506493507</v>
+        <v>0.3970588235294118</v>
       </c>
       <c r="G166" t="n">
         <v>4.001527883880826</v>
@@ -8410,16 +8410,16 @@
         <v>0.02609868211287066</v>
       </c>
       <c r="J166" t="n">
-        <v>1.405051546391753</v>
+        <v>1.493965300477747</v>
       </c>
       <c r="K166" t="n">
-        <v>0.8327239972447411</v>
+        <v>0.8221385227034945</v>
       </c>
       <c r="L166" t="n">
         <v>0.2288135593220339</v>
       </c>
       <c r="M166" t="n">
-        <v>0.2882823391297967</v>
+        <v>0.3306404106707061</v>
       </c>
       <c r="N166" t="n">
         <v>0.3738540870893812</v>
@@ -8428,25 +8428,25 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN'})</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
           <t>frozenset({'SCOTTIE DOG HOT WATER BOTTLE'})</t>
         </is>
       </c>
-      <c r="B167" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN'})</t>
-        </is>
-      </c>
       <c r="C167" t="n">
+        <v>0.09922680412371133</v>
+      </c>
+      <c r="D167" t="n">
         <v>0.08762886597938144</v>
-      </c>
-      <c r="D167" t="n">
-        <v>0.09922680412371133</v>
       </c>
       <c r="E167" t="n">
         <v>0.03479381443298969</v>
       </c>
       <c r="F167" t="n">
-        <v>0.3970588235294118</v>
+        <v>0.3506493506493507</v>
       </c>
       <c r="G167" t="n">
         <v>4.001527883880826</v>
@@ -8458,16 +8458,16 @@
         <v>0.02609868211287066</v>
       </c>
       <c r="J167" t="n">
-        <v>1.493965300477747</v>
+        <v>1.405051546391753</v>
       </c>
       <c r="K167" t="n">
-        <v>0.8221385227034945</v>
+        <v>0.8327239972447411</v>
       </c>
       <c r="L167" t="n">
         <v>0.2288135593220339</v>
       </c>
       <c r="M167" t="n">
-        <v>0.3306404106707061</v>
+        <v>0.2882823391297967</v>
       </c>
       <c r="N167" t="n">
         <v>0.3738540870893812</v>
@@ -8764,25 +8764,25 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
+          <t>frozenset({'HOT WATER BOTTLE TEA AND SYMPATHY'})</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
           <t>frozenset({'SCOTTIE DOG HOT WATER BOTTLE'})</t>
         </is>
       </c>
-      <c r="B174" t="inlineStr">
-        <is>
-          <t>frozenset({'HOT WATER BOTTLE TEA AND SYMPATHY'})</t>
-        </is>
-      </c>
       <c r="C174" t="n">
+        <v>0.09278350515463918</v>
+      </c>
+      <c r="D174" t="n">
         <v>0.08762886597938144</v>
-      </c>
-      <c r="D174" t="n">
-        <v>0.09278350515463918</v>
       </c>
       <c r="E174" t="n">
         <v>0.03092783505154639</v>
       </c>
       <c r="F174" t="n">
-        <v>0.3529411764705883</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="G174" t="n">
         <v>3.803921568627451</v>
@@ -8794,16 +8794,16 @@
         <v>0.02279732171325327</v>
       </c>
       <c r="J174" t="n">
-        <v>1.402061855670103</v>
+        <v>1.368556701030928</v>
       </c>
       <c r="K174" t="n">
-        <v>0.8079096045197741</v>
+        <v>0.8125</v>
       </c>
       <c r="L174" t="n">
         <v>0.206896551724138</v>
       </c>
       <c r="M174" t="n">
-        <v>0.286764705882353</v>
+        <v>0.2693032015065913</v>
       </c>
       <c r="N174" t="n">
         <v>0.3431372549019608</v>
@@ -8812,25 +8812,25 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
+          <t>frozenset({'SCOTTIE DOG HOT WATER BOTTLE'})</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
           <t>frozenset({'HOT WATER BOTTLE TEA AND SYMPATHY'})</t>
         </is>
       </c>
-      <c r="B175" t="inlineStr">
-        <is>
-          <t>frozenset({'SCOTTIE DOG HOT WATER BOTTLE'})</t>
-        </is>
-      </c>
       <c r="C175" t="n">
+        <v>0.08762886597938144</v>
+      </c>
+      <c r="D175" t="n">
         <v>0.09278350515463918</v>
-      </c>
-      <c r="D175" t="n">
-        <v>0.08762886597938144</v>
       </c>
       <c r="E175" t="n">
         <v>0.03092783505154639</v>
       </c>
       <c r="F175" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.3529411764705883</v>
       </c>
       <c r="G175" t="n">
         <v>3.803921568627451</v>
@@ -8842,16 +8842,16 @@
         <v>0.02279732171325327</v>
       </c>
       <c r="J175" t="n">
-        <v>1.368556701030928</v>
+        <v>1.402061855670103</v>
       </c>
       <c r="K175" t="n">
-        <v>0.8125</v>
+        <v>0.8079096045197741</v>
       </c>
       <c r="L175" t="n">
         <v>0.206896551724138</v>
       </c>
       <c r="M175" t="n">
-        <v>0.2693032015065913</v>
+        <v>0.286764705882353</v>
       </c>
       <c r="N175" t="n">
         <v>0.3431372549019608</v>
@@ -8860,25 +8860,25 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
+          <t>frozenset({'WHITE SKULL HOT WATER BOTTLE '})</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER OWL DESIGN'})</t>
         </is>
       </c>
-      <c r="B176" t="inlineStr">
-        <is>
-          <t>frozenset({'WHITE SKULL HOT WATER BOTTLE '})</t>
-        </is>
-      </c>
       <c r="C176" t="n">
+        <v>0.08505154639175258</v>
+      </c>
+      <c r="D176" t="n">
         <v>0.09793814432989691</v>
-      </c>
-      <c r="D176" t="n">
-        <v>0.08505154639175258</v>
       </c>
       <c r="E176" t="n">
         <v>0.03092783505154639</v>
       </c>
       <c r="F176" t="n">
-        <v>0.3157894736842106</v>
+        <v>0.3636363636363636</v>
       </c>
       <c r="G176" t="n">
         <v>3.712918660287082</v>
@@ -8890,16 +8890,16 @@
         <v>0.02259804442555001</v>
       </c>
       <c r="J176" t="n">
-        <v>1.337232355273593</v>
+        <v>1.417525773195876</v>
       </c>
       <c r="K176" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.7985915492957746</v>
       </c>
       <c r="L176" t="n">
         <v>0.2033898305084746</v>
       </c>
       <c r="M176" t="n">
-        <v>0.252186805040771</v>
+        <v>0.2945454545454546</v>
       </c>
       <c r="N176" t="n">
         <v>0.3397129186602871</v>
@@ -8908,25 +8908,25 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER OWL DESIGN'})</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
           <t>frozenset({'WHITE SKULL HOT WATER BOTTLE '})</t>
         </is>
       </c>
-      <c r="B177" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER OWL DESIGN'})</t>
-        </is>
-      </c>
       <c r="C177" t="n">
+        <v>0.09793814432989691</v>
+      </c>
+      <c r="D177" t="n">
         <v>0.08505154639175258</v>
-      </c>
-      <c r="D177" t="n">
-        <v>0.09793814432989691</v>
       </c>
       <c r="E177" t="n">
         <v>0.03092783505154639</v>
       </c>
       <c r="F177" t="n">
-        <v>0.3636363636363636</v>
+        <v>0.3157894736842106</v>
       </c>
       <c r="G177" t="n">
         <v>3.712918660287082</v>
@@ -8938,16 +8938,16 @@
         <v>0.02259804442555001</v>
       </c>
       <c r="J177" t="n">
-        <v>1.417525773195876</v>
+        <v>1.337232355273593</v>
       </c>
       <c r="K177" t="n">
-        <v>0.7985915492957746</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="L177" t="n">
         <v>0.2033898305084746</v>
       </c>
       <c r="M177" t="n">
-        <v>0.2945454545454546</v>
+        <v>0.252186805040771</v>
       </c>
       <c r="N177" t="n">
         <v>0.3397129186602871</v>
@@ -9148,25 +9148,25 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
+          <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.'})</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
           <t>frozenset({'WHITE HANGING HEART T-LIGHT HOLDER'})</t>
         </is>
       </c>
-      <c r="B182" t="inlineStr">
-        <is>
-          <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.'})</t>
-        </is>
-      </c>
       <c r="C182" t="n">
+        <v>0.1005154639175258</v>
+      </c>
+      <c r="D182" t="n">
         <v>0.1378865979381443</v>
-      </c>
-      <c r="D182" t="n">
-        <v>0.1005154639175258</v>
       </c>
       <c r="E182" t="n">
         <v>0.04896907216494845</v>
       </c>
       <c r="F182" t="n">
-        <v>0.3551401869158878</v>
+        <v>0.4871794871794872</v>
       </c>
       <c r="G182" t="n">
         <v>3.53318955188114</v>
@@ -9178,16 +9178,16 @@
         <v>0.03510933680518652</v>
       </c>
       <c r="J182" t="n">
-        <v>1.394852831316301</v>
+        <v>1.681121134020619</v>
       </c>
       <c r="K182" t="n">
-        <v>0.8316418849815119</v>
+        <v>0.7970894284421655</v>
       </c>
       <c r="L182" t="n">
         <v>0.2585034013605442</v>
       </c>
       <c r="M182" t="n">
-        <v>0.2830784886056288</v>
+        <v>0.4051588670422751</v>
       </c>
       <c r="N182" t="n">
         <v>0.4211598370476875</v>
@@ -9196,25 +9196,25 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
+          <t>frozenset({'WHITE HANGING HEART T-LIGHT HOLDER'})</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
           <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.'})</t>
         </is>
       </c>
-      <c r="B183" t="inlineStr">
-        <is>
-          <t>frozenset({'WHITE HANGING HEART T-LIGHT HOLDER'})</t>
-        </is>
-      </c>
       <c r="C183" t="n">
+        <v>0.1378865979381443</v>
+      </c>
+      <c r="D183" t="n">
         <v>0.1005154639175258</v>
-      </c>
-      <c r="D183" t="n">
-        <v>0.1378865979381443</v>
       </c>
       <c r="E183" t="n">
         <v>0.04896907216494845</v>
       </c>
       <c r="F183" t="n">
-        <v>0.4871794871794872</v>
+        <v>0.3551401869158878</v>
       </c>
       <c r="G183" t="n">
         <v>3.53318955188114</v>
@@ -9226,16 +9226,16 @@
         <v>0.03510933680518652</v>
       </c>
       <c r="J183" t="n">
-        <v>1.681121134020619</v>
+        <v>1.394852831316301</v>
       </c>
       <c r="K183" t="n">
-        <v>0.7970894284421655</v>
+        <v>0.8316418849815119</v>
       </c>
       <c r="L183" t="n">
         <v>0.2585034013605442</v>
       </c>
       <c r="M183" t="n">
-        <v>0.4051588670422751</v>
+        <v>0.2830784886056288</v>
       </c>
       <c r="N183" t="n">
         <v>0.4211598370476875</v>
@@ -9340,25 +9340,25 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER BIRD DESIGN'})</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER UNION JACK'})</t>
         </is>
       </c>
-      <c r="B186" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER BIRD DESIGN'})</t>
-        </is>
-      </c>
       <c r="C186" t="n">
+        <v>0.1275773195876289</v>
+      </c>
+      <c r="D186" t="n">
         <v>0.1134020618556701</v>
-      </c>
-      <c r="D186" t="n">
-        <v>0.1275773195876289</v>
       </c>
       <c r="E186" t="n">
         <v>0.04896907216494845</v>
       </c>
       <c r="F186" t="n">
-        <v>0.4318181818181818</v>
+        <v>0.3838383838383839</v>
       </c>
       <c r="G186" t="n">
         <v>3.38475665748393</v>
@@ -9370,16 +9370,16 @@
         <v>0.03450154107769157</v>
       </c>
       <c r="J186" t="n">
-        <v>1.535463917525773</v>
+        <v>1.438904850430962</v>
       </c>
       <c r="K186" t="n">
-        <v>0.7946756425948592</v>
+        <v>0.8075876545129441</v>
       </c>
       <c r="L186" t="n">
         <v>0.2550335570469799</v>
       </c>
       <c r="M186" t="n">
-        <v>0.3487310326305895</v>
+        <v>0.30502701432934</v>
       </c>
       <c r="N186" t="n">
         <v>0.4078282828282829</v>
@@ -9388,25 +9388,25 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER UNION JACK'})</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER BIRD DESIGN'})</t>
         </is>
       </c>
-      <c r="B187" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER UNION JACK'})</t>
-        </is>
-      </c>
       <c r="C187" t="n">
+        <v>0.1134020618556701</v>
+      </c>
+      <c r="D187" t="n">
         <v>0.1275773195876289</v>
-      </c>
-      <c r="D187" t="n">
-        <v>0.1134020618556701</v>
       </c>
       <c r="E187" t="n">
         <v>0.04896907216494845</v>
       </c>
       <c r="F187" t="n">
-        <v>0.3838383838383839</v>
+        <v>0.4318181818181818</v>
       </c>
       <c r="G187" t="n">
         <v>3.38475665748393</v>
@@ -9418,16 +9418,16 @@
         <v>0.03450154107769157</v>
       </c>
       <c r="J187" t="n">
-        <v>1.438904850430962</v>
+        <v>1.535463917525773</v>
       </c>
       <c r="K187" t="n">
-        <v>0.8075876545129441</v>
+        <v>0.7946756425948592</v>
       </c>
       <c r="L187" t="n">
         <v>0.2550335570469799</v>
       </c>
       <c r="M187" t="n">
-        <v>0.30502701432934</v>
+        <v>0.3487310326305895</v>
       </c>
       <c r="N187" t="n">
         <v>0.4078282828282829</v>
@@ -9916,25 +9916,25 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER BIRD DESIGN'})</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
           <t>frozenset({'HOT WATER BOTTLE TEA AND SYMPATHY'})</t>
         </is>
       </c>
-      <c r="B198" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER BIRD DESIGN'})</t>
-        </is>
-      </c>
       <c r="C198" t="n">
+        <v>0.1275773195876289</v>
+      </c>
+      <c r="D198" t="n">
         <v>0.09278350515463918</v>
-      </c>
-      <c r="D198" t="n">
-        <v>0.1275773195876289</v>
       </c>
       <c r="E198" t="n">
         <v>0.03737113402061856</v>
       </c>
       <c r="F198" t="n">
-        <v>0.4027777777777777</v>
+        <v>0.2929292929292929</v>
       </c>
       <c r="G198" t="n">
         <v>3.15712682379349</v>
@@ -9946,16 +9946,16 @@
         <v>0.02553406313104474</v>
       </c>
       <c r="J198" t="n">
-        <v>1.460800767202109</v>
+        <v>1.283063328424153</v>
       </c>
       <c r="K198" t="n">
-        <v>0.7531347962382445</v>
+        <v>0.7831711913614833</v>
       </c>
       <c r="L198" t="n">
         <v>0.2042253521126761</v>
       </c>
       <c r="M198" t="n">
-        <v>0.3154439520761529</v>
+        <v>0.2206152433425161</v>
       </c>
       <c r="N198" t="n">
         <v>0.3478535353535354</v>
@@ -9964,25 +9964,25 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
+          <t>frozenset({'HOT WATER BOTTLE TEA AND SYMPATHY'})</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER BIRD DESIGN'})</t>
         </is>
       </c>
-      <c r="B199" t="inlineStr">
-        <is>
-          <t>frozenset({'HOT WATER BOTTLE TEA AND SYMPATHY'})</t>
-        </is>
-      </c>
       <c r="C199" t="n">
+        <v>0.09278350515463918</v>
+      </c>
+      <c r="D199" t="n">
         <v>0.1275773195876289</v>
-      </c>
-      <c r="D199" t="n">
-        <v>0.09278350515463918</v>
       </c>
       <c r="E199" t="n">
         <v>0.03737113402061856</v>
       </c>
       <c r="F199" t="n">
-        <v>0.2929292929292929</v>
+        <v>0.4027777777777777</v>
       </c>
       <c r="G199" t="n">
         <v>3.15712682379349</v>
@@ -9994,16 +9994,16 @@
         <v>0.02553406313104474</v>
       </c>
       <c r="J199" t="n">
-        <v>1.283063328424153</v>
+        <v>1.460800767202109</v>
       </c>
       <c r="K199" t="n">
-        <v>0.7831711913614833</v>
+        <v>0.7531347962382445</v>
       </c>
       <c r="L199" t="n">
         <v>0.2042253521126761</v>
       </c>
       <c r="M199" t="n">
-        <v>0.2206152433425161</v>
+        <v>0.3154439520761529</v>
       </c>
       <c r="N199" t="n">
         <v>0.3478535353535354</v>
@@ -10300,25 +10300,25 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
+          <t>frozenset({"PAPER CHAIN KIT 50'S CHRISTMAS "})</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER BIRD DESIGN'})</t>
         </is>
       </c>
-      <c r="B206" t="inlineStr">
-        <is>
-          <t>frozenset({"PAPER CHAIN KIT 50'S CHRISTMAS "})</t>
-        </is>
-      </c>
       <c r="C206" t="n">
+        <v>0.1134020618556701</v>
+      </c>
+      <c r="D206" t="n">
         <v>0.1275773195876289</v>
-      </c>
-      <c r="D206" t="n">
-        <v>0.1134020618556701</v>
       </c>
       <c r="E206" t="n">
         <v>0.03994845360824742</v>
       </c>
       <c r="F206" t="n">
-        <v>0.3131313131313131</v>
+        <v>0.3522727272727272</v>
       </c>
       <c r="G206" t="n">
         <v>2.761248852157943</v>
@@ -10330,16 +10330,16 @@
         <v>0.02548092252099054</v>
       </c>
       <c r="J206" t="n">
-        <v>1.290782292298363</v>
+        <v>1.346898173268222</v>
       </c>
       <c r="K206" t="n">
-        <v>0.7311192643064753</v>
+        <v>0.7194298574643662</v>
       </c>
       <c r="L206" t="n">
         <v>0.1987179487179487</v>
       </c>
       <c r="M206" t="n">
-        <v>0.2252760159736904</v>
+        <v>0.257553377198872</v>
       </c>
       <c r="N206" t="n">
         <v>0.3327020202020202</v>
@@ -10348,25 +10348,25 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER BIRD DESIGN'})</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
           <t>frozenset({"PAPER CHAIN KIT 50'S CHRISTMAS "})</t>
         </is>
       </c>
-      <c r="B207" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER BIRD DESIGN'})</t>
-        </is>
-      </c>
       <c r="C207" t="n">
+        <v>0.1275773195876289</v>
+      </c>
+      <c r="D207" t="n">
         <v>0.1134020618556701</v>
-      </c>
-      <c r="D207" t="n">
-        <v>0.1275773195876289</v>
       </c>
       <c r="E207" t="n">
         <v>0.03994845360824742</v>
       </c>
       <c r="F207" t="n">
-        <v>0.3522727272727272</v>
+        <v>0.3131313131313131</v>
       </c>
       <c r="G207" t="n">
         <v>2.761248852157943</v>
@@ -10378,16 +10378,16 @@
         <v>0.02548092252099054</v>
       </c>
       <c r="J207" t="n">
-        <v>1.346898173268222</v>
+        <v>1.290782292298363</v>
       </c>
       <c r="K207" t="n">
-        <v>0.7194298574643662</v>
+        <v>0.7311192643064753</v>
       </c>
       <c r="L207" t="n">
         <v>0.1987179487179487</v>
       </c>
       <c r="M207" t="n">
-        <v>0.257553377198872</v>
+        <v>0.2252760159736904</v>
       </c>
       <c r="N207" t="n">
         <v>0.3327020202020202</v>
@@ -10492,25 +10492,25 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER BIRD DESIGN'})</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
           <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.'})</t>
         </is>
       </c>
-      <c r="B210" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER BIRD DESIGN'})</t>
-        </is>
-      </c>
       <c r="C210" t="n">
+        <v>0.1275773195876289</v>
+      </c>
+      <c r="D210" t="n">
         <v>0.1005154639175258</v>
-      </c>
-      <c r="D210" t="n">
-        <v>0.1275773195876289</v>
       </c>
       <c r="E210" t="n">
         <v>0.03092783505154639</v>
       </c>
       <c r="F210" t="n">
-        <v>0.3076923076923077</v>
+        <v>0.2424242424242425</v>
       </c>
       <c r="G210" t="n">
         <v>2.411810411810412</v>
@@ -10522,16 +10522,16 @@
         <v>0.01810434158784143</v>
       </c>
       <c r="J210" t="n">
-        <v>1.26016609392898</v>
+        <v>1.187319587628866</v>
       </c>
       <c r="K210" t="n">
-        <v>0.6507879656160459</v>
+        <v>0.6709748892171346</v>
       </c>
       <c r="L210" t="n">
         <v>0.1568627450980392</v>
       </c>
       <c r="M210" t="n">
-        <v>0.2064538120668106</v>
+        <v>0.1577667795432839</v>
       </c>
       <c r="N210" t="n">
         <v>0.2750582750582751</v>
@@ -10540,25 +10540,25 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
+          <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.'})</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER BIRD DESIGN'})</t>
         </is>
       </c>
-      <c r="B211" t="inlineStr">
-        <is>
-          <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.'})</t>
-        </is>
-      </c>
       <c r="C211" t="n">
+        <v>0.1005154639175258</v>
+      </c>
+      <c r="D211" t="n">
         <v>0.1275773195876289</v>
-      </c>
-      <c r="D211" t="n">
-        <v>0.1005154639175258</v>
       </c>
       <c r="E211" t="n">
         <v>0.03092783505154639</v>
       </c>
       <c r="F211" t="n">
-        <v>0.2424242424242425</v>
+        <v>0.3076923076923077</v>
       </c>
       <c r="G211" t="n">
         <v>2.411810411810412</v>
@@ -10570,16 +10570,16 @@
         <v>0.01810434158784143</v>
       </c>
       <c r="J211" t="n">
-        <v>1.187319587628866</v>
+        <v>1.26016609392898</v>
       </c>
       <c r="K211" t="n">
-        <v>0.6709748892171346</v>
+        <v>0.6507879656160459</v>
       </c>
       <c r="L211" t="n">
         <v>0.1568627450980392</v>
       </c>
       <c r="M211" t="n">
-        <v>0.1577667795432839</v>
+        <v>0.2064538120668106</v>
       </c>
       <c r="N211" t="n">
         <v>0.2750582750582751</v>

</xml_diff>

<commit_message>
Add visulation and save graph and some changes
</commit_message>
<xml_diff>
--- a/output/association_rules.xlsx
+++ b/output/association_rules.xlsx
@@ -508,25 +508,25 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>frozenset({"POPPY'S PLAYHOUSE BEDROOM "})</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
           <t>frozenset({"POPPY'S PLAYHOUSE KITCHEN"})</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>frozenset({"POPPY'S PLAYHOUSE BEDROOM "})</t>
-        </is>
-      </c>
       <c r="C2" t="n">
+        <v>0.04510309278350515</v>
+      </c>
+      <c r="D2" t="n">
         <v>0.04381443298969072</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.04510309278350515</v>
       </c>
       <c r="E2" t="n">
         <v>0.03608247422680412</v>
       </c>
       <c r="F2" t="n">
-        <v>0.8235294117647058</v>
+        <v>0.7999999999999999</v>
       </c>
       <c r="G2" t="n">
         <v>18.25882352941176</v>
@@ -538,16 +538,16 @@
         <v>0.03410630779041343</v>
       </c>
       <c r="J2" t="n">
-        <v>5.411082474226803</v>
+        <v>4.780927835051545</v>
       </c>
       <c r="K2" t="n">
-        <v>0.9885444743935309</v>
+        <v>0.9898785425101214</v>
       </c>
       <c r="L2" t="n">
         <v>0.6829268292682927</v>
       </c>
       <c r="M2" t="n">
-        <v>0.8151940938318647</v>
+        <v>0.7908355795148247</v>
       </c>
       <c r="N2" t="n">
         <v>0.8117647058823529</v>
@@ -556,25 +556,25 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>frozenset({"POPPY'S PLAYHOUSE KITCHEN"})</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
           <t>frozenset({"POPPY'S PLAYHOUSE BEDROOM "})</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>frozenset({"POPPY'S PLAYHOUSE KITCHEN"})</t>
-        </is>
-      </c>
       <c r="C3" t="n">
+        <v>0.04381443298969072</v>
+      </c>
+      <c r="D3" t="n">
         <v>0.04510309278350515</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.04381443298969072</v>
       </c>
       <c r="E3" t="n">
         <v>0.03608247422680412</v>
       </c>
       <c r="F3" t="n">
-        <v>0.7999999999999999</v>
+        <v>0.8235294117647058</v>
       </c>
       <c r="G3" t="n">
         <v>18.25882352941176</v>
@@ -586,16 +586,16 @@
         <v>0.03410630779041343</v>
       </c>
       <c r="J3" t="n">
-        <v>4.780927835051545</v>
+        <v>5.411082474226803</v>
       </c>
       <c r="K3" t="n">
-        <v>0.9898785425101214</v>
+        <v>0.9885444743935309</v>
       </c>
       <c r="L3" t="n">
         <v>0.6829268292682927</v>
       </c>
       <c r="M3" t="n">
-        <v>0.7908355795148247</v>
+        <v>0.8151940938318647</v>
       </c>
       <c r="N3" t="n">
         <v>0.8117647058823529</v>
@@ -604,25 +604,25 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>frozenset({'ROSES REGENCY TEACUP AND SAUCER '})</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
           <t>frozenset({'GREEN REGENCY TEACUP AND SAUCER'})</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>frozenset({'ROSES REGENCY TEACUP AND SAUCER '})</t>
-        </is>
-      </c>
       <c r="C4" t="n">
+        <v>0.04252577319587629</v>
+      </c>
+      <c r="D4" t="n">
         <v>0.04510309278350515</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.04252577319587629</v>
       </c>
       <c r="E4" t="n">
         <v>0.03221649484536082</v>
       </c>
       <c r="F4" t="n">
-        <v>0.7142857142857142</v>
+        <v>0.7575757575757575</v>
       </c>
       <c r="G4" t="n">
         <v>16.7965367965368</v>
@@ -634,16 +634,16 @@
         <v>0.03029845095121692</v>
       </c>
       <c r="J4" t="n">
-        <v>3.351159793814432</v>
+        <v>3.93894974226804</v>
       </c>
       <c r="K4" t="n">
-        <v>0.9848852901484479</v>
+        <v>0.9822341857335126</v>
       </c>
       <c r="L4" t="n">
         <v>0.5813953488372092</v>
       </c>
       <c r="M4" t="n">
-        <v>0.7015958469525091</v>
+        <v>0.7461252198094303</v>
       </c>
       <c r="N4" t="n">
         <v>0.7359307359307359</v>
@@ -652,25 +652,25 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>frozenset({'GREEN REGENCY TEACUP AND SAUCER'})</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
           <t>frozenset({'ROSES REGENCY TEACUP AND SAUCER '})</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>frozenset({'GREEN REGENCY TEACUP AND SAUCER'})</t>
-        </is>
-      </c>
       <c r="C5" t="n">
+        <v>0.04510309278350515</v>
+      </c>
+      <c r="D5" t="n">
         <v>0.04252577319587629</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.04510309278350515</v>
       </c>
       <c r="E5" t="n">
         <v>0.03221649484536082</v>
       </c>
       <c r="F5" t="n">
-        <v>0.7575757575757575</v>
+        <v>0.7142857142857142</v>
       </c>
       <c r="G5" t="n">
         <v>16.7965367965368</v>
@@ -682,16 +682,16 @@
         <v>0.03029845095121692</v>
       </c>
       <c r="J5" t="n">
-        <v>3.93894974226804</v>
+        <v>3.351159793814432</v>
       </c>
       <c r="K5" t="n">
-        <v>0.9822341857335126</v>
+        <v>0.9848852901484479</v>
       </c>
       <c r="L5" t="n">
         <v>0.5813953488372092</v>
       </c>
       <c r="M5" t="n">
-        <v>0.7461252198094303</v>
+        <v>0.7015958469525091</v>
       </c>
       <c r="N5" t="n">
         <v>0.7359307359307359</v>
@@ -988,25 +988,25 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
+          <t>frozenset({'SMALL POPCORN HOLDER'})</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
           <t>frozenset({'LARGE POPCORN HOLDER '})</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>frozenset({'SMALL POPCORN HOLDER'})</t>
-        </is>
-      </c>
       <c r="C12" t="n">
+        <v>0.06829896907216494</v>
+      </c>
+      <c r="D12" t="n">
         <v>0.04123711340206185</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0.06829896907216494</v>
       </c>
       <c r="E12" t="n">
         <v>0.03608247422680412</v>
       </c>
       <c r="F12" t="n">
-        <v>0.8749999999999999</v>
+        <v>0.5283018867924528</v>
       </c>
       <c r="G12" t="n">
         <v>12.81132075471698</v>
@@ -1018,16 +1018,16 @@
         <v>0.03326602189393134</v>
       </c>
       <c r="J12" t="n">
-        <v>7.453608247422674</v>
+        <v>2.032577319587629</v>
       </c>
       <c r="K12" t="n">
-        <v>0.9615975422427036</v>
+        <v>0.9895277613119936</v>
       </c>
       <c r="L12" t="n">
         <v>0.4912280701754385</v>
       </c>
       <c r="M12" t="n">
-        <v>0.8658367911479944</v>
+        <v>0.5080137959018056</v>
       </c>
       <c r="N12" t="n">
         <v>0.7016509433962264</v>
@@ -1036,25 +1036,25 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>frozenset({'LARGE POPCORN HOLDER '})</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
           <t>frozenset({'SMALL POPCORN HOLDER'})</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>frozenset({'LARGE POPCORN HOLDER '})</t>
-        </is>
-      </c>
       <c r="C13" t="n">
+        <v>0.04123711340206185</v>
+      </c>
+      <c r="D13" t="n">
         <v>0.06829896907216494</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0.04123711340206185</v>
       </c>
       <c r="E13" t="n">
         <v>0.03608247422680412</v>
       </c>
       <c r="F13" t="n">
-        <v>0.5283018867924528</v>
+        <v>0.8749999999999999</v>
       </c>
       <c r="G13" t="n">
         <v>12.81132075471698</v>
@@ -1066,16 +1066,16 @@
         <v>0.03326602189393134</v>
       </c>
       <c r="J13" t="n">
-        <v>2.032577319587629</v>
+        <v>7.453608247422674</v>
       </c>
       <c r="K13" t="n">
-        <v>0.9895277613119936</v>
+        <v>0.9615975422427036</v>
       </c>
       <c r="L13" t="n">
         <v>0.4912280701754385</v>
       </c>
       <c r="M13" t="n">
-        <v>0.5080137959018056</v>
+        <v>0.8658367911479944</v>
       </c>
       <c r="N13" t="n">
         <v>0.7016509433962264</v>
@@ -1180,25 +1180,25 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>frozenset({'PACK OF 72 RETROSPOT CAKE CASES'})</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
           <t>frozenset({'PACK OF 60 PINK PAISLEY CAKE CASES'})</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>frozenset({'PACK OF 72 RETROSPOT CAKE CASES'})</t>
-        </is>
-      </c>
       <c r="C16" t="n">
+        <v>0.06572164948453608</v>
+      </c>
+      <c r="D16" t="n">
         <v>0.03737113402061856</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0.06572164948453608</v>
       </c>
       <c r="E16" t="n">
         <v>0.03092783505154639</v>
       </c>
       <c r="F16" t="n">
-        <v>0.8275862068965518</v>
+        <v>0.4705882352941176</v>
       </c>
       <c r="G16" t="n">
         <v>12.59229208924949</v>
@@ -1210,16 +1210,16 @@
         <v>0.02847174248060368</v>
       </c>
       <c r="J16" t="n">
-        <v>5.418814432989694</v>
+        <v>1.818298969072165</v>
       </c>
       <c r="K16" t="n">
-        <v>0.9563253012048193</v>
+        <v>0.9853448275862069</v>
       </c>
       <c r="L16" t="n">
         <v>0.4285714285714286</v>
       </c>
       <c r="M16" t="n">
-        <v>0.8154577883472058</v>
+        <v>0.4500354358610914</v>
       </c>
       <c r="N16" t="n">
         <v>0.6490872210953347</v>
@@ -1228,25 +1228,25 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
+          <t>frozenset({'PACK OF 60 PINK PAISLEY CAKE CASES'})</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
           <t>frozenset({'PACK OF 72 RETROSPOT CAKE CASES'})</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>frozenset({'PACK OF 60 PINK PAISLEY CAKE CASES'})</t>
-        </is>
-      </c>
       <c r="C17" t="n">
+        <v>0.03737113402061856</v>
+      </c>
+      <c r="D17" t="n">
         <v>0.06572164948453608</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0.03737113402061856</v>
       </c>
       <c r="E17" t="n">
         <v>0.03092783505154639</v>
       </c>
       <c r="F17" t="n">
-        <v>0.4705882352941176</v>
+        <v>0.8275862068965518</v>
       </c>
       <c r="G17" t="n">
         <v>12.59229208924949</v>
@@ -1258,16 +1258,16 @@
         <v>0.02847174248060368</v>
       </c>
       <c r="J17" t="n">
-        <v>1.818298969072165</v>
+        <v>5.418814432989694</v>
       </c>
       <c r="K17" t="n">
-        <v>0.9853448275862069</v>
+        <v>0.9563253012048193</v>
       </c>
       <c r="L17" t="n">
         <v>0.4285714285714286</v>
       </c>
       <c r="M17" t="n">
-        <v>0.4500354358610914</v>
+        <v>0.8154577883472058</v>
       </c>
       <c r="N17" t="n">
         <v>0.6490872210953347</v>
@@ -1564,25 +1564,25 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
+          <t>frozenset({'60 TEATIME FAIRY CAKE CASES'})</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
           <t>frozenset({'PACK OF 72 RETROSPOT CAKE CASES'})</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>frozenset({'60 TEATIME FAIRY CAKE CASES'})</t>
-        </is>
-      </c>
       <c r="C24" t="n">
+        <v>0.04381443298969072</v>
+      </c>
+      <c r="D24" t="n">
         <v>0.06572164948453608</v>
-      </c>
-      <c r="D24" t="n">
-        <v>0.04381443298969072</v>
       </c>
       <c r="E24" t="n">
         <v>0.03221649484536082</v>
       </c>
       <c r="F24" t="n">
-        <v>0.4901960784313725</v>
+        <v>0.7352941176470588</v>
       </c>
       <c r="G24" t="n">
         <v>11.18800461361015</v>
@@ -1594,16 +1594,16 @@
         <v>0.02933693803804868</v>
       </c>
       <c r="J24" t="n">
-        <v>1.875594766058683</v>
+        <v>3.529495990836196</v>
       </c>
       <c r="K24" t="n">
-        <v>0.9746758620689656</v>
+        <v>0.952345013477089</v>
       </c>
       <c r="L24" t="n">
         <v>0.4166666666666666</v>
       </c>
       <c r="M24" t="n">
-        <v>0.4668357909201415</v>
+        <v>0.7166734279918864</v>
       </c>
       <c r="N24" t="n">
         <v>0.6127450980392156</v>
@@ -1612,25 +1612,25 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
+          <t>frozenset({'PACK OF 72 RETROSPOT CAKE CASES'})</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
           <t>frozenset({'60 TEATIME FAIRY CAKE CASES'})</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>frozenset({'PACK OF 72 RETROSPOT CAKE CASES'})</t>
-        </is>
-      </c>
       <c r="C25" t="n">
+        <v>0.06572164948453608</v>
+      </c>
+      <c r="D25" t="n">
         <v>0.04381443298969072</v>
-      </c>
-      <c r="D25" t="n">
-        <v>0.06572164948453608</v>
       </c>
       <c r="E25" t="n">
         <v>0.03221649484536082</v>
       </c>
       <c r="F25" t="n">
-        <v>0.7352941176470588</v>
+        <v>0.4901960784313725</v>
       </c>
       <c r="G25" t="n">
         <v>11.18800461361015</v>
@@ -1642,16 +1642,16 @@
         <v>0.02933693803804868</v>
       </c>
       <c r="J25" t="n">
-        <v>3.529495990836196</v>
+        <v>1.875594766058683</v>
       </c>
       <c r="K25" t="n">
-        <v>0.952345013477089</v>
+        <v>0.9746758620689656</v>
       </c>
       <c r="L25" t="n">
         <v>0.4166666666666666</v>
       </c>
       <c r="M25" t="n">
-        <v>0.7166734279918864</v>
+        <v>0.4668357909201415</v>
       </c>
       <c r="N25" t="n">
         <v>0.6127450980392156</v>
@@ -1665,7 +1665,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.', 'WHITE HANGING HEART T-LIGHT HOLDER'})</t>
+          <t>frozenset({'WHITE HANGING HEART T-LIGHT HOLDER', 'RED WOOLLY HOTTIE WHITE HEART.'})</t>
         </is>
       </c>
       <c r="C26" t="n">
@@ -1708,7 +1708,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.', 'WHITE HANGING HEART T-LIGHT HOLDER'})</t>
+          <t>frozenset({'WHITE HANGING HEART T-LIGHT HOLDER', 'RED WOOLLY HOTTIE WHITE HEART.'})</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1756,25 +1756,25 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
+          <t>frozenset({'60 CAKE CASES VINTAGE CHRISTMAS'})</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
           <t>frozenset({'SET OF 20 VINTAGE CHRISTMAS NAPKINS'})</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>frozenset({'60 CAKE CASES VINTAGE CHRISTMAS'})</t>
-        </is>
-      </c>
       <c r="C28" t="n">
+        <v>0.05798969072164949</v>
+      </c>
+      <c r="D28" t="n">
         <v>0.06056701030927835</v>
-      </c>
-      <c r="D28" t="n">
-        <v>0.05798969072164949</v>
       </c>
       <c r="E28" t="n">
         <v>0.03350515463917526</v>
       </c>
       <c r="F28" t="n">
-        <v>0.5531914893617021</v>
+        <v>0.5777777777777777</v>
       </c>
       <c r="G28" t="n">
         <v>9.539479905437352</v>
@@ -1786,16 +1786,16 @@
         <v>0.02999289244340525</v>
       </c>
       <c r="J28" t="n">
-        <v>2.108308787432499</v>
+        <v>2.22497287032013</v>
       </c>
       <c r="K28" t="n">
-        <v>0.9528859343674158</v>
+        <v>0.950278859307587</v>
       </c>
       <c r="L28" t="n">
         <v>0.3939393939393939</v>
       </c>
       <c r="M28" t="n">
-        <v>0.5256861774893035</v>
+        <v>0.5505563176345069</v>
       </c>
       <c r="N28" t="n">
         <v>0.5654846335697399</v>
@@ -1804,25 +1804,25 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
+          <t>frozenset({'SET OF 20 VINTAGE CHRISTMAS NAPKINS'})</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
           <t>frozenset({'60 CAKE CASES VINTAGE CHRISTMAS'})</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>frozenset({'SET OF 20 VINTAGE CHRISTMAS NAPKINS'})</t>
-        </is>
-      </c>
       <c r="C29" t="n">
+        <v>0.06056701030927835</v>
+      </c>
+      <c r="D29" t="n">
         <v>0.05798969072164949</v>
-      </c>
-      <c r="D29" t="n">
-        <v>0.06056701030927835</v>
       </c>
       <c r="E29" t="n">
         <v>0.03350515463917526</v>
       </c>
       <c r="F29" t="n">
-        <v>0.5777777777777777</v>
+        <v>0.5531914893617021</v>
       </c>
       <c r="G29" t="n">
         <v>9.539479905437352</v>
@@ -1834,16 +1834,16 @@
         <v>0.02999289244340525</v>
       </c>
       <c r="J29" t="n">
-        <v>2.22497287032013</v>
+        <v>2.108308787432499</v>
       </c>
       <c r="K29" t="n">
-        <v>0.950278859307587</v>
+        <v>0.9528859343674158</v>
       </c>
       <c r="L29" t="n">
         <v>0.3939393939393939</v>
       </c>
       <c r="M29" t="n">
-        <v>0.5505563176345069</v>
+        <v>0.5256861774893035</v>
       </c>
       <c r="N29" t="n">
         <v>0.5654846335697399</v>
@@ -1948,25 +1948,25 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
+          <t>frozenset({'WHITE HANGING HEART T-LIGHT HOLDER', 'KNITTED UNION FLAG HOT WATER BOTTLE'})</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
           <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.'})</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>frozenset({'WHITE HANGING HEART T-LIGHT HOLDER', 'KNITTED UNION FLAG HOT WATER BOTTLE'})</t>
-        </is>
-      </c>
       <c r="C32" t="n">
+        <v>0.04639175257731959</v>
+      </c>
+      <c r="D32" t="n">
         <v>0.1005154639175258</v>
-      </c>
-      <c r="D32" t="n">
-        <v>0.04639175257731959</v>
       </c>
       <c r="E32" t="n">
         <v>0.03865979381443299</v>
       </c>
       <c r="F32" t="n">
-        <v>0.3846153846153846</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="G32" t="n">
         <v>8.290598290598291</v>
@@ -1978,16 +1978,16 @@
         <v>0.03399670528217664</v>
       </c>
       <c r="J32" t="n">
-        <v>1.549613402061855</v>
+        <v>5.396907216494847</v>
       </c>
       <c r="K32" t="n">
-        <v>0.9776504297994268</v>
+        <v>0.9221621621621622</v>
       </c>
       <c r="L32" t="n">
         <v>0.3571428571428572</v>
       </c>
       <c r="M32" t="n">
-        <v>0.3546777546777547</v>
+        <v>0.8147086914995225</v>
       </c>
       <c r="N32" t="n">
         <v>0.608974358974359</v>
@@ -1996,25 +1996,25 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
+          <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.'})</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
           <t>frozenset({'WHITE HANGING HEART T-LIGHT HOLDER', 'KNITTED UNION FLAG HOT WATER BOTTLE'})</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.'})</t>
-        </is>
-      </c>
       <c r="C33" t="n">
+        <v>0.1005154639175258</v>
+      </c>
+      <c r="D33" t="n">
         <v>0.04639175257731959</v>
-      </c>
-      <c r="D33" t="n">
-        <v>0.1005154639175258</v>
       </c>
       <c r="E33" t="n">
         <v>0.03865979381443299</v>
       </c>
       <c r="F33" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.3846153846153846</v>
       </c>
       <c r="G33" t="n">
         <v>8.290598290598291</v>
@@ -2026,16 +2026,16 @@
         <v>0.03399670528217664</v>
       </c>
       <c r="J33" t="n">
-        <v>5.396907216494847</v>
+        <v>1.549613402061855</v>
       </c>
       <c r="K33" t="n">
-        <v>0.9221621621621622</v>
+        <v>0.9776504297994268</v>
       </c>
       <c r="L33" t="n">
         <v>0.3571428571428572</v>
       </c>
       <c r="M33" t="n">
-        <v>0.8147086914995225</v>
+        <v>0.3546777546777547</v>
       </c>
       <c r="N33" t="n">
         <v>0.608974358974359</v>
@@ -2044,25 +2044,25 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER RED RETROSPOT', 'HAND WARMER OWL DESIGN'})</t>
+          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN'})</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN'})</t>
+          <t>frozenset({'HAND WARMER OWL DESIGN', 'HAND WARMER RED RETROSPOT'})</t>
         </is>
       </c>
       <c r="C34" t="n">
+        <v>0.09922680412371133</v>
+      </c>
+      <c r="D34" t="n">
         <v>0.04896907216494845</v>
-      </c>
-      <c r="D34" t="n">
-        <v>0.09922680412371133</v>
       </c>
       <c r="E34" t="n">
         <v>0.03865979381443299</v>
       </c>
       <c r="F34" t="n">
-        <v>0.7894736842105263</v>
+        <v>0.3896103896103896</v>
       </c>
       <c r="G34" t="n">
         <v>7.956254272043746</v>
@@ -2074,16 +2074,16 @@
         <v>0.03380074928260177</v>
       </c>
       <c r="J34" t="n">
-        <v>4.278672680412371</v>
+        <v>1.558071945602106</v>
       </c>
       <c r="K34" t="n">
-        <v>0.9193315266486</v>
+        <v>0.9706247019551741</v>
       </c>
       <c r="L34" t="n">
         <v>0.3529411764705883</v>
       </c>
       <c r="M34" t="n">
-        <v>0.7662826594382953</v>
+        <v>0.3581811142786753</v>
       </c>
       <c r="N34" t="n">
         <v>0.589542036910458</v>
@@ -2092,25 +2092,25 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER OWL DESIGN', 'HAND WARMER RED RETROSPOT'})</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN'})</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER RED RETROSPOT', 'HAND WARMER OWL DESIGN'})</t>
-        </is>
-      </c>
       <c r="C35" t="n">
+        <v>0.04896907216494845</v>
+      </c>
+      <c r="D35" t="n">
         <v>0.09922680412371133</v>
-      </c>
-      <c r="D35" t="n">
-        <v>0.04896907216494845</v>
       </c>
       <c r="E35" t="n">
         <v>0.03865979381443299</v>
       </c>
       <c r="F35" t="n">
-        <v>0.3896103896103896</v>
+        <v>0.7894736842105263</v>
       </c>
       <c r="G35" t="n">
         <v>7.956254272043746</v>
@@ -2122,16 +2122,16 @@
         <v>0.03380074928260177</v>
       </c>
       <c r="J35" t="n">
-        <v>1.558071945602106</v>
+        <v>4.278672680412371</v>
       </c>
       <c r="K35" t="n">
-        <v>0.9706247019551741</v>
+        <v>0.9193315266486</v>
       </c>
       <c r="L35" t="n">
         <v>0.3529411764705883</v>
       </c>
       <c r="M35" t="n">
-        <v>0.3581811142786753</v>
+        <v>0.7662826594382953</v>
       </c>
       <c r="N35" t="n">
         <v>0.589542036910458</v>
@@ -2332,25 +2332,25 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
+          <t>frozenset({'CHOCOLATE HOT WATER BOTTLE'})</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
           <t>frozenset({'HOT WATER BOTTLE I AM SO POORLY'})</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>frozenset({'CHOCOLATE HOT WATER BOTTLE'})</t>
-        </is>
-      </c>
       <c r="C40" t="n">
+        <v>0.07860824742268041</v>
+      </c>
+      <c r="D40" t="n">
         <v>0.05798969072164949</v>
-      </c>
-      <c r="D40" t="n">
-        <v>0.07860824742268041</v>
       </c>
       <c r="E40" t="n">
         <v>0.03479381443298969</v>
       </c>
       <c r="F40" t="n">
-        <v>0.6</v>
+        <v>0.4426229508196722</v>
       </c>
       <c r="G40" t="n">
         <v>7.632786885245902</v>
@@ -2362,16 +2362,16 @@
         <v>0.03023534647677755</v>
       </c>
       <c r="J40" t="n">
-        <v>2.303479381443299</v>
+        <v>1.690077319587629</v>
       </c>
       <c r="K40" t="n">
-        <v>0.9224806201550387</v>
+        <v>0.943123543123543</v>
       </c>
       <c r="L40" t="n">
         <v>0.3417721518987342</v>
       </c>
       <c r="M40" t="n">
-        <v>0.5658741258741258</v>
+        <v>0.4083110941669844</v>
       </c>
       <c r="N40" t="n">
         <v>0.521311475409836</v>
@@ -2380,25 +2380,25 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
+          <t>frozenset({'HOT WATER BOTTLE I AM SO POORLY'})</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
           <t>frozenset({'CHOCOLATE HOT WATER BOTTLE'})</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>frozenset({'HOT WATER BOTTLE I AM SO POORLY'})</t>
-        </is>
-      </c>
       <c r="C41" t="n">
+        <v>0.05798969072164949</v>
+      </c>
+      <c r="D41" t="n">
         <v>0.07860824742268041</v>
-      </c>
-      <c r="D41" t="n">
-        <v>0.05798969072164949</v>
       </c>
       <c r="E41" t="n">
         <v>0.03479381443298969</v>
       </c>
       <c r="F41" t="n">
-        <v>0.4426229508196722</v>
+        <v>0.6</v>
       </c>
       <c r="G41" t="n">
         <v>7.632786885245902</v>
@@ -2410,16 +2410,16 @@
         <v>0.03023534647677755</v>
       </c>
       <c r="J41" t="n">
-        <v>1.690077319587629</v>
+        <v>2.303479381443299</v>
       </c>
       <c r="K41" t="n">
-        <v>0.943123543123543</v>
+        <v>0.9224806201550387</v>
       </c>
       <c r="L41" t="n">
         <v>0.3417721518987342</v>
       </c>
       <c r="M41" t="n">
-        <v>0.4083110941669844</v>
+        <v>0.5658741258741258</v>
       </c>
       <c r="N41" t="n">
         <v>0.521311475409836</v>
@@ -2625,7 +2625,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER UNION JACK', 'HAND WARMER OWL DESIGN'})</t>
+          <t>frozenset({'HAND WARMER OWL DESIGN', 'HAND WARMER UNION JACK'})</t>
         </is>
       </c>
       <c r="C46" t="n">
@@ -2668,7 +2668,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER UNION JACK', 'HAND WARMER OWL DESIGN'})</t>
+          <t>frozenset({'HAND WARMER OWL DESIGN', 'HAND WARMER UNION JACK'})</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -2812,7 +2812,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN', 'HAND WARMER OWL DESIGN'})</t>
+          <t>frozenset({'HAND WARMER OWL DESIGN', 'HAND WARMER SCOTTY DOG DESIGN'})</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -2865,7 +2865,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN', 'HAND WARMER OWL DESIGN'})</t>
+          <t>frozenset({'HAND WARMER OWL DESIGN', 'HAND WARMER SCOTTY DOG DESIGN'})</t>
         </is>
       </c>
       <c r="C51" t="n">
@@ -2913,7 +2913,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN', 'HAND WARMER BIRD DESIGN'})</t>
+          <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER SCOTTY DOG DESIGN'})</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -2956,7 +2956,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN', 'HAND WARMER BIRD DESIGN'})</t>
+          <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER SCOTTY DOG DESIGN'})</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -3004,25 +3004,25 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER OWL DESIGN'})</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN'})</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER OWL DESIGN'})</t>
-        </is>
-      </c>
       <c r="C54" t="n">
+        <v>0.05798969072164949</v>
+      </c>
+      <c r="D54" t="n">
         <v>0.09922680412371133</v>
-      </c>
-      <c r="D54" t="n">
-        <v>0.05798969072164949</v>
       </c>
       <c r="E54" t="n">
         <v>0.03994845360824742</v>
       </c>
       <c r="F54" t="n">
-        <v>0.4025974025974026</v>
+        <v>0.6888888888888888</v>
       </c>
       <c r="G54" t="n">
         <v>6.942568542568542</v>
@@ -3034,16 +3034,16 @@
         <v>0.0341943219258157</v>
       </c>
       <c r="J54" t="n">
-        <v>1.576843343792022</v>
+        <v>2.895342415316641</v>
       </c>
       <c r="K54" t="n">
-        <v>0.950251511375698</v>
+        <v>0.9086536339967344</v>
       </c>
       <c r="L54" t="n">
         <v>0.3406593406593406</v>
       </c>
       <c r="M54" t="n">
-        <v>0.3658215929077762</v>
+        <v>0.6546177078365918</v>
       </c>
       <c r="N54" t="n">
         <v>0.5457431457431456</v>
@@ -3052,25 +3052,25 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN'})</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER OWL DESIGN'})</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN'})</t>
-        </is>
-      </c>
       <c r="C55" t="n">
+        <v>0.09922680412371133</v>
+      </c>
+      <c r="D55" t="n">
         <v>0.05798969072164949</v>
-      </c>
-      <c r="D55" t="n">
-        <v>0.09922680412371133</v>
       </c>
       <c r="E55" t="n">
         <v>0.03994845360824742</v>
       </c>
       <c r="F55" t="n">
-        <v>0.6888888888888888</v>
+        <v>0.4025974025974026</v>
       </c>
       <c r="G55" t="n">
         <v>6.942568542568542</v>
@@ -3082,16 +3082,16 @@
         <v>0.0341943219258157</v>
       </c>
       <c r="J55" t="n">
-        <v>2.895342415316641</v>
+        <v>1.576843343792022</v>
       </c>
       <c r="K55" t="n">
-        <v>0.9086536339967344</v>
+        <v>0.950251511375698</v>
       </c>
       <c r="L55" t="n">
         <v>0.3406593406593406</v>
       </c>
       <c r="M55" t="n">
-        <v>0.6546177078365918</v>
+        <v>0.3658215929077762</v>
       </c>
       <c r="N55" t="n">
         <v>0.5457431457431456</v>
@@ -3100,25 +3100,25 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
+          <t>frozenset({'HEART OF WICKER SMALL'})</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
           <t>frozenset({'HEART OF WICKER LARGE'})</t>
         </is>
       </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>frozenset({'HEART OF WICKER SMALL'})</t>
-        </is>
-      </c>
       <c r="C56" t="n">
+        <v>0.08505154639175258</v>
+      </c>
+      <c r="D56" t="n">
         <v>0.07860824742268041</v>
-      </c>
-      <c r="D56" t="n">
-        <v>0.08505154639175258</v>
       </c>
       <c r="E56" t="n">
         <v>0.04639175257731959</v>
       </c>
       <c r="F56" t="n">
-        <v>0.5901639344262295</v>
+        <v>0.5454545454545454</v>
       </c>
       <c r="G56" t="n">
         <v>6.938897168405365</v>
@@ -3130,16 +3130,16 @@
         <v>0.03970599957487512</v>
       </c>
       <c r="J56" t="n">
-        <v>2.232474226804124</v>
+        <v>2.027061855670103</v>
       </c>
       <c r="K56" t="n">
-        <v>0.9289044289044287</v>
+        <v>0.9354460093896714</v>
       </c>
       <c r="L56" t="n">
         <v>0.3956043956043956</v>
       </c>
       <c r="M56" t="n">
-        <v>0.552066497344724</v>
+        <v>0.5066751430387794</v>
       </c>
       <c r="N56" t="n">
         <v>0.5678092399403875</v>
@@ -3148,25 +3148,25 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
+          <t>frozenset({'HEART OF WICKER LARGE'})</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
           <t>frozenset({'HEART OF WICKER SMALL'})</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>frozenset({'HEART OF WICKER LARGE'})</t>
-        </is>
-      </c>
       <c r="C57" t="n">
+        <v>0.07860824742268041</v>
+      </c>
+      <c r="D57" t="n">
         <v>0.08505154639175258</v>
-      </c>
-      <c r="D57" t="n">
-        <v>0.07860824742268041</v>
       </c>
       <c r="E57" t="n">
         <v>0.04639175257731959</v>
       </c>
       <c r="F57" t="n">
-        <v>0.5454545454545454</v>
+        <v>0.5901639344262295</v>
       </c>
       <c r="G57" t="n">
         <v>6.938897168405365</v>
@@ -3178,16 +3178,16 @@
         <v>0.03970599957487512</v>
       </c>
       <c r="J57" t="n">
-        <v>2.027061855670103</v>
+        <v>2.232474226804124</v>
       </c>
       <c r="K57" t="n">
-        <v>0.9354460093896714</v>
+        <v>0.9289044289044287</v>
       </c>
       <c r="L57" t="n">
         <v>0.3956043956043956</v>
       </c>
       <c r="M57" t="n">
-        <v>0.5066751430387794</v>
+        <v>0.552066497344724</v>
       </c>
       <c r="N57" t="n">
         <v>0.5678092399403875</v>
@@ -3196,25 +3196,25 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
+          <t>frozenset({'JAM MAKING SET WITH JARS'})</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
           <t>frozenset({'JAM MAKING SET PRINTED'})</t>
         </is>
       </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>frozenset({'JAM MAKING SET WITH JARS'})</t>
-        </is>
-      </c>
       <c r="C58" t="n">
+        <v>0.06572164948453608</v>
+      </c>
+      <c r="D58" t="n">
         <v>0.08762886597938144</v>
-      </c>
-      <c r="D58" t="n">
-        <v>0.06572164948453608</v>
       </c>
       <c r="E58" t="n">
         <v>0.03994845360824742</v>
       </c>
       <c r="F58" t="n">
-        <v>0.4558823529411765</v>
+        <v>0.6078431372549019</v>
       </c>
       <c r="G58" t="n">
         <v>6.936562860438293</v>
@@ -3226,16 +3226,16 @@
         <v>0.03418933999362313</v>
       </c>
       <c r="J58" t="n">
-        <v>1.717052103650042</v>
+        <v>2.326546391752577</v>
       </c>
       <c r="K58" t="n">
-        <v>0.9380353562967014</v>
+        <v>0.9160400444938821</v>
       </c>
       <c r="L58" t="n">
         <v>0.3522727272727272</v>
       </c>
       <c r="M58" t="n">
-        <v>0.417606490872211</v>
+        <v>0.5701783538274066</v>
       </c>
       <c r="N58" t="n">
         <v>0.5318627450980392</v>
@@ -3244,25 +3244,25 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
+          <t>frozenset({'JAM MAKING SET PRINTED'})</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
           <t>frozenset({'JAM MAKING SET WITH JARS'})</t>
         </is>
       </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>frozenset({'JAM MAKING SET PRINTED'})</t>
-        </is>
-      </c>
       <c r="C59" t="n">
+        <v>0.08762886597938144</v>
+      </c>
+      <c r="D59" t="n">
         <v>0.06572164948453608</v>
-      </c>
-      <c r="D59" t="n">
-        <v>0.08762886597938144</v>
       </c>
       <c r="E59" t="n">
         <v>0.03994845360824742</v>
       </c>
       <c r="F59" t="n">
-        <v>0.6078431372549019</v>
+        <v>0.4558823529411765</v>
       </c>
       <c r="G59" t="n">
         <v>6.936562860438293</v>
@@ -3274,16 +3274,16 @@
         <v>0.03418933999362313</v>
       </c>
       <c r="J59" t="n">
-        <v>2.326546391752577</v>
+        <v>1.717052103650042</v>
       </c>
       <c r="K59" t="n">
-        <v>0.9160400444938821</v>
+        <v>0.9380353562967014</v>
       </c>
       <c r="L59" t="n">
         <v>0.3522727272727272</v>
       </c>
       <c r="M59" t="n">
-        <v>0.5701783538274066</v>
+        <v>0.417606490872211</v>
       </c>
       <c r="N59" t="n">
         <v>0.5318627450980392</v>
@@ -3297,7 +3297,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN', 'HAND WARMER BIRD DESIGN'})</t>
+          <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER SCOTTY DOG DESIGN'})</t>
         </is>
       </c>
       <c r="C60" t="n">
@@ -3340,7 +3340,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN', 'HAND WARMER BIRD DESIGN'})</t>
+          <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER SCOTTY DOG DESIGN'})</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -3676,25 +3676,25 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
+          <t>frozenset({'60 CAKE CASES VINTAGE CHRISTMAS'})</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
           <t>frozenset({'PAPER CHAIN KIT VINTAGE CHRISTMAS'})</t>
         </is>
       </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>frozenset({'60 CAKE CASES VINTAGE CHRISTMAS'})</t>
-        </is>
-      </c>
       <c r="C68" t="n">
+        <v>0.05798969072164949</v>
+      </c>
+      <c r="D68" t="n">
         <v>0.09020618556701031</v>
-      </c>
-      <c r="D68" t="n">
-        <v>0.05798969072164949</v>
       </c>
       <c r="E68" t="n">
         <v>0.03479381443298969</v>
       </c>
       <c r="F68" t="n">
-        <v>0.3857142857142857</v>
+        <v>0.6</v>
       </c>
       <c r="G68" t="n">
         <v>6.651428571428571</v>
@@ -3706,16 +3706,16 @@
         <v>0.02956278563077904</v>
       </c>
       <c r="J68" t="n">
-        <v>1.533505154639175</v>
+        <v>2.274484536082474</v>
       </c>
       <c r="K68" t="n">
-        <v>0.9338999055712937</v>
+        <v>0.9019607843137255</v>
       </c>
       <c r="L68" t="n">
         <v>0.3068181818181818</v>
       </c>
       <c r="M68" t="n">
-        <v>0.3478991596638655</v>
+        <v>0.5603399433427761</v>
       </c>
       <c r="N68" t="n">
         <v>0.4928571428571429</v>
@@ -3724,25 +3724,25 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
+          <t>frozenset({'PAPER CHAIN KIT VINTAGE CHRISTMAS'})</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
           <t>frozenset({'60 CAKE CASES VINTAGE CHRISTMAS'})</t>
         </is>
       </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>frozenset({'PAPER CHAIN KIT VINTAGE CHRISTMAS'})</t>
-        </is>
-      </c>
       <c r="C69" t="n">
+        <v>0.09020618556701031</v>
+      </c>
+      <c r="D69" t="n">
         <v>0.05798969072164949</v>
-      </c>
-      <c r="D69" t="n">
-        <v>0.09020618556701031</v>
       </c>
       <c r="E69" t="n">
         <v>0.03479381443298969</v>
       </c>
       <c r="F69" t="n">
-        <v>0.6</v>
+        <v>0.3857142857142857</v>
       </c>
       <c r="G69" t="n">
         <v>6.651428571428571</v>
@@ -3754,16 +3754,16 @@
         <v>0.02956278563077904</v>
       </c>
       <c r="J69" t="n">
-        <v>2.274484536082474</v>
+        <v>1.533505154639175</v>
       </c>
       <c r="K69" t="n">
-        <v>0.9019607843137255</v>
+        <v>0.9338999055712937</v>
       </c>
       <c r="L69" t="n">
         <v>0.3068181818181818</v>
       </c>
       <c r="M69" t="n">
-        <v>0.5603399433427761</v>
+        <v>0.3478991596638655</v>
       </c>
       <c r="N69" t="n">
         <v>0.4928571428571429</v>
@@ -3772,25 +3772,25 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN'})</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER OWL DESIGN'})</t>
         </is>
       </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN'})</t>
-        </is>
-      </c>
       <c r="C70" t="n">
+        <v>0.09922680412371133</v>
+      </c>
+      <c r="D70" t="n">
         <v>0.09793814432989691</v>
-      </c>
-      <c r="D70" t="n">
-        <v>0.09922680412371133</v>
       </c>
       <c r="E70" t="n">
         <v>0.06443298969072164</v>
       </c>
       <c r="F70" t="n">
-        <v>0.6578947368421052</v>
+        <v>0.6493506493506493</v>
       </c>
       <c r="G70" t="n">
         <v>6.630211893369788</v>
@@ -3802,16 +3802,16 @@
         <v>0.05471490062705919</v>
       </c>
       <c r="J70" t="n">
-        <v>2.633029341792228</v>
+        <v>2.572546773577701</v>
       </c>
       <c r="K70" t="n">
-        <v>0.9413714285714285</v>
+        <v>0.9427181688125893</v>
       </c>
       <c r="L70" t="n">
         <v>0.4854368932038834</v>
       </c>
       <c r="M70" t="n">
-        <v>0.6202093215872299</v>
+        <v>0.6112801484230056</v>
       </c>
       <c r="N70" t="n">
         <v>0.6536226930963773</v>
@@ -3820,25 +3820,25 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER OWL DESIGN'})</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN'})</t>
         </is>
       </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER OWL DESIGN'})</t>
-        </is>
-      </c>
       <c r="C71" t="n">
+        <v>0.09793814432989691</v>
+      </c>
+      <c r="D71" t="n">
         <v>0.09922680412371133</v>
-      </c>
-      <c r="D71" t="n">
-        <v>0.09793814432989691</v>
       </c>
       <c r="E71" t="n">
         <v>0.06443298969072164</v>
       </c>
       <c r="F71" t="n">
-        <v>0.6493506493506493</v>
+        <v>0.6578947368421052</v>
       </c>
       <c r="G71" t="n">
         <v>6.630211893369788</v>
@@ -3850,16 +3850,16 @@
         <v>0.05471490062705919</v>
       </c>
       <c r="J71" t="n">
-        <v>2.572546773577701</v>
+        <v>2.633029341792228</v>
       </c>
       <c r="K71" t="n">
-        <v>0.9427181688125893</v>
+        <v>0.9413714285714285</v>
       </c>
       <c r="L71" t="n">
         <v>0.4854368932038834</v>
       </c>
       <c r="M71" t="n">
-        <v>0.6112801484230056</v>
+        <v>0.6202093215872299</v>
       </c>
       <c r="N71" t="n">
         <v>0.6536226930963773</v>
@@ -3873,7 +3873,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER UNION JACK', 'HAND WARMER BIRD DESIGN'})</t>
+          <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER UNION JACK'})</t>
         </is>
       </c>
       <c r="C72" t="n">
@@ -3916,7 +3916,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER UNION JACK', 'HAND WARMER BIRD DESIGN'})</t>
+          <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER UNION JACK'})</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -3964,25 +3964,25 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER OWL DESIGN'})</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER RED RETROSPOT'})</t>
         </is>
       </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER OWL DESIGN'})</t>
-        </is>
-      </c>
       <c r="C74" t="n">
+        <v>0.05798969072164949</v>
+      </c>
+      <c r="D74" t="n">
         <v>0.08505154639175258</v>
-      </c>
-      <c r="D74" t="n">
-        <v>0.05798969072164949</v>
       </c>
       <c r="E74" t="n">
         <v>0.03221649484536082</v>
       </c>
       <c r="F74" t="n">
-        <v>0.3787878787878787</v>
+        <v>0.5555555555555555</v>
       </c>
       <c r="G74" t="n">
         <v>6.531986531986531</v>
@@ -3994,16 +3994,16 @@
         <v>0.02728438197470507</v>
       </c>
       <c r="J74" t="n">
-        <v>1.516406839326125</v>
+        <v>2.058634020618556</v>
       </c>
       <c r="K74" t="n">
-        <v>0.9256338028169014</v>
+        <v>0.8990424076607387</v>
       </c>
       <c r="L74" t="n">
         <v>0.2906976744186046</v>
       </c>
       <c r="M74" t="n">
-        <v>0.3405463665381585</v>
+        <v>0.5142410015649451</v>
       </c>
       <c r="N74" t="n">
         <v>0.4671717171717171</v>
@@ -4012,25 +4012,25 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER RED RETROSPOT'})</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER OWL DESIGN'})</t>
         </is>
       </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER RED RETROSPOT'})</t>
-        </is>
-      </c>
       <c r="C75" t="n">
+        <v>0.08505154639175258</v>
+      </c>
+      <c r="D75" t="n">
         <v>0.05798969072164949</v>
-      </c>
-      <c r="D75" t="n">
-        <v>0.08505154639175258</v>
       </c>
       <c r="E75" t="n">
         <v>0.03221649484536082</v>
       </c>
       <c r="F75" t="n">
-        <v>0.5555555555555555</v>
+        <v>0.3787878787878787</v>
       </c>
       <c r="G75" t="n">
         <v>6.531986531986531</v>
@@ -4042,16 +4042,16 @@
         <v>0.02728438197470507</v>
       </c>
       <c r="J75" t="n">
-        <v>2.058634020618556</v>
+        <v>1.516406839326125</v>
       </c>
       <c r="K75" t="n">
-        <v>0.8990424076607387</v>
+        <v>0.9256338028169014</v>
       </c>
       <c r="L75" t="n">
         <v>0.2906976744186046</v>
       </c>
       <c r="M75" t="n">
-        <v>0.5142410015649451</v>
+        <v>0.3405463665381585</v>
       </c>
       <c r="N75" t="n">
         <v>0.4671717171717171</v>
@@ -4065,7 +4065,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER UNION JACK', 'HAND WARMER BIRD DESIGN'})</t>
+          <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER UNION JACK'})</t>
         </is>
       </c>
       <c r="C76" t="n">
@@ -4108,7 +4108,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER UNION JACK', 'HAND WARMER BIRD DESIGN'})</t>
+          <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER UNION JACK'})</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -4348,25 +4348,25 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
+          <t>frozenset({'CHOCOLATE HOT WATER BOTTLE'})</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr">
+        <is>
           <t>frozenset({'HOT WATER BOTTLE TEA AND SYMPATHY'})</t>
         </is>
       </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>frozenset({'CHOCOLATE HOT WATER BOTTLE'})</t>
-        </is>
-      </c>
       <c r="C82" t="n">
+        <v>0.07860824742268041</v>
+      </c>
+      <c r="D82" t="n">
         <v>0.09278350515463918</v>
-      </c>
-      <c r="D82" t="n">
-        <v>0.07860824742268041</v>
       </c>
       <c r="E82" t="n">
         <v>0.04639175257731959</v>
       </c>
       <c r="F82" t="n">
-        <v>0.5</v>
+        <v>0.5901639344262295</v>
       </c>
       <c r="G82" t="n">
         <v>6.360655737704918</v>
@@ -4378,16 +4378,16 @@
         <v>0.03909820384738017</v>
       </c>
       <c r="J82" t="n">
-        <v>1.842783505154639</v>
+        <v>2.21360824742268</v>
       </c>
       <c r="K82" t="n">
-        <v>0.9289772727272728</v>
+        <v>0.9146853146853147</v>
       </c>
       <c r="L82" t="n">
         <v>0.3711340206185567</v>
       </c>
       <c r="M82" t="n">
-        <v>0.4573426573426573</v>
+        <v>0.5482488822652757</v>
       </c>
       <c r="N82" t="n">
         <v>0.5450819672131147</v>
@@ -4396,25 +4396,25 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
+          <t>frozenset({'HOT WATER BOTTLE TEA AND SYMPATHY'})</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr">
+        <is>
           <t>frozenset({'CHOCOLATE HOT WATER BOTTLE'})</t>
         </is>
       </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>frozenset({'HOT WATER BOTTLE TEA AND SYMPATHY'})</t>
-        </is>
-      </c>
       <c r="C83" t="n">
+        <v>0.09278350515463918</v>
+      </c>
+      <c r="D83" t="n">
         <v>0.07860824742268041</v>
-      </c>
-      <c r="D83" t="n">
-        <v>0.09278350515463918</v>
       </c>
       <c r="E83" t="n">
         <v>0.04639175257731959</v>
       </c>
       <c r="F83" t="n">
-        <v>0.5901639344262295</v>
+        <v>0.5</v>
       </c>
       <c r="G83" t="n">
         <v>6.360655737704918</v>
@@ -4426,16 +4426,16 @@
         <v>0.03909820384738017</v>
       </c>
       <c r="J83" t="n">
-        <v>2.21360824742268</v>
+        <v>1.842783505154639</v>
       </c>
       <c r="K83" t="n">
-        <v>0.9146853146853147</v>
+        <v>0.9289772727272728</v>
       </c>
       <c r="L83" t="n">
         <v>0.3711340206185567</v>
       </c>
       <c r="M83" t="n">
-        <v>0.5482488822652757</v>
+        <v>0.4573426573426573</v>
       </c>
       <c r="N83" t="n">
         <v>0.5450819672131147</v>
@@ -4444,25 +4444,25 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
+          <t>frozenset({'WHITE SKULL HOT WATER BOTTLE '})</t>
+        </is>
+      </c>
+      <c r="B84" t="inlineStr">
+        <is>
           <t>frozenset({'HOT WATER BOTTLE I AM SO POORLY'})</t>
         </is>
       </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>frozenset({'WHITE SKULL HOT WATER BOTTLE '})</t>
-        </is>
-      </c>
       <c r="C84" t="n">
+        <v>0.08505154639175258</v>
+      </c>
+      <c r="D84" t="n">
         <v>0.05798969072164949</v>
-      </c>
-      <c r="D84" t="n">
-        <v>0.08505154639175258</v>
       </c>
       <c r="E84" t="n">
         <v>0.03092783505154639</v>
       </c>
       <c r="F84" t="n">
-        <v>0.5333333333333333</v>
+        <v>0.3636363636363636</v>
       </c>
       <c r="G84" t="n">
         <v>6.27070707070707</v>
@@ -4474,16 +4474,16 @@
         <v>0.02599572218089064</v>
       </c>
       <c r="J84" t="n">
-        <v>1.96060382916053</v>
+        <v>1.480301914580265</v>
       </c>
       <c r="K84" t="n">
-        <v>0.8922708618331053</v>
+        <v>0.918661971830986</v>
       </c>
       <c r="L84" t="n">
         <v>0.2758620689655173</v>
       </c>
       <c r="M84" t="n">
-        <v>0.4899530516431925</v>
+        <v>0.3244621315756747</v>
       </c>
       <c r="N84" t="n">
         <v>0.4484848484848485</v>
@@ -4492,25 +4492,25 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
+          <t>frozenset({'HOT WATER BOTTLE I AM SO POORLY'})</t>
+        </is>
+      </c>
+      <c r="B85" t="inlineStr">
+        <is>
           <t>frozenset({'WHITE SKULL HOT WATER BOTTLE '})</t>
         </is>
       </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>frozenset({'HOT WATER BOTTLE I AM SO POORLY'})</t>
-        </is>
-      </c>
       <c r="C85" t="n">
+        <v>0.05798969072164949</v>
+      </c>
+      <c r="D85" t="n">
         <v>0.08505154639175258</v>
-      </c>
-      <c r="D85" t="n">
-        <v>0.05798969072164949</v>
       </c>
       <c r="E85" t="n">
         <v>0.03092783505154639</v>
       </c>
       <c r="F85" t="n">
-        <v>0.3636363636363636</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="G85" t="n">
         <v>6.27070707070707</v>
@@ -4522,16 +4522,16 @@
         <v>0.02599572218089064</v>
       </c>
       <c r="J85" t="n">
-        <v>1.480301914580265</v>
+        <v>1.96060382916053</v>
       </c>
       <c r="K85" t="n">
-        <v>0.918661971830986</v>
+        <v>0.8922708618331053</v>
       </c>
       <c r="L85" t="n">
         <v>0.2758620689655173</v>
       </c>
       <c r="M85" t="n">
-        <v>0.3244621315756747</v>
+        <v>0.4899530516431925</v>
       </c>
       <c r="N85" t="n">
         <v>0.4484848484848485</v>
@@ -4636,25 +4636,25 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER RED RETROSPOT'})</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN'})</t>
         </is>
       </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER RED RETROSPOT'})</t>
-        </is>
-      </c>
       <c r="C88" t="n">
+        <v>0.08505154639175258</v>
+      </c>
+      <c r="D88" t="n">
         <v>0.09922680412371133</v>
-      </c>
-      <c r="D88" t="n">
-        <v>0.08505154639175258</v>
       </c>
       <c r="E88" t="n">
         <v>0.05154639175257732</v>
       </c>
       <c r="F88" t="n">
-        <v>0.5194805194805194</v>
+        <v>0.606060606060606</v>
       </c>
       <c r="G88" t="n">
         <v>6.107831562377016</v>
@@ -4666,16 +4666,16 @@
         <v>0.04310699861834413</v>
       </c>
       <c r="J88" t="n">
-        <v>1.904081916968515</v>
+        <v>2.28657811260904</v>
       </c>
       <c r="K88" t="n">
-        <v>0.9283977110157366</v>
+        <v>0.9140140845070422</v>
       </c>
       <c r="L88" t="n">
         <v>0.3883495145631067</v>
       </c>
       <c r="M88" t="n">
-        <v>0.4748125114322297</v>
+        <v>0.5626652794034768</v>
       </c>
       <c r="N88" t="n">
         <v>0.5627705627705627</v>
@@ -4684,25 +4684,25 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN'})</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER RED RETROSPOT'})</t>
         </is>
       </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN'})</t>
-        </is>
-      </c>
       <c r="C89" t="n">
+        <v>0.09922680412371133</v>
+      </c>
+      <c r="D89" t="n">
         <v>0.08505154639175258</v>
-      </c>
-      <c r="D89" t="n">
-        <v>0.09922680412371133</v>
       </c>
       <c r="E89" t="n">
         <v>0.05154639175257732</v>
       </c>
       <c r="F89" t="n">
-        <v>0.606060606060606</v>
+        <v>0.5194805194805194</v>
       </c>
       <c r="G89" t="n">
         <v>6.107831562377016</v>
@@ -4714,16 +4714,16 @@
         <v>0.04310699861834413</v>
       </c>
       <c r="J89" t="n">
-        <v>2.28657811260904</v>
+        <v>1.904081916968515</v>
       </c>
       <c r="K89" t="n">
-        <v>0.9140140845070422</v>
+        <v>0.9283977110157366</v>
       </c>
       <c r="L89" t="n">
         <v>0.3883495145631067</v>
       </c>
       <c r="M89" t="n">
-        <v>0.5626652794034768</v>
+        <v>0.4748125114322297</v>
       </c>
       <c r="N89" t="n">
         <v>0.5627705627705627</v>
@@ -5500,7 +5500,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER UNION JACK', 'HAND WARMER OWL DESIGN'})</t>
+          <t>frozenset({'HAND WARMER OWL DESIGN', 'HAND WARMER UNION JACK'})</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -5553,7 +5553,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER UNION JACK', 'HAND WARMER OWL DESIGN'})</t>
+          <t>frozenset({'HAND WARMER OWL DESIGN', 'HAND WARMER UNION JACK'})</t>
         </is>
       </c>
       <c r="C107" t="n">
@@ -5596,25 +5596,25 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
+          <t>frozenset({'WHITE HANGING HEART T-LIGHT HOLDER'})</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
           <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.', 'KNITTED UNION FLAG HOT WATER BOTTLE'})</t>
         </is>
       </c>
-      <c r="B108" t="inlineStr">
-        <is>
-          <t>frozenset({'WHITE HANGING HEART T-LIGHT HOLDER'})</t>
-        </is>
-      </c>
       <c r="C108" t="n">
+        <v>0.1378865979381443</v>
+      </c>
+      <c r="D108" t="n">
         <v>0.05283505154639175</v>
-      </c>
-      <c r="D108" t="n">
-        <v>0.1378865979381443</v>
       </c>
       <c r="E108" t="n">
         <v>0.03865979381443299</v>
       </c>
       <c r="F108" t="n">
-        <v>0.7317073170731707</v>
+        <v>0.2803738317757009</v>
       </c>
       <c r="G108" t="n">
         <v>5.306587645315705</v>
@@ -5626,16 +5626,16 @@
         <v>0.03137454830481454</v>
       </c>
       <c r="J108" t="n">
-        <v>3.213331771321462</v>
+        <v>1.316190253045923</v>
       </c>
       <c r="K108" t="n">
-        <v>0.8568253968253967</v>
+        <v>0.9413552566018932</v>
       </c>
       <c r="L108" t="n">
         <v>0.2542372881355932</v>
       </c>
       <c r="M108" t="n">
-        <v>0.6887965292208976</v>
+        <v>0.240231419670672</v>
       </c>
       <c r="N108" t="n">
         <v>0.5060405744244358</v>
@@ -5644,25 +5644,25 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
+          <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.', 'KNITTED UNION FLAG HOT WATER BOTTLE'})</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
           <t>frozenset({'WHITE HANGING HEART T-LIGHT HOLDER'})</t>
         </is>
       </c>
-      <c r="B109" t="inlineStr">
-        <is>
-          <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.', 'KNITTED UNION FLAG HOT WATER BOTTLE'})</t>
-        </is>
-      </c>
       <c r="C109" t="n">
+        <v>0.05283505154639175</v>
+      </c>
+      <c r="D109" t="n">
         <v>0.1378865979381443</v>
-      </c>
-      <c r="D109" t="n">
-        <v>0.05283505154639175</v>
       </c>
       <c r="E109" t="n">
         <v>0.03865979381443299</v>
       </c>
       <c r="F109" t="n">
-        <v>0.2803738317757009</v>
+        <v>0.7317073170731707</v>
       </c>
       <c r="G109" t="n">
         <v>5.306587645315705</v>
@@ -5674,16 +5674,16 @@
         <v>0.03137454830481454</v>
       </c>
       <c r="J109" t="n">
-        <v>1.316190253045923</v>
+        <v>3.213331771321462</v>
       </c>
       <c r="K109" t="n">
-        <v>0.9413552566018932</v>
+        <v>0.8568253968253967</v>
       </c>
       <c r="L109" t="n">
         <v>0.2542372881355932</v>
       </c>
       <c r="M109" t="n">
-        <v>0.240231419670672</v>
+        <v>0.6887965292208976</v>
       </c>
       <c r="N109" t="n">
         <v>0.5060405744244358</v>
@@ -5884,25 +5884,25 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
+          <t>frozenset({'FAWN BLUE HOT WATER BOTTLE'})</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
           <t>frozenset({'SCOTTIE DOG HOT WATER BOTTLE'})</t>
         </is>
       </c>
-      <c r="B114" t="inlineStr">
-        <is>
-          <t>frozenset({'FAWN BLUE HOT WATER BOTTLE'})</t>
-        </is>
-      </c>
       <c r="C114" t="n">
+        <v>0.06829896907216494</v>
+      </c>
+      <c r="D114" t="n">
         <v>0.08762886597938144</v>
-      </c>
-      <c r="D114" t="n">
-        <v>0.06829896907216494</v>
       </c>
       <c r="E114" t="n">
         <v>0.03092783505154639</v>
       </c>
       <c r="F114" t="n">
-        <v>0.3529411764705883</v>
+        <v>0.4528301886792453</v>
       </c>
       <c r="G114" t="n">
         <v>5.167591564927859</v>
@@ -5914,16 +5914,16 @@
         <v>0.02494287384419173</v>
       </c>
       <c r="J114" t="n">
-        <v>1.439901593252109</v>
+        <v>1.667436900106648</v>
       </c>
       <c r="K114" t="n">
-        <v>0.8839453860640303</v>
+        <v>0.8656062701705857</v>
       </c>
       <c r="L114" t="n">
         <v>0.2474226804123711</v>
       </c>
       <c r="M114" t="n">
-        <v>0.3055080953543243</v>
+        <v>0.4002771559535232</v>
       </c>
       <c r="N114" t="n">
         <v>0.4028856825749168</v>
@@ -5932,25 +5932,25 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
+          <t>frozenset({'SCOTTIE DOG HOT WATER BOTTLE'})</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
           <t>frozenset({'FAWN BLUE HOT WATER BOTTLE'})</t>
         </is>
       </c>
-      <c r="B115" t="inlineStr">
-        <is>
-          <t>frozenset({'SCOTTIE DOG HOT WATER BOTTLE'})</t>
-        </is>
-      </c>
       <c r="C115" t="n">
+        <v>0.08762886597938144</v>
+      </c>
+      <c r="D115" t="n">
         <v>0.06829896907216494</v>
-      </c>
-      <c r="D115" t="n">
-        <v>0.08762886597938144</v>
       </c>
       <c r="E115" t="n">
         <v>0.03092783505154639</v>
       </c>
       <c r="F115" t="n">
-        <v>0.4528301886792453</v>
+        <v>0.3529411764705883</v>
       </c>
       <c r="G115" t="n">
         <v>5.167591564927859</v>
@@ -5962,16 +5962,16 @@
         <v>0.02494287384419173</v>
       </c>
       <c r="J115" t="n">
-        <v>1.667436900106648</v>
+        <v>1.439901593252109</v>
       </c>
       <c r="K115" t="n">
-        <v>0.8656062701705857</v>
+        <v>0.8839453860640303</v>
       </c>
       <c r="L115" t="n">
         <v>0.2474226804123711</v>
       </c>
       <c r="M115" t="n">
-        <v>0.4002771559535232</v>
+        <v>0.3055080953543243</v>
       </c>
       <c r="N115" t="n">
         <v>0.4028856825749168</v>
@@ -5985,7 +5985,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER RED RETROSPOT', 'HAND WARMER OWL DESIGN'})</t>
+          <t>frozenset({'HAND WARMER OWL DESIGN', 'HAND WARMER RED RETROSPOT'})</t>
         </is>
       </c>
       <c r="C116" t="n">
@@ -6028,7 +6028,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER RED RETROSPOT', 'HAND WARMER OWL DESIGN'})</t>
+          <t>frozenset({'HAND WARMER UNION JACK', 'HAND WARMER SCOTTY DOG DESIGN'})</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -6124,7 +6124,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER UNION JACK', 'HAND WARMER SCOTTY DOG DESIGN'})</t>
+          <t>frozenset({'HAND WARMER OWL DESIGN', 'HAND WARMER RED RETROSPOT'})</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -6172,25 +6172,25 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
+          <t>frozenset({'WHITE HANGING HEART T-LIGHT HOLDER'})</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
           <t>frozenset({'WHITE METAL LANTERN'})</t>
         </is>
       </c>
-      <c r="B120" t="inlineStr">
-        <is>
-          <t>frozenset({'WHITE HANGING HEART T-LIGHT HOLDER'})</t>
-        </is>
-      </c>
       <c r="C120" t="n">
+        <v>0.1378865979381443</v>
+      </c>
+      <c r="D120" t="n">
         <v>0.04381443298969072</v>
-      </c>
-      <c r="D120" t="n">
-        <v>0.1378865979381443</v>
       </c>
       <c r="E120" t="n">
         <v>0.03092783505154639</v>
       </c>
       <c r="F120" t="n">
-        <v>0.7058823529411765</v>
+        <v>0.2242990654205607</v>
       </c>
       <c r="G120" t="n">
         <v>5.119296316657504</v>
@@ -6202,16 +6202,16 @@
         <v>0.02488641194600914</v>
       </c>
       <c r="J120" t="n">
-        <v>2.93118556701031</v>
+        <v>1.23267295988076</v>
       </c>
       <c r="K120" t="n">
-        <v>0.8415318957771788</v>
+        <v>0.9333582461385151</v>
       </c>
       <c r="L120" t="n">
         <v>0.2051282051282051</v>
       </c>
       <c r="M120" t="n">
-        <v>0.6588411149213048</v>
+        <v>0.1887548177444139</v>
       </c>
       <c r="N120" t="n">
         <v>0.4650907091808686</v>
@@ -6220,25 +6220,25 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
+          <t>frozenset({'WHITE METAL LANTERN'})</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
           <t>frozenset({'WHITE HANGING HEART T-LIGHT HOLDER'})</t>
         </is>
       </c>
-      <c r="B121" t="inlineStr">
-        <is>
-          <t>frozenset({'WHITE METAL LANTERN'})</t>
-        </is>
-      </c>
       <c r="C121" t="n">
+        <v>0.04381443298969072</v>
+      </c>
+      <c r="D121" t="n">
         <v>0.1378865979381443</v>
-      </c>
-      <c r="D121" t="n">
-        <v>0.04381443298969072</v>
       </c>
       <c r="E121" t="n">
         <v>0.03092783505154639</v>
       </c>
       <c r="F121" t="n">
-        <v>0.2242990654205607</v>
+        <v>0.7058823529411765</v>
       </c>
       <c r="G121" t="n">
         <v>5.119296316657504</v>
@@ -6250,16 +6250,16 @@
         <v>0.02488641194600914</v>
       </c>
       <c r="J121" t="n">
-        <v>1.23267295988076</v>
+        <v>2.93118556701031</v>
       </c>
       <c r="K121" t="n">
-        <v>0.9333582461385151</v>
+        <v>0.8415318957771788</v>
       </c>
       <c r="L121" t="n">
         <v>0.2051282051282051</v>
       </c>
       <c r="M121" t="n">
-        <v>0.1887548177444139</v>
+        <v>0.6588411149213048</v>
       </c>
       <c r="N121" t="n">
         <v>0.4650907091808686</v>
@@ -6460,25 +6460,25 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
+          <t>frozenset({'WOOD 2 DRAWER CABINET WHITE FINISH'})</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
           <t>frozenset({'WHITE HANGING HEART T-LIGHT HOLDER'})</t>
         </is>
       </c>
-      <c r="B126" t="inlineStr">
-        <is>
-          <t>frozenset({'WOOD 2 DRAWER CABINET WHITE FINISH'})</t>
-        </is>
-      </c>
       <c r="C126" t="n">
+        <v>0.04510309278350515</v>
+      </c>
+      <c r="D126" t="n">
         <v>0.1378865979381443</v>
-      </c>
-      <c r="D126" t="n">
-        <v>0.04510309278350515</v>
       </c>
       <c r="E126" t="n">
         <v>0.03092783505154639</v>
       </c>
       <c r="F126" t="n">
-        <v>0.2242990654205607</v>
+        <v>0.6857142857142857</v>
       </c>
       <c r="G126" t="n">
         <v>4.973030707610147</v>
@@ -6490,16 +6490,16 @@
         <v>0.0247087230311404</v>
       </c>
       <c r="J126" t="n">
-        <v>1.231011675568253</v>
+        <v>2.743088097469541</v>
       </c>
       <c r="K126" t="n">
-        <v>0.9266940707523666</v>
+        <v>0.8366509221772379</v>
       </c>
       <c r="L126" t="n">
         <v>0.2033898305084746</v>
       </c>
       <c r="M126" t="n">
-        <v>0.1876600199276048</v>
+        <v>0.635447362801623</v>
       </c>
       <c r="N126" t="n">
         <v>0.4550066755674232</v>
@@ -6508,25 +6508,25 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
+          <t>frozenset({'WHITE HANGING HEART T-LIGHT HOLDER'})</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
           <t>frozenset({'WOOD 2 DRAWER CABINET WHITE FINISH'})</t>
         </is>
       </c>
-      <c r="B127" t="inlineStr">
-        <is>
-          <t>frozenset({'WHITE HANGING HEART T-LIGHT HOLDER'})</t>
-        </is>
-      </c>
       <c r="C127" t="n">
+        <v>0.1378865979381443</v>
+      </c>
+      <c r="D127" t="n">
         <v>0.04510309278350515</v>
-      </c>
-      <c r="D127" t="n">
-        <v>0.1378865979381443</v>
       </c>
       <c r="E127" t="n">
         <v>0.03092783505154639</v>
       </c>
       <c r="F127" t="n">
-        <v>0.6857142857142857</v>
+        <v>0.2242990654205607</v>
       </c>
       <c r="G127" t="n">
         <v>4.973030707610147</v>
@@ -6538,16 +6538,16 @@
         <v>0.0247087230311404</v>
       </c>
       <c r="J127" t="n">
-        <v>2.743088097469541</v>
+        <v>1.231011675568253</v>
       </c>
       <c r="K127" t="n">
-        <v>0.8366509221772379</v>
+        <v>0.9266940707523666</v>
       </c>
       <c r="L127" t="n">
         <v>0.2033898305084746</v>
       </c>
       <c r="M127" t="n">
-        <v>0.635447362801623</v>
+        <v>0.1876600199276048</v>
       </c>
       <c r="N127" t="n">
         <v>0.4550066755674232</v>
@@ -6556,25 +6556,25 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN', 'HAND WARMER BIRD DESIGN'})</t>
+          <t>frozenset({'HAND WARMER UNION JACK'})</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER UNION JACK'})</t>
+          <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER SCOTTY DOG DESIGN'})</t>
         </is>
       </c>
       <c r="C128" t="n">
+        <v>0.1134020618556701</v>
+      </c>
+      <c r="D128" t="n">
         <v>0.05798969072164949</v>
-      </c>
-      <c r="D128" t="n">
-        <v>0.1134020618556701</v>
       </c>
       <c r="E128" t="n">
         <v>0.03221649484536082</v>
       </c>
       <c r="F128" t="n">
-        <v>0.5555555555555555</v>
+        <v>0.2840909090909091</v>
       </c>
       <c r="G128" t="n">
         <v>4.898989898989898</v>
@@ -6586,16 +6586,16 @@
         <v>0.02564034435115315</v>
       </c>
       <c r="J128" t="n">
-        <v>1.994845360824742</v>
+        <v>1.315823924071347</v>
       </c>
       <c r="K128" t="n">
-        <v>0.8448700410396717</v>
+        <v>0.8976744186046511</v>
       </c>
       <c r="L128" t="n">
         <v>0.2314814814814815</v>
       </c>
       <c r="M128" t="n">
-        <v>0.4987080103359173</v>
+        <v>0.240019898022634</v>
       </c>
       <c r="N128" t="n">
         <v>0.4198232323232323</v>
@@ -6604,25 +6604,25 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER SCOTTY DOG DESIGN'})</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER UNION JACK'})</t>
         </is>
       </c>
-      <c r="B129" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN', 'HAND WARMER BIRD DESIGN'})</t>
-        </is>
-      </c>
       <c r="C129" t="n">
+        <v>0.05798969072164949</v>
+      </c>
+      <c r="D129" t="n">
         <v>0.1134020618556701</v>
-      </c>
-      <c r="D129" t="n">
-        <v>0.05798969072164949</v>
       </c>
       <c r="E129" t="n">
         <v>0.03221649484536082</v>
       </c>
       <c r="F129" t="n">
-        <v>0.2840909090909091</v>
+        <v>0.5555555555555555</v>
       </c>
       <c r="G129" t="n">
         <v>4.898989898989898</v>
@@ -6634,16 +6634,16 @@
         <v>0.02564034435115315</v>
       </c>
       <c r="J129" t="n">
-        <v>1.315823924071347</v>
+        <v>1.994845360824742</v>
       </c>
       <c r="K129" t="n">
-        <v>0.8976744186046511</v>
+        <v>0.8448700410396717</v>
       </c>
       <c r="L129" t="n">
         <v>0.2314814814814815</v>
       </c>
       <c r="M129" t="n">
-        <v>0.240019898022634</v>
+        <v>0.4987080103359173</v>
       </c>
       <c r="N129" t="n">
         <v>0.4198232323232323</v>
@@ -6945,7 +6945,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN', 'HAND WARMER OWL DESIGN'})</t>
+          <t>frozenset({'HAND WARMER OWL DESIGN', 'HAND WARMER SCOTTY DOG DESIGN'})</t>
         </is>
       </c>
       <c r="C136" t="n">
@@ -6988,7 +6988,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN', 'HAND WARMER OWL DESIGN'})</t>
+          <t>frozenset({'HAND WARMER OWL DESIGN', 'HAND WARMER SCOTTY DOG DESIGN'})</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -7036,25 +7036,25 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER OWL DESIGN'})</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER UNION JACK'})</t>
         </is>
       </c>
-      <c r="B138" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER OWL DESIGN'})</t>
-        </is>
-      </c>
       <c r="C138" t="n">
+        <v>0.05798969072164949</v>
+      </c>
+      <c r="D138" t="n">
         <v>0.1134020618556701</v>
-      </c>
-      <c r="D138" t="n">
-        <v>0.05798969072164949</v>
       </c>
       <c r="E138" t="n">
         <v>0.03092783505154639</v>
       </c>
       <c r="F138" t="n">
-        <v>0.2727272727272728</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="G138" t="n">
         <v>4.703030303030303</v>
@@ -7066,16 +7066,16 @@
         <v>0.02435168455733872</v>
       </c>
       <c r="J138" t="n">
-        <v>1.295264175257732</v>
+        <v>1.899852724594993</v>
       </c>
       <c r="K138" t="n">
-        <v>0.8880813953488372</v>
+        <v>0.8358413132694938</v>
       </c>
       <c r="L138" t="n">
         <v>0.2201834862385321</v>
       </c>
       <c r="M138" t="n">
-        <v>0.2279567218007711</v>
+        <v>0.4736434108527132</v>
       </c>
       <c r="N138" t="n">
         <v>0.4030303030303031</v>
@@ -7084,25 +7084,25 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER UNION JACK'})</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER BIRD DESIGN', 'HAND WARMER OWL DESIGN'})</t>
         </is>
       </c>
-      <c r="B139" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER UNION JACK'})</t>
-        </is>
-      </c>
       <c r="C139" t="n">
+        <v>0.1134020618556701</v>
+      </c>
+      <c r="D139" t="n">
         <v>0.05798969072164949</v>
-      </c>
-      <c r="D139" t="n">
-        <v>0.1134020618556701</v>
       </c>
       <c r="E139" t="n">
         <v>0.03092783505154639</v>
       </c>
       <c r="F139" t="n">
-        <v>0.5333333333333333</v>
+        <v>0.2727272727272728</v>
       </c>
       <c r="G139" t="n">
         <v>4.703030303030303</v>
@@ -7114,16 +7114,16 @@
         <v>0.02435168455733872</v>
       </c>
       <c r="J139" t="n">
-        <v>1.899852724594993</v>
+        <v>1.295264175257732</v>
       </c>
       <c r="K139" t="n">
-        <v>0.8358413132694938</v>
+        <v>0.8880813953488372</v>
       </c>
       <c r="L139" t="n">
         <v>0.2201834862385321</v>
       </c>
       <c r="M139" t="n">
-        <v>0.4736434108527132</v>
+        <v>0.2279567218007711</v>
       </c>
       <c r="N139" t="n">
         <v>0.4030303030303031</v>
@@ -7132,25 +7132,25 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
+          <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.'})</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
           <t>frozenset({'WHITE SKULL HOT WATER BOTTLE '})</t>
         </is>
       </c>
-      <c r="B140" t="inlineStr">
-        <is>
-          <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.'})</t>
-        </is>
-      </c>
       <c r="C140" t="n">
+        <v>0.1005154639175258</v>
+      </c>
+      <c r="D140" t="n">
         <v>0.08505154639175258</v>
-      </c>
-      <c r="D140" t="n">
-        <v>0.1005154639175258</v>
       </c>
       <c r="E140" t="n">
         <v>0.03994845360824742</v>
       </c>
       <c r="F140" t="n">
-        <v>0.4696969696969697</v>
+        <v>0.3974358974358974</v>
       </c>
       <c r="G140" t="n">
         <v>4.672882672882673</v>
@@ -7162,16 +7162,16 @@
         <v>0.03139945796577744</v>
       </c>
       <c r="J140" t="n">
-        <v>1.696170839469809</v>
+        <v>1.518425093222198</v>
       </c>
       <c r="K140" t="n">
-        <v>0.8590640617900954</v>
+        <v>0.8738330714483777</v>
       </c>
       <c r="L140" t="n">
         <v>0.2743362831858407</v>
       </c>
       <c r="M140" t="n">
-        <v>0.4104367456802986</v>
+        <v>0.3414228963524738</v>
       </c>
       <c r="N140" t="n">
         <v>0.4335664335664335</v>
@@ -7180,25 +7180,25 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
+          <t>frozenset({'WHITE SKULL HOT WATER BOTTLE '})</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
           <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.'})</t>
         </is>
       </c>
-      <c r="B141" t="inlineStr">
-        <is>
-          <t>frozenset({'WHITE SKULL HOT WATER BOTTLE '})</t>
-        </is>
-      </c>
       <c r="C141" t="n">
+        <v>0.08505154639175258</v>
+      </c>
+      <c r="D141" t="n">
         <v>0.1005154639175258</v>
-      </c>
-      <c r="D141" t="n">
-        <v>0.08505154639175258</v>
       </c>
       <c r="E141" t="n">
         <v>0.03994845360824742</v>
       </c>
       <c r="F141" t="n">
-        <v>0.3974358974358974</v>
+        <v>0.4696969696969697</v>
       </c>
       <c r="G141" t="n">
         <v>4.672882672882673</v>
@@ -7210,16 +7210,16 @@
         <v>0.03139945796577744</v>
       </c>
       <c r="J141" t="n">
-        <v>1.518425093222198</v>
+        <v>1.696170839469809</v>
       </c>
       <c r="K141" t="n">
-        <v>0.8738330714483777</v>
+        <v>0.8590640617900954</v>
       </c>
       <c r="L141" t="n">
         <v>0.2743362831858407</v>
       </c>
       <c r="M141" t="n">
-        <v>0.3414228963524738</v>
+        <v>0.4104367456802986</v>
       </c>
       <c r="N141" t="n">
         <v>0.4335664335664335</v>
@@ -7516,25 +7516,25 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
+          <t>frozenset({'HOT WATER BOTTLE TEA AND SYMPATHY'})</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
           <t>frozenset({'WHITE SKULL HOT WATER BOTTLE '})</t>
         </is>
       </c>
-      <c r="B148" t="inlineStr">
-        <is>
-          <t>frozenset({'HOT WATER BOTTLE TEA AND SYMPATHY'})</t>
-        </is>
-      </c>
       <c r="C148" t="n">
+        <v>0.09278350515463918</v>
+      </c>
+      <c r="D148" t="n">
         <v>0.08505154639175258</v>
-      </c>
-      <c r="D148" t="n">
-        <v>0.09278350515463918</v>
       </c>
       <c r="E148" t="n">
         <v>0.03608247422680412</v>
       </c>
       <c r="F148" t="n">
-        <v>0.4242424242424242</v>
+        <v>0.3888888888888888</v>
       </c>
       <c r="G148" t="n">
         <v>4.572390572390572</v>
@@ -7546,16 +7546,16 @@
         <v>0.02819109363375491</v>
       </c>
       <c r="J148" t="n">
-        <v>1.575691806836679</v>
+        <v>1.497188378631678</v>
       </c>
       <c r="K148" t="n">
-        <v>0.8539235412474848</v>
+        <v>0.8612012987012986</v>
       </c>
       <c r="L148" t="n">
         <v>0.2545454545454545</v>
       </c>
       <c r="M148" t="n">
-        <v>0.365358126721763</v>
+        <v>0.3320813771517996</v>
       </c>
       <c r="N148" t="n">
         <v>0.4065656565656565</v>
@@ -7564,25 +7564,25 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
+          <t>frozenset({'WHITE SKULL HOT WATER BOTTLE '})</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
           <t>frozenset({'HOT WATER BOTTLE TEA AND SYMPATHY'})</t>
         </is>
       </c>
-      <c r="B149" t="inlineStr">
-        <is>
-          <t>frozenset({'WHITE SKULL HOT WATER BOTTLE '})</t>
-        </is>
-      </c>
       <c r="C149" t="n">
+        <v>0.08505154639175258</v>
+      </c>
+      <c r="D149" t="n">
         <v>0.09278350515463918</v>
-      </c>
-      <c r="D149" t="n">
-        <v>0.08505154639175258</v>
       </c>
       <c r="E149" t="n">
         <v>0.03608247422680412</v>
       </c>
       <c r="F149" t="n">
-        <v>0.3888888888888888</v>
+        <v>0.4242424242424242</v>
       </c>
       <c r="G149" t="n">
         <v>4.572390572390572</v>
@@ -7594,16 +7594,16 @@
         <v>0.02819109363375491</v>
       </c>
       <c r="J149" t="n">
-        <v>1.497188378631678</v>
+        <v>1.575691806836679</v>
       </c>
       <c r="K149" t="n">
-        <v>0.8612012987012986</v>
+        <v>0.8539235412474848</v>
       </c>
       <c r="L149" t="n">
         <v>0.2545454545454545</v>
       </c>
       <c r="M149" t="n">
-        <v>0.3320813771517996</v>
+        <v>0.365358126721763</v>
       </c>
       <c r="N149" t="n">
         <v>0.4065656565656565</v>
@@ -7612,25 +7612,25 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER OWL DESIGN', 'HAND WARMER SCOTTY DOG DESIGN'})</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER UNION JACK'})</t>
         </is>
       </c>
-      <c r="B150" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN', 'HAND WARMER OWL DESIGN'})</t>
-        </is>
-      </c>
       <c r="C150" t="n">
+        <v>0.06443298969072164</v>
+      </c>
+      <c r="D150" t="n">
         <v>0.1134020618556701</v>
-      </c>
-      <c r="D150" t="n">
-        <v>0.06443298969072164</v>
       </c>
       <c r="E150" t="n">
         <v>0.03221649484536082</v>
       </c>
       <c r="F150" t="n">
-        <v>0.2840909090909091</v>
+        <v>0.5</v>
       </c>
       <c r="G150" t="n">
         <v>4.409090909090909</v>
@@ -7642,16 +7642,16 @@
         <v>0.02490966096290785</v>
       </c>
       <c r="J150" t="n">
-        <v>1.306823760432008</v>
+        <v>1.77319587628866</v>
       </c>
       <c r="K150" t="n">
-        <v>0.8720930232558139</v>
+        <v>0.8264462809917354</v>
       </c>
       <c r="L150" t="n">
         <v>0.2212389380530974</v>
       </c>
       <c r="M150" t="n">
-        <v>0.234785875281743</v>
+        <v>0.436046511627907</v>
       </c>
       <c r="N150" t="n">
         <v>0.3920454545454545</v>
@@ -7660,25 +7660,25 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN', 'HAND WARMER OWL DESIGN'})</t>
+          <t>frozenset({'HAND WARMER UNION JACK'})</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>frozenset({'HAND WARMER UNION JACK'})</t>
+          <t>frozenset({'HAND WARMER OWL DESIGN', 'HAND WARMER SCOTTY DOG DESIGN'})</t>
         </is>
       </c>
       <c r="C151" t="n">
+        <v>0.1134020618556701</v>
+      </c>
+      <c r="D151" t="n">
         <v>0.06443298969072164</v>
-      </c>
-      <c r="D151" t="n">
-        <v>0.1134020618556701</v>
       </c>
       <c r="E151" t="n">
         <v>0.03221649484536082</v>
       </c>
       <c r="F151" t="n">
-        <v>0.5</v>
+        <v>0.2840909090909091</v>
       </c>
       <c r="G151" t="n">
         <v>4.409090909090909</v>
@@ -7690,16 +7690,16 @@
         <v>0.02490966096290785</v>
       </c>
       <c r="J151" t="n">
-        <v>1.77319587628866</v>
+        <v>1.306823760432008</v>
       </c>
       <c r="K151" t="n">
-        <v>0.8264462809917354</v>
+        <v>0.8720930232558139</v>
       </c>
       <c r="L151" t="n">
         <v>0.2212389380530974</v>
       </c>
       <c r="M151" t="n">
-        <v>0.436046511627907</v>
+        <v>0.234785875281743</v>
       </c>
       <c r="N151" t="n">
         <v>0.3920454545454545</v>
@@ -7996,25 +7996,25 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
+          <t>frozenset({'WOODEN FRAME ANTIQUE WHITE '})</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
           <t>frozenset({'WHITE HANGING HEART T-LIGHT HOLDER'})</t>
         </is>
       </c>
-      <c r="B158" t="inlineStr">
-        <is>
-          <t>frozenset({'WOODEN FRAME ANTIQUE WHITE '})</t>
-        </is>
-      </c>
       <c r="C158" t="n">
+        <v>0.06314432989690721</v>
+      </c>
+      <c r="D158" t="n">
         <v>0.1378865979381443</v>
-      </c>
-      <c r="D158" t="n">
-        <v>0.06314432989690721</v>
       </c>
       <c r="E158" t="n">
         <v>0.03737113402061856</v>
       </c>
       <c r="F158" t="n">
-        <v>0.2710280373831775</v>
+        <v>0.5918367346938775</v>
       </c>
       <c r="G158" t="n">
         <v>4.29219912263971</v>
@@ -8026,16 +8026,16 @@
         <v>0.02866437719205017</v>
       </c>
       <c r="J158" t="n">
-        <v>1.285173803859371</v>
+        <v>2.112177835051547</v>
       </c>
       <c r="K158" t="n">
-        <v>0.8896964074016803</v>
+        <v>0.8187165014466632</v>
       </c>
       <c r="L158" t="n">
         <v>0.2283464566929134</v>
       </c>
       <c r="M158" t="n">
-        <v>0.2218951265603105</v>
+        <v>0.5265550166254842</v>
       </c>
       <c r="N158" t="n">
         <v>0.4314323860385275</v>
@@ -8044,25 +8044,25 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
+          <t>frozenset({'WHITE HANGING HEART T-LIGHT HOLDER'})</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
           <t>frozenset({'WOODEN FRAME ANTIQUE WHITE '})</t>
         </is>
       </c>
-      <c r="B159" t="inlineStr">
-        <is>
-          <t>frozenset({'WHITE HANGING HEART T-LIGHT HOLDER'})</t>
-        </is>
-      </c>
       <c r="C159" t="n">
+        <v>0.1378865979381443</v>
+      </c>
+      <c r="D159" t="n">
         <v>0.06314432989690721</v>
-      </c>
-      <c r="D159" t="n">
-        <v>0.1378865979381443</v>
       </c>
       <c r="E159" t="n">
         <v>0.03737113402061856</v>
       </c>
       <c r="F159" t="n">
-        <v>0.5918367346938775</v>
+        <v>0.2710280373831775</v>
       </c>
       <c r="G159" t="n">
         <v>4.29219912263971</v>
@@ -8074,16 +8074,16 @@
         <v>0.02866437719205017</v>
       </c>
       <c r="J159" t="n">
-        <v>2.112177835051547</v>
+        <v>1.285173803859371</v>
       </c>
       <c r="K159" t="n">
-        <v>0.8187165014466632</v>
+        <v>0.8896964074016803</v>
       </c>
       <c r="L159" t="n">
         <v>0.2283464566929134</v>
       </c>
       <c r="M159" t="n">
-        <v>0.5265550166254842</v>
+        <v>0.2218951265603105</v>
       </c>
       <c r="N159" t="n">
         <v>0.4314323860385275</v>
@@ -8284,25 +8284,25 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER OWL DESIGN'})</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER UNION JACK'})</t>
         </is>
       </c>
-      <c r="B164" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER OWL DESIGN'})</t>
-        </is>
-      </c>
       <c r="C164" t="n">
+        <v>0.09793814432989691</v>
+      </c>
+      <c r="D164" t="n">
         <v>0.1134020618556701</v>
-      </c>
-      <c r="D164" t="n">
-        <v>0.09793814432989691</v>
       </c>
       <c r="E164" t="n">
         <v>0.04510309278350515</v>
       </c>
       <c r="F164" t="n">
-        <v>0.3977272727272727</v>
+        <v>0.4605263157894737</v>
       </c>
       <c r="G164" t="n">
         <v>4.061004784688995</v>
@@ -8314,16 +8314,16 @@
         <v>0.03399670528217664</v>
       </c>
       <c r="J164" t="n">
-        <v>1.497763081112624</v>
+        <v>1.643449836560221</v>
       </c>
       <c r="K164" t="n">
-        <v>0.8501661129568105</v>
+        <v>0.8355918367346939</v>
       </c>
       <c r="L164" t="n">
         <v>0.2713178294573643</v>
       </c>
       <c r="M164" t="n">
-        <v>0.3323376623376623</v>
+        <v>0.3915238678090576</v>
       </c>
       <c r="N164" t="n">
         <v>0.4291267942583732</v>
@@ -8332,25 +8332,25 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER UNION JACK'})</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER OWL DESIGN'})</t>
         </is>
       </c>
-      <c r="B165" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER UNION JACK'})</t>
-        </is>
-      </c>
       <c r="C165" t="n">
+        <v>0.1134020618556701</v>
+      </c>
+      <c r="D165" t="n">
         <v>0.09793814432989691</v>
-      </c>
-      <c r="D165" t="n">
-        <v>0.1134020618556701</v>
       </c>
       <c r="E165" t="n">
         <v>0.04510309278350515</v>
       </c>
       <c r="F165" t="n">
-        <v>0.4605263157894737</v>
+        <v>0.3977272727272727</v>
       </c>
       <c r="G165" t="n">
         <v>4.061004784688995</v>
@@ -8362,16 +8362,16 @@
         <v>0.03399670528217664</v>
       </c>
       <c r="J165" t="n">
-        <v>1.643449836560221</v>
+        <v>1.497763081112624</v>
       </c>
       <c r="K165" t="n">
-        <v>0.8355918367346939</v>
+        <v>0.8501661129568105</v>
       </c>
       <c r="L165" t="n">
         <v>0.2713178294573643</v>
       </c>
       <c r="M165" t="n">
-        <v>0.3915238678090576</v>
+        <v>0.3323376623376623</v>
       </c>
       <c r="N165" t="n">
         <v>0.4291267942583732</v>
@@ -8380,25 +8380,25 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN'})</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
           <t>frozenset({'SCOTTIE DOG HOT WATER BOTTLE'})</t>
         </is>
       </c>
-      <c r="B166" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN'})</t>
-        </is>
-      </c>
       <c r="C166" t="n">
+        <v>0.09922680412371133</v>
+      </c>
+      <c r="D166" t="n">
         <v>0.08762886597938144</v>
-      </c>
-      <c r="D166" t="n">
-        <v>0.09922680412371133</v>
       </c>
       <c r="E166" t="n">
         <v>0.03479381443298969</v>
       </c>
       <c r="F166" t="n">
-        <v>0.3970588235294118</v>
+        <v>0.3506493506493507</v>
       </c>
       <c r="G166" t="n">
         <v>4.001527883880826</v>
@@ -8410,16 +8410,16 @@
         <v>0.02609868211287066</v>
       </c>
       <c r="J166" t="n">
-        <v>1.493965300477747</v>
+        <v>1.405051546391753</v>
       </c>
       <c r="K166" t="n">
-        <v>0.8221385227034945</v>
+        <v>0.8327239972447411</v>
       </c>
       <c r="L166" t="n">
         <v>0.2288135593220339</v>
       </c>
       <c r="M166" t="n">
-        <v>0.3306404106707061</v>
+        <v>0.2882823391297967</v>
       </c>
       <c r="N166" t="n">
         <v>0.3738540870893812</v>
@@ -8428,25 +8428,25 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
+          <t>frozenset({'SCOTTIE DOG HOT WATER BOTTLE'})</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER SCOTTY DOG DESIGN'})</t>
         </is>
       </c>
-      <c r="B167" t="inlineStr">
-        <is>
-          <t>frozenset({'SCOTTIE DOG HOT WATER BOTTLE'})</t>
-        </is>
-      </c>
       <c r="C167" t="n">
+        <v>0.08762886597938144</v>
+      </c>
+      <c r="D167" t="n">
         <v>0.09922680412371133</v>
-      </c>
-      <c r="D167" t="n">
-        <v>0.08762886597938144</v>
       </c>
       <c r="E167" t="n">
         <v>0.03479381443298969</v>
       </c>
       <c r="F167" t="n">
-        <v>0.3506493506493507</v>
+        <v>0.3970588235294118</v>
       </c>
       <c r="G167" t="n">
         <v>4.001527883880826</v>
@@ -8458,16 +8458,16 @@
         <v>0.02609868211287066</v>
       </c>
       <c r="J167" t="n">
-        <v>1.405051546391753</v>
+        <v>1.493965300477747</v>
       </c>
       <c r="K167" t="n">
-        <v>0.8327239972447411</v>
+        <v>0.8221385227034945</v>
       </c>
       <c r="L167" t="n">
         <v>0.2288135593220339</v>
       </c>
       <c r="M167" t="n">
-        <v>0.2882823391297967</v>
+        <v>0.3306404106707061</v>
       </c>
       <c r="N167" t="n">
         <v>0.3738540870893812</v>
@@ -8860,25 +8860,25 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER OWL DESIGN'})</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
           <t>frozenset({'WHITE SKULL HOT WATER BOTTLE '})</t>
         </is>
       </c>
-      <c r="B176" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER OWL DESIGN'})</t>
-        </is>
-      </c>
       <c r="C176" t="n">
+        <v>0.09793814432989691</v>
+      </c>
+      <c r="D176" t="n">
         <v>0.08505154639175258</v>
-      </c>
-      <c r="D176" t="n">
-        <v>0.09793814432989691</v>
       </c>
       <c r="E176" t="n">
         <v>0.03092783505154639</v>
       </c>
       <c r="F176" t="n">
-        <v>0.3636363636363636</v>
+        <v>0.3157894736842106</v>
       </c>
       <c r="G176" t="n">
         <v>3.712918660287082</v>
@@ -8890,16 +8890,16 @@
         <v>0.02259804442555001</v>
       </c>
       <c r="J176" t="n">
-        <v>1.417525773195876</v>
+        <v>1.337232355273593</v>
       </c>
       <c r="K176" t="n">
-        <v>0.7985915492957746</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="L176" t="n">
         <v>0.2033898305084746</v>
       </c>
       <c r="M176" t="n">
-        <v>0.2945454545454546</v>
+        <v>0.252186805040771</v>
       </c>
       <c r="N176" t="n">
         <v>0.3397129186602871</v>
@@ -8908,25 +8908,25 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
+          <t>frozenset({'WHITE SKULL HOT WATER BOTTLE '})</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER OWL DESIGN'})</t>
         </is>
       </c>
-      <c r="B177" t="inlineStr">
-        <is>
-          <t>frozenset({'WHITE SKULL HOT WATER BOTTLE '})</t>
-        </is>
-      </c>
       <c r="C177" t="n">
+        <v>0.08505154639175258</v>
+      </c>
+      <c r="D177" t="n">
         <v>0.09793814432989691</v>
-      </c>
-      <c r="D177" t="n">
-        <v>0.08505154639175258</v>
       </c>
       <c r="E177" t="n">
         <v>0.03092783505154639</v>
       </c>
       <c r="F177" t="n">
-        <v>0.3157894736842106</v>
+        <v>0.3636363636363636</v>
       </c>
       <c r="G177" t="n">
         <v>3.712918660287082</v>
@@ -8938,16 +8938,16 @@
         <v>0.02259804442555001</v>
       </c>
       <c r="J177" t="n">
-        <v>1.337232355273593</v>
+        <v>1.417525773195876</v>
       </c>
       <c r="K177" t="n">
-        <v>0.8100000000000001</v>
+        <v>0.7985915492957746</v>
       </c>
       <c r="L177" t="n">
         <v>0.2033898305084746</v>
       </c>
       <c r="M177" t="n">
-        <v>0.252186805040771</v>
+        <v>0.2945454545454546</v>
       </c>
       <c r="N177" t="n">
         <v>0.3397129186602871</v>
@@ -9148,25 +9148,25 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
+          <t>frozenset({'WHITE HANGING HEART T-LIGHT HOLDER'})</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
           <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.'})</t>
         </is>
       </c>
-      <c r="B182" t="inlineStr">
-        <is>
-          <t>frozenset({'WHITE HANGING HEART T-LIGHT HOLDER'})</t>
-        </is>
-      </c>
       <c r="C182" t="n">
+        <v>0.1378865979381443</v>
+      </c>
+      <c r="D182" t="n">
         <v>0.1005154639175258</v>
-      </c>
-      <c r="D182" t="n">
-        <v>0.1378865979381443</v>
       </c>
       <c r="E182" t="n">
         <v>0.04896907216494845</v>
       </c>
       <c r="F182" t="n">
-        <v>0.4871794871794872</v>
+        <v>0.3551401869158878</v>
       </c>
       <c r="G182" t="n">
         <v>3.53318955188114</v>
@@ -9178,16 +9178,16 @@
         <v>0.03510933680518652</v>
       </c>
       <c r="J182" t="n">
-        <v>1.681121134020619</v>
+        <v>1.394852831316301</v>
       </c>
       <c r="K182" t="n">
-        <v>0.7970894284421655</v>
+        <v>0.8316418849815119</v>
       </c>
       <c r="L182" t="n">
         <v>0.2585034013605442</v>
       </c>
       <c r="M182" t="n">
-        <v>0.4051588670422751</v>
+        <v>0.2830784886056288</v>
       </c>
       <c r="N182" t="n">
         <v>0.4211598370476875</v>
@@ -9196,25 +9196,25 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
+          <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.'})</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
           <t>frozenset({'WHITE HANGING HEART T-LIGHT HOLDER'})</t>
         </is>
       </c>
-      <c r="B183" t="inlineStr">
-        <is>
-          <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.'})</t>
-        </is>
-      </c>
       <c r="C183" t="n">
+        <v>0.1005154639175258</v>
+      </c>
+      <c r="D183" t="n">
         <v>0.1378865979381443</v>
-      </c>
-      <c r="D183" t="n">
-        <v>0.1005154639175258</v>
       </c>
       <c r="E183" t="n">
         <v>0.04896907216494845</v>
       </c>
       <c r="F183" t="n">
-        <v>0.3551401869158878</v>
+        <v>0.4871794871794872</v>
       </c>
       <c r="G183" t="n">
         <v>3.53318955188114</v>
@@ -9226,16 +9226,16 @@
         <v>0.03510933680518652</v>
       </c>
       <c r="J183" t="n">
-        <v>1.394852831316301</v>
+        <v>1.681121134020619</v>
       </c>
       <c r="K183" t="n">
-        <v>0.8316418849815119</v>
+        <v>0.7970894284421655</v>
       </c>
       <c r="L183" t="n">
         <v>0.2585034013605442</v>
       </c>
       <c r="M183" t="n">
-        <v>0.2830784886056288</v>
+        <v>0.4051588670422751</v>
       </c>
       <c r="N183" t="n">
         <v>0.4211598370476875</v>
@@ -9340,25 +9340,25 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER UNION JACK'})</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER BIRD DESIGN'})</t>
         </is>
       </c>
-      <c r="B186" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER UNION JACK'})</t>
-        </is>
-      </c>
       <c r="C186" t="n">
+        <v>0.1134020618556701</v>
+      </c>
+      <c r="D186" t="n">
         <v>0.1275773195876289</v>
-      </c>
-      <c r="D186" t="n">
-        <v>0.1134020618556701</v>
       </c>
       <c r="E186" t="n">
         <v>0.04896907216494845</v>
       </c>
       <c r="F186" t="n">
-        <v>0.3838383838383839</v>
+        <v>0.4318181818181818</v>
       </c>
       <c r="G186" t="n">
         <v>3.38475665748393</v>
@@ -9370,16 +9370,16 @@
         <v>0.03450154107769157</v>
       </c>
       <c r="J186" t="n">
-        <v>1.438904850430962</v>
+        <v>1.535463917525773</v>
       </c>
       <c r="K186" t="n">
-        <v>0.8075876545129441</v>
+        <v>0.7946756425948592</v>
       </c>
       <c r="L186" t="n">
         <v>0.2550335570469799</v>
       </c>
       <c r="M186" t="n">
-        <v>0.30502701432934</v>
+        <v>0.3487310326305895</v>
       </c>
       <c r="N186" t="n">
         <v>0.4078282828282829</v>
@@ -9388,25 +9388,25 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER BIRD DESIGN'})</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER UNION JACK'})</t>
         </is>
       </c>
-      <c r="B187" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER BIRD DESIGN'})</t>
-        </is>
-      </c>
       <c r="C187" t="n">
+        <v>0.1275773195876289</v>
+      </c>
+      <c r="D187" t="n">
         <v>0.1134020618556701</v>
-      </c>
-      <c r="D187" t="n">
-        <v>0.1275773195876289</v>
       </c>
       <c r="E187" t="n">
         <v>0.04896907216494845</v>
       </c>
       <c r="F187" t="n">
-        <v>0.4318181818181818</v>
+        <v>0.3838383838383839</v>
       </c>
       <c r="G187" t="n">
         <v>3.38475665748393</v>
@@ -9418,16 +9418,16 @@
         <v>0.03450154107769157</v>
       </c>
       <c r="J187" t="n">
-        <v>1.535463917525773</v>
+        <v>1.438904850430962</v>
       </c>
       <c r="K187" t="n">
-        <v>0.7946756425948592</v>
+        <v>0.8075876545129441</v>
       </c>
       <c r="L187" t="n">
         <v>0.2550335570469799</v>
       </c>
       <c r="M187" t="n">
-        <v>0.3487310326305895</v>
+        <v>0.30502701432934</v>
       </c>
       <c r="N187" t="n">
         <v>0.4078282828282829</v>
@@ -9916,25 +9916,25 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
+          <t>frozenset({'HOT WATER BOTTLE TEA AND SYMPATHY'})</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER BIRD DESIGN'})</t>
         </is>
       </c>
-      <c r="B198" t="inlineStr">
-        <is>
-          <t>frozenset({'HOT WATER BOTTLE TEA AND SYMPATHY'})</t>
-        </is>
-      </c>
       <c r="C198" t="n">
+        <v>0.09278350515463918</v>
+      </c>
+      <c r="D198" t="n">
         <v>0.1275773195876289</v>
-      </c>
-      <c r="D198" t="n">
-        <v>0.09278350515463918</v>
       </c>
       <c r="E198" t="n">
         <v>0.03737113402061856</v>
       </c>
       <c r="F198" t="n">
-        <v>0.2929292929292929</v>
+        <v>0.4027777777777777</v>
       </c>
       <c r="G198" t="n">
         <v>3.15712682379349</v>
@@ -9946,16 +9946,16 @@
         <v>0.02553406313104474</v>
       </c>
       <c r="J198" t="n">
-        <v>1.283063328424153</v>
+        <v>1.460800767202109</v>
       </c>
       <c r="K198" t="n">
-        <v>0.7831711913614833</v>
+        <v>0.7531347962382445</v>
       </c>
       <c r="L198" t="n">
         <v>0.2042253521126761</v>
       </c>
       <c r="M198" t="n">
-        <v>0.2206152433425161</v>
+        <v>0.3154439520761529</v>
       </c>
       <c r="N198" t="n">
         <v>0.3478535353535354</v>
@@ -9964,25 +9964,25 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER BIRD DESIGN'})</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
           <t>frozenset({'HOT WATER BOTTLE TEA AND SYMPATHY'})</t>
         </is>
       </c>
-      <c r="B199" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER BIRD DESIGN'})</t>
-        </is>
-      </c>
       <c r="C199" t="n">
+        <v>0.1275773195876289</v>
+      </c>
+      <c r="D199" t="n">
         <v>0.09278350515463918</v>
-      </c>
-      <c r="D199" t="n">
-        <v>0.1275773195876289</v>
       </c>
       <c r="E199" t="n">
         <v>0.03737113402061856</v>
       </c>
       <c r="F199" t="n">
-        <v>0.4027777777777777</v>
+        <v>0.2929292929292929</v>
       </c>
       <c r="G199" t="n">
         <v>3.15712682379349</v>
@@ -9994,16 +9994,16 @@
         <v>0.02553406313104474</v>
       </c>
       <c r="J199" t="n">
-        <v>1.460800767202109</v>
+        <v>1.283063328424153</v>
       </c>
       <c r="K199" t="n">
-        <v>0.7531347962382445</v>
+        <v>0.7831711913614833</v>
       </c>
       <c r="L199" t="n">
         <v>0.2042253521126761</v>
       </c>
       <c r="M199" t="n">
-        <v>0.3154439520761529</v>
+        <v>0.2206152433425161</v>
       </c>
       <c r="N199" t="n">
         <v>0.3478535353535354</v>
@@ -10300,25 +10300,25 @@
     <row r="206">
       <c r="A206" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER BIRD DESIGN'})</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
           <t>frozenset({"PAPER CHAIN KIT 50'S CHRISTMAS "})</t>
         </is>
       </c>
-      <c r="B206" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER BIRD DESIGN'})</t>
-        </is>
-      </c>
       <c r="C206" t="n">
+        <v>0.1275773195876289</v>
+      </c>
+      <c r="D206" t="n">
         <v>0.1134020618556701</v>
-      </c>
-      <c r="D206" t="n">
-        <v>0.1275773195876289</v>
       </c>
       <c r="E206" t="n">
         <v>0.03994845360824742</v>
       </c>
       <c r="F206" t="n">
-        <v>0.3522727272727272</v>
+        <v>0.3131313131313131</v>
       </c>
       <c r="G206" t="n">
         <v>2.761248852157943</v>
@@ -10330,16 +10330,16 @@
         <v>0.02548092252099054</v>
       </c>
       <c r="J206" t="n">
-        <v>1.346898173268222</v>
+        <v>1.290782292298363</v>
       </c>
       <c r="K206" t="n">
-        <v>0.7194298574643662</v>
+        <v>0.7311192643064753</v>
       </c>
       <c r="L206" t="n">
         <v>0.1987179487179487</v>
       </c>
       <c r="M206" t="n">
-        <v>0.257553377198872</v>
+        <v>0.2252760159736904</v>
       </c>
       <c r="N206" t="n">
         <v>0.3327020202020202</v>
@@ -10348,25 +10348,25 @@
     <row r="207">
       <c r="A207" t="inlineStr">
         <is>
+          <t>frozenset({"PAPER CHAIN KIT 50'S CHRISTMAS "})</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER BIRD DESIGN'})</t>
         </is>
       </c>
-      <c r="B207" t="inlineStr">
-        <is>
-          <t>frozenset({"PAPER CHAIN KIT 50'S CHRISTMAS "})</t>
-        </is>
-      </c>
       <c r="C207" t="n">
+        <v>0.1134020618556701</v>
+      </c>
+      <c r="D207" t="n">
         <v>0.1275773195876289</v>
-      </c>
-      <c r="D207" t="n">
-        <v>0.1134020618556701</v>
       </c>
       <c r="E207" t="n">
         <v>0.03994845360824742</v>
       </c>
       <c r="F207" t="n">
-        <v>0.3131313131313131</v>
+        <v>0.3522727272727272</v>
       </c>
       <c r="G207" t="n">
         <v>2.761248852157943</v>
@@ -10378,16 +10378,16 @@
         <v>0.02548092252099054</v>
       </c>
       <c r="J207" t="n">
-        <v>1.290782292298363</v>
+        <v>1.346898173268222</v>
       </c>
       <c r="K207" t="n">
-        <v>0.7311192643064753</v>
+        <v>0.7194298574643662</v>
       </c>
       <c r="L207" t="n">
         <v>0.1987179487179487</v>
       </c>
       <c r="M207" t="n">
-        <v>0.2252760159736904</v>
+        <v>0.257553377198872</v>
       </c>
       <c r="N207" t="n">
         <v>0.3327020202020202</v>
@@ -10492,25 +10492,25 @@
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
+          <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.'})</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
           <t>frozenset({'HAND WARMER BIRD DESIGN'})</t>
         </is>
       </c>
-      <c r="B210" t="inlineStr">
-        <is>
-          <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.'})</t>
-        </is>
-      </c>
       <c r="C210" t="n">
+        <v>0.1005154639175258</v>
+      </c>
+      <c r="D210" t="n">
         <v>0.1275773195876289</v>
-      </c>
-      <c r="D210" t="n">
-        <v>0.1005154639175258</v>
       </c>
       <c r="E210" t="n">
         <v>0.03092783505154639</v>
       </c>
       <c r="F210" t="n">
-        <v>0.2424242424242425</v>
+        <v>0.3076923076923077</v>
       </c>
       <c r="G210" t="n">
         <v>2.411810411810412</v>
@@ -10522,16 +10522,16 @@
         <v>0.01810434158784143</v>
       </c>
       <c r="J210" t="n">
-        <v>1.187319587628866</v>
+        <v>1.26016609392898</v>
       </c>
       <c r="K210" t="n">
-        <v>0.6709748892171346</v>
+        <v>0.6507879656160459</v>
       </c>
       <c r="L210" t="n">
         <v>0.1568627450980392</v>
       </c>
       <c r="M210" t="n">
-        <v>0.1577667795432839</v>
+        <v>0.2064538120668106</v>
       </c>
       <c r="N210" t="n">
         <v>0.2750582750582751</v>
@@ -10540,25 +10540,25 @@
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
+          <t>frozenset({'HAND WARMER BIRD DESIGN'})</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
           <t>frozenset({'RED WOOLLY HOTTIE WHITE HEART.'})</t>
         </is>
       </c>
-      <c r="B211" t="inlineStr">
-        <is>
-          <t>frozenset({'HAND WARMER BIRD DESIGN'})</t>
-        </is>
-      </c>
       <c r="C211" t="n">
+        <v>0.1275773195876289</v>
+      </c>
+      <c r="D211" t="n">
         <v>0.1005154639175258</v>
-      </c>
-      <c r="D211" t="n">
-        <v>0.1275773195876289</v>
       </c>
       <c r="E211" t="n">
         <v>0.03092783505154639</v>
       </c>
       <c r="F211" t="n">
-        <v>0.3076923076923077</v>
+        <v>0.2424242424242425</v>
       </c>
       <c r="G211" t="n">
         <v>2.411810411810412</v>
@@ -10570,16 +10570,16 @@
         <v>0.01810434158784143</v>
       </c>
       <c r="J211" t="n">
-        <v>1.26016609392898</v>
+        <v>1.187319587628866</v>
       </c>
       <c r="K211" t="n">
-        <v>0.6507879656160459</v>
+        <v>0.6709748892171346</v>
       </c>
       <c r="L211" t="n">
         <v>0.1568627450980392</v>
       </c>
       <c r="M211" t="n">
-        <v>0.2064538120668106</v>
+        <v>0.1577667795432839</v>
       </c>
       <c r="N211" t="n">
         <v>0.2750582750582751</v>

</xml_diff>